<commit_message>
moved sampling parameters from 2EXT_01 to 1SPL01
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants/1SPL01_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/1SPL01_plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537E067E-559B-254C-BB4D-B10514D8AB8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C08CDD-8C93-3143-98B0-46F198483705}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4700" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="-4720" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>Source Name</t>
   </si>
@@ -247,6 +247,33 @@
   </si>
   <si>
     <t>Term Accession Number [Biological replicate] (#h; #tNFDI4PSO:0000042)</t>
+  </si>
+  <si>
+    <t>Parameter [Sample Collection Method]</t>
+  </si>
+  <si>
+    <t>Term Source REF [Sample Collection Method] (#h; #tNFDI4PSO:0000009)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [Sample Collection Method] (#h; #tNFDI4PSO:0000009)</t>
+  </si>
+  <si>
+    <t>Parameter [Metabolism quenching method]</t>
+  </si>
+  <si>
+    <t>Term Source REF [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)</t>
+  </si>
+  <si>
+    <t>Parameter [Sample storage]</t>
+  </si>
+  <si>
+    <t>Term Source REF [Sample storage] (#h; #tNFDI4PSO:0000011)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)</t>
   </si>
 </sst>
 </file>
@@ -355,7 +382,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="22">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -388,6 +421,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00\ &quot;microeinstein per square meter per second&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -427,83 +463,92 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7A0FDF1-D7A7-5444-9FF6-B24A8DE79F17}" name="annotationTable" displayName="annotationTable" ref="A2:BV3" totalsRowShown="0">
-  <autoFilter ref="A2:BV3" xr:uid="{8A7F28C9-E08B-8A4D-99FD-3313667921ED}"/>
-  <tableColumns count="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7A0FDF1-D7A7-5444-9FF6-B24A8DE79F17}" name="annotationTable" displayName="annotationTable" ref="A2:CE3" totalsRowShown="0">
+  <autoFilter ref="A2:CE3" xr:uid="{8A7F28C9-E08B-8A4D-99FD-3313667921ED}"/>
+  <tableColumns count="83">
     <tableColumn id="1" xr3:uid="{9B8F9057-2F20-7A45-8C27-9A36422B26D5}" name="Source Name"/>
     <tableColumn id="2" xr3:uid="{CC93B5FA-49F4-9B4C-B1F6-452471229F30}" name="Sample Name"/>
-    <tableColumn id="72" xr3:uid="{A33FCD3B-AD29-A742-9D63-6ECAFBEE068E}" name="Characteristics [Biological replicate]" dataDxfId="0"/>
+    <tableColumn id="72" xr3:uid="{A33FCD3B-AD29-A742-9D63-6ECAFBEE068E}" name="Characteristics [Biological replicate]" dataDxfId="21"/>
     <tableColumn id="73" xr3:uid="{4059FECC-FE9D-5947-9219-570196389DAE}" name="Term Source REF [Biological replicate] (#h; #tNFDI4PSO:0000042)"/>
     <tableColumn id="74" xr3:uid="{E04811ED-EF58-AD4F-84F5-156D9251E904}" name="Term Accession Number [Biological replicate] (#h; #tNFDI4PSO:0000042)"/>
-    <tableColumn id="3" xr3:uid="{6A7FF2B3-5F1E-8245-AC4F-6198097A8123}" name="Characteristics [Organism]" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{6A7FF2B3-5F1E-8245-AC4F-6198097A8123}" name="Characteristics [Organism]" dataDxfId="20"/>
     <tableColumn id="4" xr3:uid="{CC831F2C-80A0-C84F-829F-23F6C78F2EEB}" name="Term Source REF [Organism] (#h; #tNFDI4PSO:0000030)"/>
     <tableColumn id="5" xr3:uid="{D6E59B6D-D53F-A840-A182-24AE5A460E1D}" name="Term Accession Number [Organism] (#h; #tNFDI4PSO:0000030)"/>
-    <tableColumn id="14" xr3:uid="{000DCCE3-5EF7-4F4E-A82A-AD088FF36730}" name="Characteristics [Genotype]" dataDxfId="17"/>
+    <tableColumn id="14" xr3:uid="{000DCCE3-5EF7-4F4E-A82A-AD088FF36730}" name="Characteristics [Genotype]" dataDxfId="19"/>
     <tableColumn id="15" xr3:uid="{E2A1AEEB-EF2B-F448-824C-2953C18CC24A}" name="Term Source REF [Genotype] (#h; #tNFDI4PSO:0000031)"/>
     <tableColumn id="16" xr3:uid="{A998FE5F-8994-6E40-94FA-F0EF6DC905E4}" name="Term Accession Number [Genotype] (#h; #tNFDI4PSO:0000031)"/>
-    <tableColumn id="17" xr3:uid="{0EB867DC-9BB4-6243-BEE9-01764D9FEB35}" name="Characteristics [Organism part]" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{0EB867DC-9BB4-6243-BEE9-01764D9FEB35}" name="Characteristics [Organism part]" dataDxfId="18"/>
     <tableColumn id="18" xr3:uid="{B0CCF08F-B694-6C4F-94E6-E17AFD4C0A63}" name="Term Source REF [Organism part] (#h; #tNFDI4PSO:0000032)"/>
     <tableColumn id="19" xr3:uid="{6A02A31E-2B72-BE41-BF86-71E587B29D13}" name="Term Accession Number [Organism part] (#h; #tNFDI4PSO:0000032)"/>
-    <tableColumn id="20" xr3:uid="{96C34AC4-65C0-774B-A5A0-1BC98C955028}" name="Characteristics [age]" dataDxfId="15"/>
+    <tableColumn id="20" xr3:uid="{96C34AC4-65C0-774B-A5A0-1BC98C955028}" name="Characteristics [age]" dataDxfId="17"/>
     <tableColumn id="21" xr3:uid="{325D3F43-A306-2F47-AD9C-92F61C0649E5}" name="Term Source REF [age] (#h; #tNFDI4PSO:0000033)"/>
     <tableColumn id="22" xr3:uid="{334AF647-E268-2E41-950D-8973A43E29C8}" name="Term Accession Number [age] (#h; #tNFDI4PSO:0000033)"/>
-    <tableColumn id="26" xr3:uid="{5E219BCA-059A-CC41-93BF-8CD61AA9572D}" name="Characteristics [study type]" dataDxfId="14"/>
+    <tableColumn id="26" xr3:uid="{5E219BCA-059A-CC41-93BF-8CD61AA9572D}" name="Characteristics [study type]" dataDxfId="16"/>
     <tableColumn id="27" xr3:uid="{5FF2BBBF-350F-9842-8FDF-2F895B07EADF}" name="Term Source REF [study type] (#h; #tPECO:0007231)"/>
     <tableColumn id="28" xr3:uid="{E12790EC-754D-3244-8A7A-1242F7942612}" name="Term Accession Number [study type] (#h; #tPECO:0007231)"/>
-    <tableColumn id="23" xr3:uid="{E0A293FE-1EF5-A949-9C12-ADF40314B418}" name="Characteristics [plant growth medium exposure]" dataDxfId="13"/>
+    <tableColumn id="23" xr3:uid="{E0A293FE-1EF5-A949-9C12-ADF40314B418}" name="Characteristics [plant growth medium exposure]" dataDxfId="15"/>
     <tableColumn id="24" xr3:uid="{0C19F4A6-F9E8-1F4F-9B61-EB31E6DF451A}" name="Term Source REF [plant growth medium exposure] (#h; #tPECO:0007147)"/>
     <tableColumn id="25" xr3:uid="{7BBED07D-F814-A245-B090-723342B3D631}" name="Term Accession Number [plant growth medium exposure] (#h; #tPECO:0007147)"/>
-    <tableColumn id="29" xr3:uid="{C386EF1A-F4F8-C543-99A0-ABD311BD175F}" name="Characteristics [growth plot design]" dataDxfId="12"/>
+    <tableColumn id="29" xr3:uid="{C386EF1A-F4F8-C543-99A0-ABD311BD175F}" name="Characteristics [growth plot design]" dataDxfId="14"/>
     <tableColumn id="30" xr3:uid="{86FAE20B-4F89-EE4F-91E6-CE3B7E712F95}" name="Term Source REF [growth plot design] (#h; #tNFDI4PSO:0000001)"/>
     <tableColumn id="31" xr3:uid="{C0949892-595C-9742-BCD1-75134FAC012F}" name="Term Accession Number [growth plot design] (#h; #tNFDI4PSO:0000001)"/>
-    <tableColumn id="32" xr3:uid="{B90A4652-69D5-2E4F-8A64-A3A5A5CB24DB}" name="Characteristics [Growth day length]" dataDxfId="11"/>
+    <tableColumn id="32" xr3:uid="{B90A4652-69D5-2E4F-8A64-A3A5A5CB24DB}" name="Characteristics [Growth day length]" dataDxfId="13"/>
     <tableColumn id="33" xr3:uid="{4E2448E1-3D08-504C-8FE3-D71B801F4DC9}" name="Term Source REF [Growth day length] (#h; #tNFDI4PSO:0000041)"/>
     <tableColumn id="34" xr3:uid="{D47410BE-0000-B648-8CE5-966EE8968909}" name="Term Accession Number [Growth day length] (#h; #tNFDI4PSO:0000041)"/>
-    <tableColumn id="35" xr3:uid="{27034924-8879-044A-819B-7DC832A9D603}" name="Characteristics [light intensity exposure]" dataDxfId="10"/>
+    <tableColumn id="35" xr3:uid="{27034924-8879-044A-819B-7DC832A9D603}" name="Characteristics [light intensity exposure]" dataDxfId="12"/>
     <tableColumn id="36" xr3:uid="{FD04748E-7F58-4A46-A167-E5EB1375A50B}" name="Term Source REF [light intensity exposure] (#h; #tPECO:0007224)"/>
     <tableColumn id="37" xr3:uid="{D76E6422-DF20-B94A-B5A6-4FD7F7923EBF}" name="Term Accession Number [light intensity exposure] (#h; #tPECO:0007224)"/>
     <tableColumn id="6" xr3:uid="{8E446DD1-817A-E84A-9536-47B88B72BFD8}" name="Unit [microeinstein per square meter per second] (#h; #tUO:0000160; #u)"/>
     <tableColumn id="7" xr3:uid="{BCB29467-6D87-F141-98A0-60243765731F}" name="Term Source REF [microeinstein per square meter per second] (#h; #tUO:0000160; #u)"/>
     <tableColumn id="8" xr3:uid="{D2565EAD-7C86-C343-800D-E37FD463093B}" name="Term Accession Number [microeinstein per square meter per second] (#h; #tUO:0000160; #u)"/>
-    <tableColumn id="38" xr3:uid="{21746D48-E9A2-5B42-BC00-F5AFD4793AA7}" name="Characteristics [Humidity Day]" dataDxfId="9"/>
+    <tableColumn id="38" xr3:uid="{21746D48-E9A2-5B42-BC00-F5AFD4793AA7}" name="Characteristics [Humidity Day]" dataDxfId="11"/>
     <tableColumn id="39" xr3:uid="{8B1D9CC4-6026-674C-9852-06A06365907B}" name="Term Source REF [Humidity Day] (#h; #tNFDI4PSO:0000005)"/>
     <tableColumn id="40" xr3:uid="{8CCA0026-8267-884E-8F9A-369ACCB825EA}" name="Term Accession Number [Humidity Day] (#h; #tNFDI4PSO:0000005)"/>
     <tableColumn id="9" xr3:uid="{9508FD23-5388-F64E-8286-05B533856CA2}" name="Unit [percent] (#h; #tUO:0000187; #u)"/>
     <tableColumn id="10" xr3:uid="{F796BC22-CBE1-6D41-824E-F655C3F9D5B6}" name="Term Source REF [percent] (#h; #tUO:0000187; #u)"/>
     <tableColumn id="11" xr3:uid="{32AC3DD8-82CD-4349-BFD5-0805A34144D8}" name="Term Accession Number [percent] (#h; #tUO:0000187; #u)"/>
-    <tableColumn id="41" xr3:uid="{F4E42B79-6B62-E34C-95BE-8906E80BFBC8}" name="Characteristics [Humidity Night]" dataDxfId="8"/>
+    <tableColumn id="41" xr3:uid="{F4E42B79-6B62-E34C-95BE-8906E80BFBC8}" name="Characteristics [Humidity Night]" dataDxfId="10"/>
     <tableColumn id="42" xr3:uid="{FE26FC08-E3D1-7547-8E20-1363EF47EE86}" name="Term Source REF [Humidity Night] (#h; #tNFDI4PSO:0000006)"/>
     <tableColumn id="43" xr3:uid="{C6D20AF0-60A8-874E-9614-2A2F483EB262}" name="Term Accession Number [Humidity Night] (#h; #tNFDI4PSO:0000006)"/>
     <tableColumn id="12" xr3:uid="{2866C2CF-81B3-694E-B2D9-F69059F54AA2}" name="Unit [percent] (#2; #h; #tUO:0000187; #u)"/>
     <tableColumn id="13" xr3:uid="{A885FE47-7729-3B45-B73D-03FF1F114CD5}" name="Term Source REF [percent] (#2; #h; #tUO:0000187; #u)"/>
     <tableColumn id="65" xr3:uid="{A3AEBB25-5500-F249-866E-C98439259F17}" name="Term Accession Number [percent] (#2; #h; #tUO:0000187; #u)"/>
-    <tableColumn id="44" xr3:uid="{F0571376-132B-F940-9609-6B59D9845B1B}" name="Characteristics [Temperature Day]" dataDxfId="7"/>
+    <tableColumn id="44" xr3:uid="{F0571376-132B-F940-9609-6B59D9845B1B}" name="Characteristics [Temperature Day]" dataDxfId="9"/>
     <tableColumn id="45" xr3:uid="{23233498-CFC4-9F46-94D5-39E7A6B5AFB5}" name="Term Source REF [Temperature Day] (#h; #tNFDI4PSO:0000007)"/>
     <tableColumn id="46" xr3:uid="{346D483D-D0DE-5140-A015-4AD0367BAD4D}" name="Term Accession Number [Temperature Day] (#h; #tNFDI4PSO:0000007)"/>
     <tableColumn id="66" xr3:uid="{57808D06-1B53-8D41-BEB4-1644A20F7763}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)"/>
     <tableColumn id="67" xr3:uid="{A7356A0D-0EFD-3D44-9B2F-4566273E79E8}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)"/>
     <tableColumn id="68" xr3:uid="{AD21FFE5-445B-CB42-B199-FDD8BAD5635D}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)"/>
-    <tableColumn id="47" xr3:uid="{2AB78931-B301-314A-9311-2CC2C21128D4}" name="Characteristics [Temperature Night]" dataDxfId="6"/>
+    <tableColumn id="47" xr3:uid="{2AB78931-B301-314A-9311-2CC2C21128D4}" name="Characteristics [Temperature Night]" dataDxfId="8"/>
     <tableColumn id="48" xr3:uid="{3A76D4EC-C74F-0A4B-B340-8EF3D8B86ECB}" name="Term Source REF [Temperature Night] (#h; #tNFDI4PSO:0000008)"/>
     <tableColumn id="49" xr3:uid="{87034985-F2AC-A145-AA6A-9EDB63F919F9}" name="Term Accession Number [Temperature Night] (#h; #tNFDI4PSO:0000008)"/>
     <tableColumn id="69" xr3:uid="{6D54D968-A087-944D-BF64-3AC3D5B08F80}" name="Unit [degree Celsius] (#2; #h; #tUO:0000027; #u)"/>
     <tableColumn id="70" xr3:uid="{AE04B49D-BF47-F34B-B52A-752ECD10B8C7}" name="Term Source REF [degree Celsius] (#2; #h; #tUO:0000027; #u)"/>
     <tableColumn id="71" xr3:uid="{2A40040A-D450-EF49-AB82-0CEEB3D8A599}" name="Term Accession Number [degree Celsius] (#2; #h; #tUO:0000027; #u)"/>
-    <tableColumn id="50" xr3:uid="{FC29A38A-1769-7349-A9E5-A5184C62F33A}" name="Characteristics [watering exposure]" dataDxfId="5"/>
+    <tableColumn id="50" xr3:uid="{FC29A38A-1769-7349-A9E5-A5184C62F33A}" name="Characteristics [watering exposure]" dataDxfId="7"/>
     <tableColumn id="51" xr3:uid="{808AA82E-ECE0-AD47-92D3-27D7C93007B7}" name="Term Source REF [watering exposure] (#h; #tPECO:0007383)"/>
     <tableColumn id="52" xr3:uid="{7C45B5F9-759B-E646-A40E-CB5363DF17A8}" name="Term Accession Number [watering exposure] (#h; #tPECO:0007383)"/>
-    <tableColumn id="53" xr3:uid="{70DF5752-BECA-5342-9001-FA7F5271BC54}" name="Characteristics [plant nutrient exposure]" dataDxfId="4"/>
+    <tableColumn id="53" xr3:uid="{70DF5752-BECA-5342-9001-FA7F5271BC54}" name="Characteristics [plant nutrient exposure]" dataDxfId="6"/>
     <tableColumn id="54" xr3:uid="{FD6AD7C0-D253-D04C-8B67-6124B6C5D685}" name="Term Source REF [plant nutrient exposure] (#h; #tPECO:0007241)"/>
     <tableColumn id="55" xr3:uid="{95BC5752-0FFE-8C4E-BFE3-4FED8B72A648}" name="Term Accession Number [plant nutrient exposure] (#h; #tPECO:0007241)"/>
-    <tableColumn id="56" xr3:uid="{25540F7D-0E49-F74B-8EF6-6E2314EBD1B1}" name="Characteristics [abiotic plant exposure]" dataDxfId="3"/>
+    <tableColumn id="56" xr3:uid="{25540F7D-0E49-F74B-8EF6-6E2314EBD1B1}" name="Characteristics [abiotic plant exposure]" dataDxfId="5"/>
     <tableColumn id="57" xr3:uid="{19EC9032-1152-F940-ADB1-397E054EED4E}" name="Term Source REF [abiotic plant exposure] (#h; #tPECO:0007191)"/>
     <tableColumn id="58" xr3:uid="{40EA0154-215C-C44C-A5D6-852F5DA9A25C}" name="Term Accession Number [abiotic plant exposure] (#h; #tPECO:0007191)"/>
-    <tableColumn id="59" xr3:uid="{C208C009-B835-0041-9A5C-978B7EABB59C}" name="Characteristics [biotic plant exposure]" dataDxfId="2"/>
+    <tableColumn id="59" xr3:uid="{C208C009-B835-0041-9A5C-978B7EABB59C}" name="Characteristics [biotic plant exposure]" dataDxfId="4"/>
     <tableColumn id="60" xr3:uid="{2836636A-01C7-9C4E-9B41-EE6FEE3D7B80}" name="Term Source REF [biotic plant exposure] (#h; #tPECO:0007357)"/>
     <tableColumn id="61" xr3:uid="{E4A74FCF-2E01-354A-99CE-0602774F8706}" name="Term Accession Number [biotic plant exposure] (#h; #tPECO:0007357)"/>
-    <tableColumn id="62" xr3:uid="{12C4BED6-C71D-CC43-B976-AECFD0AF0BCF}" name="Characteristics [Time point]" dataDxfId="1"/>
+    <tableColumn id="62" xr3:uid="{12C4BED6-C71D-CC43-B976-AECFD0AF0BCF}" name="Characteristics [Time point]" dataDxfId="3"/>
     <tableColumn id="63" xr3:uid="{D78E63DF-76E2-AE4F-A9AA-86CB096E0FD1}" name="Term Source REF [Time point] (#h; #tNFDI4PSO:0000034)"/>
     <tableColumn id="64" xr3:uid="{4E3E838B-D518-9B41-95E4-AE65DE3C4242}" name="Term Accession Number [Time point] (#h; #tNFDI4PSO:0000034)"/>
+    <tableColumn id="75" xr3:uid="{7FBEC602-6866-EE4C-901B-A620EADE0B55}" name="Parameter [Sample Collection Method]" dataDxfId="2"/>
+    <tableColumn id="76" xr3:uid="{082E37E1-9067-2344-AFED-4C0AB2E6608F}" name="Term Source REF [Sample Collection Method] (#h; #tNFDI4PSO:0000009)"/>
+    <tableColumn id="77" xr3:uid="{23CA10DE-9FDA-A94D-84CF-7C5F7143EE90}" name="Term Accession Number [Sample Collection Method] (#h; #tNFDI4PSO:0000009)"/>
+    <tableColumn id="78" xr3:uid="{DD36BBD7-7DDE-4B4B-B0E7-E088C0737C72}" name="Parameter [Metabolism quenching method]" dataDxfId="1"/>
+    <tableColumn id="79" xr3:uid="{E9A2A827-A7E3-E44F-8034-982633580E8D}" name="Term Source REF [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)"/>
+    <tableColumn id="80" xr3:uid="{ECB588C7-B9C0-8741-BE8A-1CDECCED4ED4}" name="Term Accession Number [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)"/>
+    <tableColumn id="81" xr3:uid="{125431A9-D115-4A4B-A917-1C0A2F361D5C}" name="Parameter [Sample storage]" dataDxfId="0"/>
+    <tableColumn id="82" xr3:uid="{A56F8F05-EAAB-FD40-8F2F-AD66235065C4}" name="Term Source REF [Sample storage] (#h; #tNFDI4PSO:0000011)"/>
+    <tableColumn id="83" xr3:uid="{AB05BD40-EE64-3547-80D7-EDD26BB0F77A}" name="Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -824,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3613D5-BDC4-E141-9C9A-87C99351C8EE}">
-  <dimension ref="A1:BV3"/>
+  <dimension ref="A1:CE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="BT1" workbookViewId="0">
+      <selection activeCell="CC11" sqref="CC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -906,9 +951,18 @@
     <col min="72" max="72" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="52" hidden="1" customWidth="1"/>
     <col min="74" max="74" width="58.1640625" hidden="1" customWidth="1"/>
+    <col min="75" max="75" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="65" hidden="1" customWidth="1"/>
+    <col min="77" max="77" width="71.33203125" hidden="1" customWidth="1"/>
+    <col min="78" max="78" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="69.1640625" hidden="1" customWidth="1"/>
+    <col min="80" max="80" width="75.33203125" hidden="1" customWidth="1"/>
+    <col min="81" max="81" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="56.1640625" hidden="1" customWidth="1"/>
+    <col min="83" max="83" width="62.33203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -982,9 +1036,18 @@
       <c r="BS1" s="4"/>
       <c r="BT1" s="4"/>
       <c r="BU1" s="4"/>
-      <c r="BV1" s="2"/>
+      <c r="BV1" s="4"/>
+      <c r="BW1" s="4"/>
+      <c r="BX1" s="4"/>
+      <c r="BY1" s="4"/>
+      <c r="BZ1" s="4"/>
+      <c r="CA1" s="4"/>
+      <c r="CB1" s="4"/>
+      <c r="CC1" s="4"/>
+      <c r="CD1" s="4"/>
+      <c r="CE1" s="2"/>
     </row>
-    <row r="2" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1207,8 +1270,35 @@
       <c r="BV2" t="s">
         <v>55</v>
       </c>
+      <c r="BW2" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="3" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.2">
       <c r="C3" s="3"/>
       <c r="F3" s="3"/>
       <c r="I3" s="3"/>
@@ -1228,6 +1318,9 @@
       <c r="BN3" s="3"/>
       <c r="BQ3" s="3"/>
       <c r="BT3" s="3"/>
+      <c r="BW3" s="3"/>
+      <c r="BZ3" s="3"/>
+      <c r="CC3" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1242,7 +1335,7 @@
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <customXml>
   <SwateTable Table="annotationTable" Worksheet="1SPL01_plants">
-    <TableValidation DateTime="2021-03-12 12:14" SwateVersion="0.4.0" TableName="annotationTable" Userlist="" WorksheetName="1SPL01_plants">
+    <TableValidation DateTime="2021-03-12 12:35" SwateVersion="0.4.0" TableName="annotationTable" Userlist="" WorksheetName="1SPL01_plants">
       <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="1" ColumnHeader="Sample Name" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="2" ColumnHeader="Characteristics [Biological replicate]" Importance="3" Unit="None" ValidationFormat="None"/>
@@ -1264,13 +1357,16 @@
       <ColumnValidation ColumnAdress="65" ColumnHeader="Characteristics [abiotic plant exposure]" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="68" ColumnHeader="Characteristics [biotic plant exposure]" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="71" ColumnHeader="Characteristics [Time point]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="74" ColumnHeader="Parameter [Sample Collection Method]" Importance="4" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="77" ColumnHeader="Parameter [Metabolism quenching method]" Importance="4" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="80" ColumnHeader="Parameter [Sample storage]" Importance="4" Unit="None" ValidationFormat="None"/>
     </TableValidation>
   </SwateTable>
 </customXml>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68619077-37D4-FC49-BBDD-765B5130B077}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74E0AF51-2E13-E446-923D-1EB873710435}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
test adding outside annotationTable in template
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants/1SPL01_plants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/1SPL01_plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C08CDD-8C93-3143-98B0-46F198483705}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBFFF0D-D095-DD45-957C-F8CE56F4AB2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4720" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="12500" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>Source Name</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)</t>
+  </si>
+  <si>
+    <t>This is a test</t>
   </si>
 </sst>
 </file>
@@ -869,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3613D5-BDC4-E141-9C9A-87C99351C8EE}">
-  <dimension ref="A1:CE3"/>
+  <dimension ref="A1:CE10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BT1" workbookViewId="0">
-      <selection activeCell="CC11" sqref="CC11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1322,6 +1325,11 @@
       <c r="BZ3" s="3"/>
       <c r="CC3" s="3"/>
     </row>
+    <row r="10" spans="1:83" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test add building block
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants/1SPL01_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/1SPL01_plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBFFF0D-D095-DD45-957C-F8CE56F4AB2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0174028-AAC3-FA49-A84C-99FFA2439084}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12500" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="12500" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Source Name</t>
   </si>
@@ -277,6 +277,15 @@
   </si>
   <si>
     <t>This is a test</t>
+  </si>
+  <si>
+    <t>Parameter [ThisIsATest]</t>
+  </si>
+  <si>
+    <t>Term Source REF [ThisIsATest] (#h)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [ThisIsATest] (#h)</t>
   </si>
 </sst>
 </file>
@@ -385,7 +394,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -466,92 +478,95 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7A0FDF1-D7A7-5444-9FF6-B24A8DE79F17}" name="annotationTable" displayName="annotationTable" ref="A2:CE3" totalsRowShown="0">
-  <autoFilter ref="A2:CE3" xr:uid="{8A7F28C9-E08B-8A4D-99FD-3313667921ED}"/>
-  <tableColumns count="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7A0FDF1-D7A7-5444-9FF6-B24A8DE79F17}" name="annotationTable" displayName="annotationTable" ref="A2:CH3" totalsRowShown="0">
+  <autoFilter ref="A2:CH3" xr:uid="{8A7F28C9-E08B-8A4D-99FD-3313667921ED}"/>
+  <tableColumns count="86">
     <tableColumn id="1" xr3:uid="{9B8F9057-2F20-7A45-8C27-9A36422B26D5}" name="Source Name"/>
     <tableColumn id="2" xr3:uid="{CC93B5FA-49F4-9B4C-B1F6-452471229F30}" name="Sample Name"/>
-    <tableColumn id="72" xr3:uid="{A33FCD3B-AD29-A742-9D63-6ECAFBEE068E}" name="Characteristics [Biological replicate]" dataDxfId="21"/>
+    <tableColumn id="72" xr3:uid="{A33FCD3B-AD29-A742-9D63-6ECAFBEE068E}" name="Characteristics [Biological replicate]" dataDxfId="22"/>
     <tableColumn id="73" xr3:uid="{4059FECC-FE9D-5947-9219-570196389DAE}" name="Term Source REF [Biological replicate] (#h; #tNFDI4PSO:0000042)"/>
     <tableColumn id="74" xr3:uid="{E04811ED-EF58-AD4F-84F5-156D9251E904}" name="Term Accession Number [Biological replicate] (#h; #tNFDI4PSO:0000042)"/>
-    <tableColumn id="3" xr3:uid="{6A7FF2B3-5F1E-8245-AC4F-6198097A8123}" name="Characteristics [Organism]" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{6A7FF2B3-5F1E-8245-AC4F-6198097A8123}" name="Characteristics [Organism]" dataDxfId="21"/>
     <tableColumn id="4" xr3:uid="{CC831F2C-80A0-C84F-829F-23F6C78F2EEB}" name="Term Source REF [Organism] (#h; #tNFDI4PSO:0000030)"/>
     <tableColumn id="5" xr3:uid="{D6E59B6D-D53F-A840-A182-24AE5A460E1D}" name="Term Accession Number [Organism] (#h; #tNFDI4PSO:0000030)"/>
-    <tableColumn id="14" xr3:uid="{000DCCE3-5EF7-4F4E-A82A-AD088FF36730}" name="Characteristics [Genotype]" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{000DCCE3-5EF7-4F4E-A82A-AD088FF36730}" name="Characteristics [Genotype]" dataDxfId="20"/>
     <tableColumn id="15" xr3:uid="{E2A1AEEB-EF2B-F448-824C-2953C18CC24A}" name="Term Source REF [Genotype] (#h; #tNFDI4PSO:0000031)"/>
     <tableColumn id="16" xr3:uid="{A998FE5F-8994-6E40-94FA-F0EF6DC905E4}" name="Term Accession Number [Genotype] (#h; #tNFDI4PSO:0000031)"/>
-    <tableColumn id="17" xr3:uid="{0EB867DC-9BB4-6243-BEE9-01764D9FEB35}" name="Characteristics [Organism part]" dataDxfId="18"/>
+    <tableColumn id="17" xr3:uid="{0EB867DC-9BB4-6243-BEE9-01764D9FEB35}" name="Characteristics [Organism part]" dataDxfId="19"/>
     <tableColumn id="18" xr3:uid="{B0CCF08F-B694-6C4F-94E6-E17AFD4C0A63}" name="Term Source REF [Organism part] (#h; #tNFDI4PSO:0000032)"/>
     <tableColumn id="19" xr3:uid="{6A02A31E-2B72-BE41-BF86-71E587B29D13}" name="Term Accession Number [Organism part] (#h; #tNFDI4PSO:0000032)"/>
-    <tableColumn id="20" xr3:uid="{96C34AC4-65C0-774B-A5A0-1BC98C955028}" name="Characteristics [age]" dataDxfId="17"/>
+    <tableColumn id="20" xr3:uid="{96C34AC4-65C0-774B-A5A0-1BC98C955028}" name="Characteristics [age]" dataDxfId="18"/>
     <tableColumn id="21" xr3:uid="{325D3F43-A306-2F47-AD9C-92F61C0649E5}" name="Term Source REF [age] (#h; #tNFDI4PSO:0000033)"/>
     <tableColumn id="22" xr3:uid="{334AF647-E268-2E41-950D-8973A43E29C8}" name="Term Accession Number [age] (#h; #tNFDI4PSO:0000033)"/>
-    <tableColumn id="26" xr3:uid="{5E219BCA-059A-CC41-93BF-8CD61AA9572D}" name="Characteristics [study type]" dataDxfId="16"/>
+    <tableColumn id="26" xr3:uid="{5E219BCA-059A-CC41-93BF-8CD61AA9572D}" name="Characteristics [study type]" dataDxfId="17"/>
     <tableColumn id="27" xr3:uid="{5FF2BBBF-350F-9842-8FDF-2F895B07EADF}" name="Term Source REF [study type] (#h; #tPECO:0007231)"/>
     <tableColumn id="28" xr3:uid="{E12790EC-754D-3244-8A7A-1242F7942612}" name="Term Accession Number [study type] (#h; #tPECO:0007231)"/>
-    <tableColumn id="23" xr3:uid="{E0A293FE-1EF5-A949-9C12-ADF40314B418}" name="Characteristics [plant growth medium exposure]" dataDxfId="15"/>
+    <tableColumn id="23" xr3:uid="{E0A293FE-1EF5-A949-9C12-ADF40314B418}" name="Characteristics [plant growth medium exposure]" dataDxfId="16"/>
     <tableColumn id="24" xr3:uid="{0C19F4A6-F9E8-1F4F-9B61-EB31E6DF451A}" name="Term Source REF [plant growth medium exposure] (#h; #tPECO:0007147)"/>
     <tableColumn id="25" xr3:uid="{7BBED07D-F814-A245-B090-723342B3D631}" name="Term Accession Number [plant growth medium exposure] (#h; #tPECO:0007147)"/>
-    <tableColumn id="29" xr3:uid="{C386EF1A-F4F8-C543-99A0-ABD311BD175F}" name="Characteristics [growth plot design]" dataDxfId="14"/>
+    <tableColumn id="29" xr3:uid="{C386EF1A-F4F8-C543-99A0-ABD311BD175F}" name="Characteristics [growth plot design]" dataDxfId="15"/>
     <tableColumn id="30" xr3:uid="{86FAE20B-4F89-EE4F-91E6-CE3B7E712F95}" name="Term Source REF [growth plot design] (#h; #tNFDI4PSO:0000001)"/>
     <tableColumn id="31" xr3:uid="{C0949892-595C-9742-BCD1-75134FAC012F}" name="Term Accession Number [growth plot design] (#h; #tNFDI4PSO:0000001)"/>
-    <tableColumn id="32" xr3:uid="{B90A4652-69D5-2E4F-8A64-A3A5A5CB24DB}" name="Characteristics [Growth day length]" dataDxfId="13"/>
+    <tableColumn id="32" xr3:uid="{B90A4652-69D5-2E4F-8A64-A3A5A5CB24DB}" name="Characteristics [Growth day length]" dataDxfId="14"/>
     <tableColumn id="33" xr3:uid="{4E2448E1-3D08-504C-8FE3-D71B801F4DC9}" name="Term Source REF [Growth day length] (#h; #tNFDI4PSO:0000041)"/>
     <tableColumn id="34" xr3:uid="{D47410BE-0000-B648-8CE5-966EE8968909}" name="Term Accession Number [Growth day length] (#h; #tNFDI4PSO:0000041)"/>
-    <tableColumn id="35" xr3:uid="{27034924-8879-044A-819B-7DC832A9D603}" name="Characteristics [light intensity exposure]" dataDxfId="12"/>
+    <tableColumn id="35" xr3:uid="{27034924-8879-044A-819B-7DC832A9D603}" name="Characteristics [light intensity exposure]" dataDxfId="13"/>
     <tableColumn id="36" xr3:uid="{FD04748E-7F58-4A46-A167-E5EB1375A50B}" name="Term Source REF [light intensity exposure] (#h; #tPECO:0007224)"/>
     <tableColumn id="37" xr3:uid="{D76E6422-DF20-B94A-B5A6-4FD7F7923EBF}" name="Term Accession Number [light intensity exposure] (#h; #tPECO:0007224)"/>
     <tableColumn id="6" xr3:uid="{8E446DD1-817A-E84A-9536-47B88B72BFD8}" name="Unit [microeinstein per square meter per second] (#h; #tUO:0000160; #u)"/>
     <tableColumn id="7" xr3:uid="{BCB29467-6D87-F141-98A0-60243765731F}" name="Term Source REF [microeinstein per square meter per second] (#h; #tUO:0000160; #u)"/>
     <tableColumn id="8" xr3:uid="{D2565EAD-7C86-C343-800D-E37FD463093B}" name="Term Accession Number [microeinstein per square meter per second] (#h; #tUO:0000160; #u)"/>
-    <tableColumn id="38" xr3:uid="{21746D48-E9A2-5B42-BC00-F5AFD4793AA7}" name="Characteristics [Humidity Day]" dataDxfId="11"/>
+    <tableColumn id="38" xr3:uid="{21746D48-E9A2-5B42-BC00-F5AFD4793AA7}" name="Characteristics [Humidity Day]" dataDxfId="12"/>
     <tableColumn id="39" xr3:uid="{8B1D9CC4-6026-674C-9852-06A06365907B}" name="Term Source REF [Humidity Day] (#h; #tNFDI4PSO:0000005)"/>
     <tableColumn id="40" xr3:uid="{8CCA0026-8267-884E-8F9A-369ACCB825EA}" name="Term Accession Number [Humidity Day] (#h; #tNFDI4PSO:0000005)"/>
     <tableColumn id="9" xr3:uid="{9508FD23-5388-F64E-8286-05B533856CA2}" name="Unit [percent] (#h; #tUO:0000187; #u)"/>
     <tableColumn id="10" xr3:uid="{F796BC22-CBE1-6D41-824E-F655C3F9D5B6}" name="Term Source REF [percent] (#h; #tUO:0000187; #u)"/>
     <tableColumn id="11" xr3:uid="{32AC3DD8-82CD-4349-BFD5-0805A34144D8}" name="Term Accession Number [percent] (#h; #tUO:0000187; #u)"/>
-    <tableColumn id="41" xr3:uid="{F4E42B79-6B62-E34C-95BE-8906E80BFBC8}" name="Characteristics [Humidity Night]" dataDxfId="10"/>
+    <tableColumn id="41" xr3:uid="{F4E42B79-6B62-E34C-95BE-8906E80BFBC8}" name="Characteristics [Humidity Night]" dataDxfId="11"/>
     <tableColumn id="42" xr3:uid="{FE26FC08-E3D1-7547-8E20-1363EF47EE86}" name="Term Source REF [Humidity Night] (#h; #tNFDI4PSO:0000006)"/>
     <tableColumn id="43" xr3:uid="{C6D20AF0-60A8-874E-9614-2A2F483EB262}" name="Term Accession Number [Humidity Night] (#h; #tNFDI4PSO:0000006)"/>
     <tableColumn id="12" xr3:uid="{2866C2CF-81B3-694E-B2D9-F69059F54AA2}" name="Unit [percent] (#2; #h; #tUO:0000187; #u)"/>
     <tableColumn id="13" xr3:uid="{A885FE47-7729-3B45-B73D-03FF1F114CD5}" name="Term Source REF [percent] (#2; #h; #tUO:0000187; #u)"/>
     <tableColumn id="65" xr3:uid="{A3AEBB25-5500-F249-866E-C98439259F17}" name="Term Accession Number [percent] (#2; #h; #tUO:0000187; #u)"/>
-    <tableColumn id="44" xr3:uid="{F0571376-132B-F940-9609-6B59D9845B1B}" name="Characteristics [Temperature Day]" dataDxfId="9"/>
+    <tableColumn id="44" xr3:uid="{F0571376-132B-F940-9609-6B59D9845B1B}" name="Characteristics [Temperature Day]" dataDxfId="10"/>
     <tableColumn id="45" xr3:uid="{23233498-CFC4-9F46-94D5-39E7A6B5AFB5}" name="Term Source REF [Temperature Day] (#h; #tNFDI4PSO:0000007)"/>
     <tableColumn id="46" xr3:uid="{346D483D-D0DE-5140-A015-4AD0367BAD4D}" name="Term Accession Number [Temperature Day] (#h; #tNFDI4PSO:0000007)"/>
     <tableColumn id="66" xr3:uid="{57808D06-1B53-8D41-BEB4-1644A20F7763}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)"/>
     <tableColumn id="67" xr3:uid="{A7356A0D-0EFD-3D44-9B2F-4566273E79E8}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)"/>
     <tableColumn id="68" xr3:uid="{AD21FFE5-445B-CB42-B199-FDD8BAD5635D}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)"/>
-    <tableColumn id="47" xr3:uid="{2AB78931-B301-314A-9311-2CC2C21128D4}" name="Characteristics [Temperature Night]" dataDxfId="8"/>
+    <tableColumn id="47" xr3:uid="{2AB78931-B301-314A-9311-2CC2C21128D4}" name="Characteristics [Temperature Night]" dataDxfId="9"/>
     <tableColumn id="48" xr3:uid="{3A76D4EC-C74F-0A4B-B340-8EF3D8B86ECB}" name="Term Source REF [Temperature Night] (#h; #tNFDI4PSO:0000008)"/>
     <tableColumn id="49" xr3:uid="{87034985-F2AC-A145-AA6A-9EDB63F919F9}" name="Term Accession Number [Temperature Night] (#h; #tNFDI4PSO:0000008)"/>
     <tableColumn id="69" xr3:uid="{6D54D968-A087-944D-BF64-3AC3D5B08F80}" name="Unit [degree Celsius] (#2; #h; #tUO:0000027; #u)"/>
     <tableColumn id="70" xr3:uid="{AE04B49D-BF47-F34B-B52A-752ECD10B8C7}" name="Term Source REF [degree Celsius] (#2; #h; #tUO:0000027; #u)"/>
     <tableColumn id="71" xr3:uid="{2A40040A-D450-EF49-AB82-0CEEB3D8A599}" name="Term Accession Number [degree Celsius] (#2; #h; #tUO:0000027; #u)"/>
-    <tableColumn id="50" xr3:uid="{FC29A38A-1769-7349-A9E5-A5184C62F33A}" name="Characteristics [watering exposure]" dataDxfId="7"/>
+    <tableColumn id="50" xr3:uid="{FC29A38A-1769-7349-A9E5-A5184C62F33A}" name="Characteristics [watering exposure]" dataDxfId="8"/>
     <tableColumn id="51" xr3:uid="{808AA82E-ECE0-AD47-92D3-27D7C93007B7}" name="Term Source REF [watering exposure] (#h; #tPECO:0007383)"/>
     <tableColumn id="52" xr3:uid="{7C45B5F9-759B-E646-A40E-CB5363DF17A8}" name="Term Accession Number [watering exposure] (#h; #tPECO:0007383)"/>
-    <tableColumn id="53" xr3:uid="{70DF5752-BECA-5342-9001-FA7F5271BC54}" name="Characteristics [plant nutrient exposure]" dataDxfId="6"/>
+    <tableColumn id="53" xr3:uid="{70DF5752-BECA-5342-9001-FA7F5271BC54}" name="Characteristics [plant nutrient exposure]" dataDxfId="7"/>
     <tableColumn id="54" xr3:uid="{FD6AD7C0-D253-D04C-8B67-6124B6C5D685}" name="Term Source REF [plant nutrient exposure] (#h; #tPECO:0007241)"/>
     <tableColumn id="55" xr3:uid="{95BC5752-0FFE-8C4E-BFE3-4FED8B72A648}" name="Term Accession Number [plant nutrient exposure] (#h; #tPECO:0007241)"/>
-    <tableColumn id="56" xr3:uid="{25540F7D-0E49-F74B-8EF6-6E2314EBD1B1}" name="Characteristics [abiotic plant exposure]" dataDxfId="5"/>
+    <tableColumn id="56" xr3:uid="{25540F7D-0E49-F74B-8EF6-6E2314EBD1B1}" name="Characteristics [abiotic plant exposure]" dataDxfId="6"/>
     <tableColumn id="57" xr3:uid="{19EC9032-1152-F940-ADB1-397E054EED4E}" name="Term Source REF [abiotic plant exposure] (#h; #tPECO:0007191)"/>
     <tableColumn id="58" xr3:uid="{40EA0154-215C-C44C-A5D6-852F5DA9A25C}" name="Term Accession Number [abiotic plant exposure] (#h; #tPECO:0007191)"/>
-    <tableColumn id="59" xr3:uid="{C208C009-B835-0041-9A5C-978B7EABB59C}" name="Characteristics [biotic plant exposure]" dataDxfId="4"/>
+    <tableColumn id="59" xr3:uid="{C208C009-B835-0041-9A5C-978B7EABB59C}" name="Characteristics [biotic plant exposure]" dataDxfId="5"/>
     <tableColumn id="60" xr3:uid="{2836636A-01C7-9C4E-9B41-EE6FEE3D7B80}" name="Term Source REF [biotic plant exposure] (#h; #tPECO:0007357)"/>
     <tableColumn id="61" xr3:uid="{E4A74FCF-2E01-354A-99CE-0602774F8706}" name="Term Accession Number [biotic plant exposure] (#h; #tPECO:0007357)"/>
-    <tableColumn id="62" xr3:uid="{12C4BED6-C71D-CC43-B976-AECFD0AF0BCF}" name="Characteristics [Time point]" dataDxfId="3"/>
+    <tableColumn id="62" xr3:uid="{12C4BED6-C71D-CC43-B976-AECFD0AF0BCF}" name="Characteristics [Time point]" dataDxfId="4"/>
     <tableColumn id="63" xr3:uid="{D78E63DF-76E2-AE4F-A9AA-86CB096E0FD1}" name="Term Source REF [Time point] (#h; #tNFDI4PSO:0000034)"/>
     <tableColumn id="64" xr3:uid="{4E3E838B-D518-9B41-95E4-AE65DE3C4242}" name="Term Accession Number [Time point] (#h; #tNFDI4PSO:0000034)"/>
-    <tableColumn id="75" xr3:uid="{7FBEC602-6866-EE4C-901B-A620EADE0B55}" name="Parameter [Sample Collection Method]" dataDxfId="2"/>
+    <tableColumn id="75" xr3:uid="{7FBEC602-6866-EE4C-901B-A620EADE0B55}" name="Parameter [Sample Collection Method]" dataDxfId="3"/>
     <tableColumn id="76" xr3:uid="{082E37E1-9067-2344-AFED-4C0AB2E6608F}" name="Term Source REF [Sample Collection Method] (#h; #tNFDI4PSO:0000009)"/>
     <tableColumn id="77" xr3:uid="{23CA10DE-9FDA-A94D-84CF-7C5F7143EE90}" name="Term Accession Number [Sample Collection Method] (#h; #tNFDI4PSO:0000009)"/>
-    <tableColumn id="78" xr3:uid="{DD36BBD7-7DDE-4B4B-B0E7-E088C0737C72}" name="Parameter [Metabolism quenching method]" dataDxfId="1"/>
+    <tableColumn id="78" xr3:uid="{DD36BBD7-7DDE-4B4B-B0E7-E088C0737C72}" name="Parameter [Metabolism quenching method]" dataDxfId="2"/>
     <tableColumn id="79" xr3:uid="{E9A2A827-A7E3-E44F-8034-982633580E8D}" name="Term Source REF [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)"/>
     <tableColumn id="80" xr3:uid="{ECB588C7-B9C0-8741-BE8A-1CDECCED4ED4}" name="Term Accession Number [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)"/>
-    <tableColumn id="81" xr3:uid="{125431A9-D115-4A4B-A917-1C0A2F361D5C}" name="Parameter [Sample storage]" dataDxfId="0"/>
+    <tableColumn id="81" xr3:uid="{125431A9-D115-4A4B-A917-1C0A2F361D5C}" name="Parameter [Sample storage]" dataDxfId="1"/>
     <tableColumn id="82" xr3:uid="{A56F8F05-EAAB-FD40-8F2F-AD66235065C4}" name="Term Source REF [Sample storage] (#h; #tNFDI4PSO:0000011)"/>
     <tableColumn id="83" xr3:uid="{AB05BD40-EE64-3547-80D7-EDD26BB0F77A}" name="Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)"/>
+    <tableColumn id="84" xr3:uid="{B5209691-29B5-3B4A-BA79-AEAF67B03ACF}" name="Parameter [ThisIsATest]" dataDxfId="0"/>
+    <tableColumn id="85" xr3:uid="{023E05C5-AC7C-864E-9712-2A648CA415E6}" name="Term Source REF [ThisIsATest] (#h)"/>
+    <tableColumn id="86" xr3:uid="{8B222B87-3F15-ED42-A0B1-C770CDC868BE}" name="Term Accession Number [ThisIsATest] (#h)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -872,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3613D5-BDC4-E141-9C9A-87C99351C8EE}">
-  <dimension ref="A1:CE10"/>
+  <dimension ref="A1:CH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="BT1" workbookViewId="0">
+      <selection activeCell="CC13" sqref="CC13:CC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -963,9 +978,12 @@
     <col min="81" max="81" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="56.1640625" hidden="1" customWidth="1"/>
     <col min="83" max="83" width="62.33203125" hidden="1" customWidth="1"/>
+    <col min="84" max="84" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="33.1640625" hidden="1" customWidth="1"/>
+    <col min="86" max="86" width="39.5" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1048,9 +1066,12 @@
       <c r="CB1" s="4"/>
       <c r="CC1" s="4"/>
       <c r="CD1" s="4"/>
-      <c r="CE1" s="2"/>
+      <c r="CE1" s="4"/>
+      <c r="CF1" s="4"/>
+      <c r="CG1" s="4"/>
+      <c r="CH1" s="2"/>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1300,8 +1321,17 @@
       <c r="CE2" t="s">
         <v>82</v>
       </c>
+      <c r="CF2" t="s">
+        <v>84</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>85</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:86" x14ac:dyDescent="0.2">
       <c r="C3" s="3"/>
       <c r="F3" s="3"/>
       <c r="I3" s="3"/>
@@ -1324,8 +1354,9 @@
       <c r="BW3" s="3"/>
       <c r="BZ3" s="3"/>
       <c r="CC3" s="3"/>
+      <c r="CF3" s="3"/>
     </row>
-    <row r="10" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
test: adding comments outside annoTable
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants/1SPL01_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/1SPL01_plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0174028-AAC3-FA49-A84C-99FFA2439084}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5982205E-232C-5A4B-879D-B5BAA251A942}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12500" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="-25000" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
   <si>
     <t>Source Name</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)</t>
   </si>
   <si>
-    <t>This is a test</t>
-  </si>
-  <si>
     <t>Parameter [ThisIsATest]</t>
   </si>
   <si>
@@ -286,6 +283,12 @@
   </si>
   <si>
     <t>Term Accession Number [ThisIsATest] (#h)</t>
+  </si>
+  <si>
+    <t>SWATE annotation table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a test </t>
   </si>
 </sst>
 </file>
@@ -297,7 +300,7 @@
     <numFmt numFmtId="165" formatCode="0.00\ &quot;percent&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -315,6 +318,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -372,10 +390,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -390,9 +410,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{13734DA0-054A-9F4C-97D4-CA0666BA285F}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{EA6456B1-9345-674B-83C0-73CFBFB7004A}"/>
   </cellStyles>
   <dxfs count="23">
     <dxf>
@@ -478,8 +503,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7A0FDF1-D7A7-5444-9FF6-B24A8DE79F17}" name="annotationTable" displayName="annotationTable" ref="A2:CH3" totalsRowShown="0">
-  <autoFilter ref="A2:CH3" xr:uid="{8A7F28C9-E08B-8A4D-99FD-3313667921ED}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7A0FDF1-D7A7-5444-9FF6-B24A8DE79F17}" name="annotationTable" displayName="annotationTable" ref="C2:CJ3" totalsRowShown="0">
+  <autoFilter ref="C2:CJ3" xr:uid="{8A7F28C9-E08B-8A4D-99FD-3313667921ED}"/>
   <tableColumns count="86">
     <tableColumn id="1" xr3:uid="{9B8F9057-2F20-7A45-8C27-9A36422B26D5}" name="Source Name"/>
     <tableColumn id="2" xr3:uid="{CC93B5FA-49F4-9B4C-B1F6-452471229F30}" name="Sample Name"/>
@@ -887,106 +912,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3613D5-BDC4-E141-9C9A-87C99351C8EE}">
-  <dimension ref="A1:CH10"/>
+  <dimension ref="A1:CJ18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BT1" workbookViewId="0">
-      <selection activeCell="CC13" sqref="CC13:CC14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="65.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="57.33203125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="51.1640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="57.33203125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="55.1640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="61.33203125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="52.1640625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="47.5" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="53.6640625" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="44.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="65.33203125" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="71.5" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="58.6640625" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="64.83203125" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="58.6640625" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="64.83203125" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="58.5" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="64.6640625" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="65.5" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="76.33203125" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="82.5" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="54.6640625" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="61" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="35.5" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="46.33203125" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="52.5" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="56" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="62.1640625" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="38.5" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="49.33203125" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="55.6640625" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="57.83203125" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="64" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="41.33203125" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="52.1640625" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="58.33203125" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="59" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="65.33203125" hidden="1" customWidth="1"/>
-    <col min="57" max="57" width="44.33203125" hidden="1" customWidth="1"/>
-    <col min="58" max="58" width="55.33203125" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="61.5" hidden="1" customWidth="1"/>
-    <col min="60" max="60" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="54.33203125" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="60.6640625" hidden="1" customWidth="1"/>
-    <col min="63" max="63" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="58.33203125" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="64.5" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="57.33203125" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="63.5" hidden="1" customWidth="1"/>
-    <col min="69" max="69" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="56.33203125" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="62.5" hidden="1" customWidth="1"/>
-    <col min="72" max="72" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="52" hidden="1" customWidth="1"/>
-    <col min="74" max="74" width="58.1640625" hidden="1" customWidth="1"/>
-    <col min="75" max="75" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="65" hidden="1" customWidth="1"/>
-    <col min="77" max="77" width="71.33203125" hidden="1" customWidth="1"/>
-    <col min="78" max="78" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="69.1640625" hidden="1" customWidth="1"/>
-    <col min="80" max="80" width="75.33203125" hidden="1" customWidth="1"/>
-    <col min="81" max="81" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="56.1640625" hidden="1" customWidth="1"/>
-    <col min="83" max="83" width="62.33203125" hidden="1" customWidth="1"/>
-    <col min="84" max="84" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="33.1640625" hidden="1" customWidth="1"/>
-    <col min="86" max="86" width="39.5" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="65.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.1640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="57.33203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51.1640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="57.33203125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="55.1640625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="61.33203125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="46" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="52.1640625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.5" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="53.6640625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="65.33203125" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="71.5" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="58.6640625" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="64.83203125" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="58.6640625" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="64.83203125" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="58.5" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="64.6640625" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="65.5" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="76.33203125" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="82.5" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="54.6640625" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="61" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="35.5" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="46.33203125" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="52.5" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="56" hidden="1" customWidth="1"/>
+    <col min="46" max="46" width="62.1640625" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="38.5" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="49.33203125" hidden="1" customWidth="1"/>
+    <col min="49" max="49" width="55.6640625" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="57.83203125" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="64" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="41.33203125" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="52.1640625" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="58.33203125" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="59" hidden="1" customWidth="1"/>
+    <col min="58" max="58" width="65.33203125" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="44.33203125" hidden="1" customWidth="1"/>
+    <col min="60" max="60" width="55.33203125" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="61.5" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="54.33203125" hidden="1" customWidth="1"/>
+    <col min="64" max="64" width="60.6640625" hidden="1" customWidth="1"/>
+    <col min="65" max="65" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="58.33203125" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="64.5" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="57.33203125" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="63.5" hidden="1" customWidth="1"/>
+    <col min="71" max="71" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="56.33203125" hidden="1" customWidth="1"/>
+    <col min="73" max="73" width="62.5" hidden="1" customWidth="1"/>
+    <col min="74" max="74" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="52" hidden="1" customWidth="1"/>
+    <col min="76" max="76" width="58.1640625" hidden="1" customWidth="1"/>
+    <col min="77" max="77" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="65" hidden="1" customWidth="1"/>
+    <col min="79" max="79" width="71.33203125" hidden="1" customWidth="1"/>
+    <col min="80" max="80" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="69.1640625" hidden="1" customWidth="1"/>
+    <col min="82" max="82" width="75.33203125" hidden="1" customWidth="1"/>
+    <col min="83" max="83" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="56.1640625" hidden="1" customWidth="1"/>
+    <col min="85" max="85" width="62.33203125" hidden="1" customWidth="1"/>
+    <col min="86" max="86" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="33.1640625" hidden="1" customWidth="1"/>
+    <col min="88" max="88" width="39.5" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+    <row r="1" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="1"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -1069,296 +1098,306 @@
       <c r="CE1" s="4"/>
       <c r="CF1" s="4"/>
       <c r="CG1" s="4"/>
-      <c r="CH1" s="2"/>
+      <c r="CH1" s="4"/>
+      <c r="CI1" s="4"/>
+      <c r="CJ1" s="2"/>
     </row>
-    <row r="2" spans="1:86" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>71</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>72</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>73</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>9</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>11</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>13</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>17</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>18</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>19</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>14</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>15</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>16</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>22</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>24</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
         <v>25</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
         <v>26</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>27</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>28</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AI2" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AJ2" t="s">
         <v>57</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AK2" t="s">
         <v>58</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
         <v>29</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AM2" t="s">
         <v>30</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AN2" t="s">
         <v>31</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AO2" t="s">
         <v>59</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AP2" t="s">
         <v>60</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AQ2" t="s">
         <v>61</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AR2" t="s">
         <v>32</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AS2" t="s">
         <v>33</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AT2" t="s">
         <v>34</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AU2" t="s">
         <v>62</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AV2" t="s">
         <v>63</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AW2" t="s">
         <v>64</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AX2" t="s">
         <v>35</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AY2" t="s">
         <v>36</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AZ2" t="s">
         <v>37</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BA2" t="s">
         <v>65</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BB2" t="s">
         <v>66</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BC2" t="s">
         <v>67</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BD2" t="s">
         <v>38</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BE2" t="s">
         <v>39</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BF2" t="s">
         <v>40</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BG2" t="s">
         <v>68</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BH2" t="s">
         <v>69</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BI2" t="s">
         <v>70</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BJ2" t="s">
         <v>41</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="BK2" t="s">
         <v>42</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="BL2" t="s">
         <v>43</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="BM2" t="s">
         <v>44</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BN2" t="s">
         <v>45</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BO2" t="s">
         <v>46</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BP2" t="s">
         <v>47</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="BQ2" t="s">
         <v>48</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="BR2" t="s">
         <v>49</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BS2" t="s">
         <v>50</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="BT2" t="s">
         <v>51</v>
       </c>
-      <c r="BS2" t="s">
+      <c r="BU2" t="s">
         <v>52</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BV2" t="s">
         <v>53</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BW2" t="s">
         <v>54</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="BX2" t="s">
         <v>55</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="BY2" t="s">
         <v>74</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="BZ2" t="s">
         <v>75</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CA2" t="s">
         <v>76</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CB2" t="s">
         <v>77</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="CC2" t="s">
         <v>78</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CD2" t="s">
         <v>79</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CE2" t="s">
         <v>80</v>
       </c>
-      <c r="CD2" t="s">
+      <c r="CF2" t="s">
         <v>81</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CG2" t="s">
         <v>82</v>
       </c>
-      <c r="CF2" t="s">
+      <c r="CH2" t="s">
+        <v>83</v>
+      </c>
+      <c r="CI2" t="s">
         <v>84</v>
       </c>
-      <c r="CG2" t="s">
+      <c r="CJ2" t="s">
         <v>85</v>
       </c>
-      <c r="CH2" t="s">
+    </row>
+    <row r="3" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>86</v>
       </c>
+      <c r="B3" s="8"/>
+      <c r="E3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AF3" s="5"/>
+      <c r="AL3" s="6"/>
+      <c r="AR3" s="6"/>
+      <c r="AX3" s="7"/>
+      <c r="BD3" s="7"/>
+      <c r="BJ3" s="3"/>
+      <c r="BM3" s="3"/>
+      <c r="BP3" s="3"/>
+      <c r="BS3" s="3"/>
+      <c r="BV3" s="3"/>
+      <c r="BY3" s="3"/>
+      <c r="CB3" s="3"/>
+      <c r="CE3" s="3"/>
+      <c r="CH3" s="3"/>
     </row>
-    <row r="3" spans="1:86" x14ac:dyDescent="0.2">
-      <c r="C3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AD3" s="5"/>
-      <c r="AJ3" s="6"/>
-      <c r="AP3" s="6"/>
-      <c r="AV3" s="7"/>
-      <c r="BB3" s="7"/>
-      <c r="BH3" s="3"/>
-      <c r="BK3" s="3"/>
-      <c r="BN3" s="3"/>
-      <c r="BQ3" s="3"/>
-      <c r="BT3" s="3"/>
-      <c r="BW3" s="3"/>
-      <c r="BZ3" s="3"/>
-      <c r="CC3" s="3"/>
-      <c r="CF3" s="3"/>
-    </row>
-    <row r="10" spans="1:86" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>83</v>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test: adding additional key to pointer json
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants/1SPL01_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/1SPL01_plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A050A96-C1EB-284A-B4B8-7C0B1EDAF26E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566F1BD4-521B-DC47-B013-D7ABB890A444}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25940" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="-25900" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="2" r:id="rId1"/>
@@ -2085,7 +2085,7 @@
   <dimension ref="A1:CK71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="CE1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add more design attributes
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants/1SPL01_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/1SPL01_plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555FE9F5-70B4-0346-9E6B-4AB19DCE193F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70074A93-05AC-1048-BC98-B2BBCCF6FCCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25900" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="-4720" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="2" r:id="rId1"/>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{F6B686F7-5A0C-0946-9A32-03596DAB1E5D}">
+    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{F6B686F7-5A0C-0946-9A32-03596DAB1E5D}">
       <text>
         <r>
           <rPr>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="223">
   <si>
     <t>Source Name</t>
   </si>
@@ -685,9 +685,6 @@
     <t>ER target term</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>ER Pipeline: MetaboLights - Metabolomics - Plants</t>
   </si>
   <si>
@@ -827,6 +824,12 @@
   </si>
   <si>
     <t>ER requirement (cv/m/o/n)</t>
+  </si>
+  <si>
+    <t>User instruction</t>
+  </si>
+  <si>
+    <t>Additional information</t>
   </si>
 </sst>
 </file>
@@ -1151,20 +1154,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -1733,6 +1722,20 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -1777,92 +1780,92 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7A0FDF1-D7A7-5444-9FF6-B24A8DE79F17}" name="annotationTable" displayName="annotationTable" ref="C2:CG3" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7A0FDF1-D7A7-5444-9FF6-B24A8DE79F17}" name="annotationTable" displayName="annotationTable" ref="C2:CG3" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83">
   <autoFilter ref="C2:CG3" xr:uid="{8A7F28C9-E08B-8A4D-99FD-3313667921ED}"/>
   <tableColumns count="83">
-    <tableColumn id="1" xr3:uid="{9B8F9057-2F20-7A45-8C27-9A36422B26D5}" name="Source Name" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{CC93B5FA-49F4-9B4C-B1F6-452471229F30}" name="Sample Name" dataDxfId="83"/>
-    <tableColumn id="72" xr3:uid="{A33FCD3B-AD29-A742-9D63-6ECAFBEE068E}" name="Characteristics [Biological replicate]" dataDxfId="82"/>
-    <tableColumn id="73" xr3:uid="{4059FECC-FE9D-5947-9219-570196389DAE}" name="Term Source REF [Biological replicate] (#h; #tNFDI4PSO:0000042)" dataDxfId="81"/>
-    <tableColumn id="74" xr3:uid="{E04811ED-EF58-AD4F-84F5-156D9251E904}" name="Term Accession Number [Biological replicate] (#h; #tNFDI4PSO:0000042)" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{6A7FF2B3-5F1E-8245-AC4F-6198097A8123}" name="Characteristics [Organism]" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{CC831F2C-80A0-C84F-829F-23F6C78F2EEB}" name="Term Source REF [Organism] (#h; #tNFDI4PSO:0000030)" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{D6E59B6D-D53F-A840-A182-24AE5A460E1D}" name="Term Accession Number [Organism] (#h; #tNFDI4PSO:0000030)" dataDxfId="77"/>
-    <tableColumn id="14" xr3:uid="{000DCCE3-5EF7-4F4E-A82A-AD088FF36730}" name="Characteristics [Genotype]" dataDxfId="76"/>
-    <tableColumn id="15" xr3:uid="{E2A1AEEB-EF2B-F448-824C-2953C18CC24A}" name="Term Source REF [Genotype] (#h; #tNFDI4PSO:0000031)" dataDxfId="75"/>
-    <tableColumn id="16" xr3:uid="{A998FE5F-8994-6E40-94FA-F0EF6DC905E4}" name="Term Accession Number [Genotype] (#h; #tNFDI4PSO:0000031)" dataDxfId="74"/>
-    <tableColumn id="17" xr3:uid="{0EB867DC-9BB4-6243-BEE9-01764D9FEB35}" name="Characteristics [Organism part]" dataDxfId="73"/>
-    <tableColumn id="18" xr3:uid="{B0CCF08F-B694-6C4F-94E6-E17AFD4C0A63}" name="Term Source REF [Organism part] (#h; #tNFDI4PSO:0000032)" dataDxfId="72"/>
-    <tableColumn id="19" xr3:uid="{6A02A31E-2B72-BE41-BF86-71E587B29D13}" name="Term Accession Number [Organism part] (#h; #tNFDI4PSO:0000032)" dataDxfId="71"/>
-    <tableColumn id="20" xr3:uid="{96C34AC4-65C0-774B-A5A0-1BC98C955028}" name="Characteristics [age]" dataDxfId="70"/>
-    <tableColumn id="21" xr3:uid="{325D3F43-A306-2F47-AD9C-92F61C0649E5}" name="Term Source REF [age] (#h; #tNFDI4PSO:0000033)" dataDxfId="69"/>
-    <tableColumn id="22" xr3:uid="{334AF647-E268-2E41-950D-8973A43E29C8}" name="Term Accession Number [age] (#h; #tNFDI4PSO:0000033)" dataDxfId="68"/>
-    <tableColumn id="26" xr3:uid="{5E219BCA-059A-CC41-93BF-8CD61AA9572D}" name="Characteristics [study type]" dataDxfId="67"/>
-    <tableColumn id="27" xr3:uid="{5FF2BBBF-350F-9842-8FDF-2F895B07EADF}" name="Term Source REF [study type] (#h; #tPECO:0007231)" dataDxfId="66"/>
-    <tableColumn id="28" xr3:uid="{E12790EC-754D-3244-8A7A-1242F7942612}" name="Term Accession Number [study type] (#h; #tPECO:0007231)" dataDxfId="65"/>
-    <tableColumn id="23" xr3:uid="{E0A293FE-1EF5-A949-9C12-ADF40314B418}" name="Characteristics [plant growth medium exposure]" dataDxfId="64"/>
-    <tableColumn id="24" xr3:uid="{0C19F4A6-F9E8-1F4F-9B61-EB31E6DF451A}" name="Term Source REF [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="63"/>
-    <tableColumn id="25" xr3:uid="{7BBED07D-F814-A245-B090-723342B3D631}" name="Term Accession Number [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="62"/>
-    <tableColumn id="29" xr3:uid="{C386EF1A-F4F8-C543-99A0-ABD311BD175F}" name="Characteristics [growth plot design]" dataDxfId="61"/>
-    <tableColumn id="30" xr3:uid="{86FAE20B-4F89-EE4F-91E6-CE3B7E712F95}" name="Term Source REF [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="60"/>
-    <tableColumn id="31" xr3:uid="{C0949892-595C-9742-BCD1-75134FAC012F}" name="Term Accession Number [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="59"/>
-    <tableColumn id="32" xr3:uid="{B90A4652-69D5-2E4F-8A64-A3A5A5CB24DB}" name="Characteristics [Growth day length]" dataDxfId="58"/>
-    <tableColumn id="33" xr3:uid="{4E2448E1-3D08-504C-8FE3-D71B801F4DC9}" name="Term Source REF [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="57"/>
-    <tableColumn id="34" xr3:uid="{D47410BE-0000-B648-8CE5-966EE8968909}" name="Term Accession Number [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="56"/>
-    <tableColumn id="35" xr3:uid="{27034924-8879-044A-819B-7DC832A9D603}" name="Characteristics [light intensity exposure]" dataDxfId="55"/>
-    <tableColumn id="36" xr3:uid="{FD04748E-7F58-4A46-A167-E5EB1375A50B}" name="Term Source REF [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="54"/>
-    <tableColumn id="37" xr3:uid="{D76E6422-DF20-B94A-B5A6-4FD7F7923EBF}" name="Term Accession Number [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{8E446DD1-817A-E84A-9536-47B88B72BFD8}" name="Unit [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{BCB29467-6D87-F141-98A0-60243765731F}" name="Term Source REF [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{D2565EAD-7C86-C343-800D-E37FD463093B}" name="Term Accession Number [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="50"/>
-    <tableColumn id="38" xr3:uid="{21746D48-E9A2-5B42-BC00-F5AFD4793AA7}" name="Characteristics [Humidity Day]" dataDxfId="49"/>
-    <tableColumn id="39" xr3:uid="{8B1D9CC4-6026-674C-9852-06A06365907B}" name="Term Source REF [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="48"/>
-    <tableColumn id="40" xr3:uid="{8CCA0026-8267-884E-8F9A-369ACCB825EA}" name="Term Accession Number [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{9508FD23-5388-F64E-8286-05B533856CA2}" name="Unit [percent] (#h; #tUO:0000187; #u)" dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{F796BC22-CBE1-6D41-824E-F655C3F9D5B6}" name="Term Source REF [percent] (#h; #tUO:0000187; #u)" dataDxfId="45"/>
-    <tableColumn id="11" xr3:uid="{32AC3DD8-82CD-4349-BFD5-0805A34144D8}" name="Term Accession Number [percent] (#h; #tUO:0000187; #u)" dataDxfId="44"/>
-    <tableColumn id="41" xr3:uid="{F4E42B79-6B62-E34C-95BE-8906E80BFBC8}" name="Characteristics [Humidity Night]" dataDxfId="43"/>
-    <tableColumn id="42" xr3:uid="{FE26FC08-E3D1-7547-8E20-1363EF47EE86}" name="Term Source REF [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="42"/>
-    <tableColumn id="43" xr3:uid="{C6D20AF0-60A8-874E-9614-2A2F483EB262}" name="Term Accession Number [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="41"/>
-    <tableColumn id="12" xr3:uid="{2866C2CF-81B3-694E-B2D9-F69059F54AA2}" name="Unit [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="40"/>
-    <tableColumn id="13" xr3:uid="{A885FE47-7729-3B45-B73D-03FF1F114CD5}" name="Term Source REF [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="39"/>
-    <tableColumn id="65" xr3:uid="{A3AEBB25-5500-F249-866E-C98439259F17}" name="Term Accession Number [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="38"/>
-    <tableColumn id="44" xr3:uid="{F0571376-132B-F940-9609-6B59D9845B1B}" name="Characteristics [Temperature Day]" dataDxfId="37"/>
-    <tableColumn id="45" xr3:uid="{23233498-CFC4-9F46-94D5-39E7A6B5AFB5}" name="Term Source REF [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="36"/>
-    <tableColumn id="46" xr3:uid="{346D483D-D0DE-5140-A015-4AD0367BAD4D}" name="Term Accession Number [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="35"/>
-    <tableColumn id="66" xr3:uid="{57808D06-1B53-8D41-BEB4-1644A20F7763}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="34"/>
-    <tableColumn id="67" xr3:uid="{A7356A0D-0EFD-3D44-9B2F-4566273E79E8}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="33"/>
-    <tableColumn id="68" xr3:uid="{AD21FFE5-445B-CB42-B199-FDD8BAD5635D}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="32"/>
-    <tableColumn id="47" xr3:uid="{2AB78931-B301-314A-9311-2CC2C21128D4}" name="Characteristics [Temperature Night]" dataDxfId="31"/>
-    <tableColumn id="48" xr3:uid="{3A76D4EC-C74F-0A4B-B340-8EF3D8B86ECB}" name="Term Source REF [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="30"/>
-    <tableColumn id="49" xr3:uid="{87034985-F2AC-A145-AA6A-9EDB63F919F9}" name="Term Accession Number [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="29"/>
-    <tableColumn id="69" xr3:uid="{6D54D968-A087-944D-BF64-3AC3D5B08F80}" name="Unit [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="28"/>
-    <tableColumn id="70" xr3:uid="{AE04B49D-BF47-F34B-B52A-752ECD10B8C7}" name="Term Source REF [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="27"/>
-    <tableColumn id="71" xr3:uid="{2A40040A-D450-EF49-AB82-0CEEB3D8A599}" name="Term Accession Number [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="26"/>
-    <tableColumn id="50" xr3:uid="{FC29A38A-1769-7349-A9E5-A5184C62F33A}" name="Characteristics [watering exposure]" dataDxfId="25"/>
-    <tableColumn id="51" xr3:uid="{808AA82E-ECE0-AD47-92D3-27D7C93007B7}" name="Term Source REF [watering exposure] (#h; #tPECO:0007383)" dataDxfId="24"/>
-    <tableColumn id="52" xr3:uid="{7C45B5F9-759B-E646-A40E-CB5363DF17A8}" name="Term Accession Number [watering exposure] (#h; #tPECO:0007383)" dataDxfId="23"/>
-    <tableColumn id="53" xr3:uid="{70DF5752-BECA-5342-9001-FA7F5271BC54}" name="Characteristics [plant nutrient exposure]" dataDxfId="22"/>
-    <tableColumn id="54" xr3:uid="{FD6AD7C0-D253-D04C-8B67-6124B6C5D685}" name="Term Source REF [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="21"/>
-    <tableColumn id="55" xr3:uid="{95BC5752-0FFE-8C4E-BFE3-4FED8B72A648}" name="Term Accession Number [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="20"/>
-    <tableColumn id="56" xr3:uid="{25540F7D-0E49-F74B-8EF6-6E2314EBD1B1}" name="Characteristics [abiotic plant exposure]" dataDxfId="19"/>
-    <tableColumn id="57" xr3:uid="{19EC9032-1152-F940-ADB1-397E054EED4E}" name="Term Source REF [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="18"/>
-    <tableColumn id="58" xr3:uid="{40EA0154-215C-C44C-A5D6-852F5DA9A25C}" name="Term Accession Number [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="17"/>
-    <tableColumn id="59" xr3:uid="{C208C009-B835-0041-9A5C-978B7EABB59C}" name="Characteristics [biotic plant exposure]" dataDxfId="16"/>
-    <tableColumn id="60" xr3:uid="{2836636A-01C7-9C4E-9B41-EE6FEE3D7B80}" name="Term Source REF [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="15"/>
-    <tableColumn id="61" xr3:uid="{E4A74FCF-2E01-354A-99CE-0602774F8706}" name="Term Accession Number [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="14"/>
-    <tableColumn id="62" xr3:uid="{12C4BED6-C71D-CC43-B976-AECFD0AF0BCF}" name="Characteristics [Time point]" dataDxfId="13"/>
-    <tableColumn id="63" xr3:uid="{D78E63DF-76E2-AE4F-A9AA-86CB096E0FD1}" name="Term Source REF [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="12"/>
-    <tableColumn id="64" xr3:uid="{4E3E838B-D518-9B41-95E4-AE65DE3C4242}" name="Term Accession Number [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="11"/>
-    <tableColumn id="75" xr3:uid="{7FBEC602-6866-EE4C-901B-A620EADE0B55}" name="Parameter [Sample Collection Method]" dataDxfId="10"/>
-    <tableColumn id="76" xr3:uid="{082E37E1-9067-2344-AFED-4C0AB2E6608F}" name="Term Source REF [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="9"/>
-    <tableColumn id="77" xr3:uid="{23CA10DE-9FDA-A94D-84CF-7C5F7143EE90}" name="Term Accession Number [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="8"/>
-    <tableColumn id="78" xr3:uid="{DD36BBD7-7DDE-4B4B-B0E7-E088C0737C72}" name="Parameter [Metabolism quenching method]" dataDxfId="7"/>
-    <tableColumn id="79" xr3:uid="{E9A2A827-A7E3-E44F-8034-982633580E8D}" name="Term Source REF [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="6"/>
-    <tableColumn id="80" xr3:uid="{ECB588C7-B9C0-8741-BE8A-1CDECCED4ED4}" name="Term Accession Number [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="5"/>
-    <tableColumn id="81" xr3:uid="{125431A9-D115-4A4B-A917-1C0A2F361D5C}" name="Parameter [Sample storage]" dataDxfId="4"/>
-    <tableColumn id="82" xr3:uid="{A56F8F05-EAAB-FD40-8F2F-AD66235065C4}" name="Term Source REF [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="3"/>
-    <tableColumn id="83" xr3:uid="{AB05BD40-EE64-3547-80D7-EDD26BB0F77A}" name="Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9B8F9057-2F20-7A45-8C27-9A36422B26D5}" name="Source Name" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{CC93B5FA-49F4-9B4C-B1F6-452471229F30}" name="Sample Name" dataDxfId="81"/>
+    <tableColumn id="72" xr3:uid="{A33FCD3B-AD29-A742-9D63-6ECAFBEE068E}" name="Characteristics [Biological replicate]" dataDxfId="80"/>
+    <tableColumn id="73" xr3:uid="{4059FECC-FE9D-5947-9219-570196389DAE}" name="Term Source REF [Biological replicate] (#h; #tNFDI4PSO:0000042)" dataDxfId="79"/>
+    <tableColumn id="74" xr3:uid="{E04811ED-EF58-AD4F-84F5-156D9251E904}" name="Term Accession Number [Biological replicate] (#h; #tNFDI4PSO:0000042)" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{6A7FF2B3-5F1E-8245-AC4F-6198097A8123}" name="Characteristics [Organism]" dataDxfId="77"/>
+    <tableColumn id="4" xr3:uid="{CC831F2C-80A0-C84F-829F-23F6C78F2EEB}" name="Term Source REF [Organism] (#h; #tNFDI4PSO:0000030)" dataDxfId="76"/>
+    <tableColumn id="5" xr3:uid="{D6E59B6D-D53F-A840-A182-24AE5A460E1D}" name="Term Accession Number [Organism] (#h; #tNFDI4PSO:0000030)" dataDxfId="75"/>
+    <tableColumn id="14" xr3:uid="{000DCCE3-5EF7-4F4E-A82A-AD088FF36730}" name="Characteristics [Genotype]" dataDxfId="74"/>
+    <tableColumn id="15" xr3:uid="{E2A1AEEB-EF2B-F448-824C-2953C18CC24A}" name="Term Source REF [Genotype] (#h; #tNFDI4PSO:0000031)" dataDxfId="73"/>
+    <tableColumn id="16" xr3:uid="{A998FE5F-8994-6E40-94FA-F0EF6DC905E4}" name="Term Accession Number [Genotype] (#h; #tNFDI4PSO:0000031)" dataDxfId="72"/>
+    <tableColumn id="17" xr3:uid="{0EB867DC-9BB4-6243-BEE9-01764D9FEB35}" name="Characteristics [Organism part]" dataDxfId="71"/>
+    <tableColumn id="18" xr3:uid="{B0CCF08F-B694-6C4F-94E6-E17AFD4C0A63}" name="Term Source REF [Organism part] (#h; #tNFDI4PSO:0000032)" dataDxfId="70"/>
+    <tableColumn id="19" xr3:uid="{6A02A31E-2B72-BE41-BF86-71E587B29D13}" name="Term Accession Number [Organism part] (#h; #tNFDI4PSO:0000032)" dataDxfId="69"/>
+    <tableColumn id="20" xr3:uid="{96C34AC4-65C0-774B-A5A0-1BC98C955028}" name="Characteristics [age]" dataDxfId="68"/>
+    <tableColumn id="21" xr3:uid="{325D3F43-A306-2F47-AD9C-92F61C0649E5}" name="Term Source REF [age] (#h; #tNFDI4PSO:0000033)" dataDxfId="67"/>
+    <tableColumn id="22" xr3:uid="{334AF647-E268-2E41-950D-8973A43E29C8}" name="Term Accession Number [age] (#h; #tNFDI4PSO:0000033)" dataDxfId="66"/>
+    <tableColumn id="26" xr3:uid="{5E219BCA-059A-CC41-93BF-8CD61AA9572D}" name="Characteristics [study type]" dataDxfId="65"/>
+    <tableColumn id="27" xr3:uid="{5FF2BBBF-350F-9842-8FDF-2F895B07EADF}" name="Term Source REF [study type] (#h; #tPECO:0007231)" dataDxfId="64"/>
+    <tableColumn id="28" xr3:uid="{E12790EC-754D-3244-8A7A-1242F7942612}" name="Term Accession Number [study type] (#h; #tPECO:0007231)" dataDxfId="63"/>
+    <tableColumn id="23" xr3:uid="{E0A293FE-1EF5-A949-9C12-ADF40314B418}" name="Characteristics [plant growth medium exposure]" dataDxfId="62"/>
+    <tableColumn id="24" xr3:uid="{0C19F4A6-F9E8-1F4F-9B61-EB31E6DF451A}" name="Term Source REF [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="61"/>
+    <tableColumn id="25" xr3:uid="{7BBED07D-F814-A245-B090-723342B3D631}" name="Term Accession Number [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="60"/>
+    <tableColumn id="29" xr3:uid="{C386EF1A-F4F8-C543-99A0-ABD311BD175F}" name="Characteristics [growth plot design]" dataDxfId="59"/>
+    <tableColumn id="30" xr3:uid="{86FAE20B-4F89-EE4F-91E6-CE3B7E712F95}" name="Term Source REF [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="58"/>
+    <tableColumn id="31" xr3:uid="{C0949892-595C-9742-BCD1-75134FAC012F}" name="Term Accession Number [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="57"/>
+    <tableColumn id="32" xr3:uid="{B90A4652-69D5-2E4F-8A64-A3A5A5CB24DB}" name="Characteristics [Growth day length]" dataDxfId="56"/>
+    <tableColumn id="33" xr3:uid="{4E2448E1-3D08-504C-8FE3-D71B801F4DC9}" name="Term Source REF [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="55"/>
+    <tableColumn id="34" xr3:uid="{D47410BE-0000-B648-8CE5-966EE8968909}" name="Term Accession Number [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="54"/>
+    <tableColumn id="35" xr3:uid="{27034924-8879-044A-819B-7DC832A9D603}" name="Characteristics [light intensity exposure]" dataDxfId="53"/>
+    <tableColumn id="36" xr3:uid="{FD04748E-7F58-4A46-A167-E5EB1375A50B}" name="Term Source REF [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="52"/>
+    <tableColumn id="37" xr3:uid="{D76E6422-DF20-B94A-B5A6-4FD7F7923EBF}" name="Term Accession Number [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{8E446DD1-817A-E84A-9536-47B88B72BFD8}" name="Unit [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{BCB29467-6D87-F141-98A0-60243765731F}" name="Term Source REF [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{D2565EAD-7C86-C343-800D-E37FD463093B}" name="Term Accession Number [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="48"/>
+    <tableColumn id="38" xr3:uid="{21746D48-E9A2-5B42-BC00-F5AFD4793AA7}" name="Characteristics [Humidity Day]" dataDxfId="47"/>
+    <tableColumn id="39" xr3:uid="{8B1D9CC4-6026-674C-9852-06A06365907B}" name="Term Source REF [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="46"/>
+    <tableColumn id="40" xr3:uid="{8CCA0026-8267-884E-8F9A-369ACCB825EA}" name="Term Accession Number [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{9508FD23-5388-F64E-8286-05B533856CA2}" name="Unit [percent] (#h; #tUO:0000187; #u)" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{F796BC22-CBE1-6D41-824E-F655C3F9D5B6}" name="Term Source REF [percent] (#h; #tUO:0000187; #u)" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{32AC3DD8-82CD-4349-BFD5-0805A34144D8}" name="Term Accession Number [percent] (#h; #tUO:0000187; #u)" dataDxfId="42"/>
+    <tableColumn id="41" xr3:uid="{F4E42B79-6B62-E34C-95BE-8906E80BFBC8}" name="Characteristics [Humidity Night]" dataDxfId="41"/>
+    <tableColumn id="42" xr3:uid="{FE26FC08-E3D1-7547-8E20-1363EF47EE86}" name="Term Source REF [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="40"/>
+    <tableColumn id="43" xr3:uid="{C6D20AF0-60A8-874E-9614-2A2F483EB262}" name="Term Accession Number [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{2866C2CF-81B3-694E-B2D9-F69059F54AA2}" name="Unit [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="38"/>
+    <tableColumn id="13" xr3:uid="{A885FE47-7729-3B45-B73D-03FF1F114CD5}" name="Term Source REF [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="37"/>
+    <tableColumn id="65" xr3:uid="{A3AEBB25-5500-F249-866E-C98439259F17}" name="Term Accession Number [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="36"/>
+    <tableColumn id="44" xr3:uid="{F0571376-132B-F940-9609-6B59D9845B1B}" name="Characteristics [Temperature Day]" dataDxfId="35"/>
+    <tableColumn id="45" xr3:uid="{23233498-CFC4-9F46-94D5-39E7A6B5AFB5}" name="Term Source REF [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="34"/>
+    <tableColumn id="46" xr3:uid="{346D483D-D0DE-5140-A015-4AD0367BAD4D}" name="Term Accession Number [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="33"/>
+    <tableColumn id="66" xr3:uid="{57808D06-1B53-8D41-BEB4-1644A20F7763}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="32"/>
+    <tableColumn id="67" xr3:uid="{A7356A0D-0EFD-3D44-9B2F-4566273E79E8}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="31"/>
+    <tableColumn id="68" xr3:uid="{AD21FFE5-445B-CB42-B199-FDD8BAD5635D}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="30"/>
+    <tableColumn id="47" xr3:uid="{2AB78931-B301-314A-9311-2CC2C21128D4}" name="Characteristics [Temperature Night]" dataDxfId="29"/>
+    <tableColumn id="48" xr3:uid="{3A76D4EC-C74F-0A4B-B340-8EF3D8B86ECB}" name="Term Source REF [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="28"/>
+    <tableColumn id="49" xr3:uid="{87034985-F2AC-A145-AA6A-9EDB63F919F9}" name="Term Accession Number [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="27"/>
+    <tableColumn id="69" xr3:uid="{6D54D968-A087-944D-BF64-3AC3D5B08F80}" name="Unit [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="26"/>
+    <tableColumn id="70" xr3:uid="{AE04B49D-BF47-F34B-B52A-752ECD10B8C7}" name="Term Source REF [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="25"/>
+    <tableColumn id="71" xr3:uid="{2A40040A-D450-EF49-AB82-0CEEB3D8A599}" name="Term Accession Number [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="24"/>
+    <tableColumn id="50" xr3:uid="{FC29A38A-1769-7349-A9E5-A5184C62F33A}" name="Characteristics [watering exposure]" dataDxfId="23"/>
+    <tableColumn id="51" xr3:uid="{808AA82E-ECE0-AD47-92D3-27D7C93007B7}" name="Term Source REF [watering exposure] (#h; #tPECO:0007383)" dataDxfId="22"/>
+    <tableColumn id="52" xr3:uid="{7C45B5F9-759B-E646-A40E-CB5363DF17A8}" name="Term Accession Number [watering exposure] (#h; #tPECO:0007383)" dataDxfId="21"/>
+    <tableColumn id="53" xr3:uid="{70DF5752-BECA-5342-9001-FA7F5271BC54}" name="Characteristics [plant nutrient exposure]" dataDxfId="20"/>
+    <tableColumn id="54" xr3:uid="{FD6AD7C0-D253-D04C-8B67-6124B6C5D685}" name="Term Source REF [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="19"/>
+    <tableColumn id="55" xr3:uid="{95BC5752-0FFE-8C4E-BFE3-4FED8B72A648}" name="Term Accession Number [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="18"/>
+    <tableColumn id="56" xr3:uid="{25540F7D-0E49-F74B-8EF6-6E2314EBD1B1}" name="Characteristics [abiotic plant exposure]" dataDxfId="17"/>
+    <tableColumn id="57" xr3:uid="{19EC9032-1152-F940-ADB1-397E054EED4E}" name="Term Source REF [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="16"/>
+    <tableColumn id="58" xr3:uid="{40EA0154-215C-C44C-A5D6-852F5DA9A25C}" name="Term Accession Number [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="15"/>
+    <tableColumn id="59" xr3:uid="{C208C009-B835-0041-9A5C-978B7EABB59C}" name="Characteristics [biotic plant exposure]" dataDxfId="14"/>
+    <tableColumn id="60" xr3:uid="{2836636A-01C7-9C4E-9B41-EE6FEE3D7B80}" name="Term Source REF [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="13"/>
+    <tableColumn id="61" xr3:uid="{E4A74FCF-2E01-354A-99CE-0602774F8706}" name="Term Accession Number [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="12"/>
+    <tableColumn id="62" xr3:uid="{12C4BED6-C71D-CC43-B976-AECFD0AF0BCF}" name="Characteristics [Time point]" dataDxfId="11"/>
+    <tableColumn id="63" xr3:uid="{D78E63DF-76E2-AE4F-A9AA-86CB096E0FD1}" name="Term Source REF [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="10"/>
+    <tableColumn id="64" xr3:uid="{4E3E838B-D518-9B41-95E4-AE65DE3C4242}" name="Term Accession Number [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="9"/>
+    <tableColumn id="75" xr3:uid="{7FBEC602-6866-EE4C-901B-A620EADE0B55}" name="Parameter [Sample Collection Method]" dataDxfId="8"/>
+    <tableColumn id="76" xr3:uid="{082E37E1-9067-2344-AFED-4C0AB2E6608F}" name="Term Source REF [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="7"/>
+    <tableColumn id="77" xr3:uid="{23CA10DE-9FDA-A94D-84CF-7C5F7143EE90}" name="Term Accession Number [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="6"/>
+    <tableColumn id="78" xr3:uid="{DD36BBD7-7DDE-4B4B-B0E7-E088C0737C72}" name="Parameter [Metabolism quenching method]" dataDxfId="5"/>
+    <tableColumn id="79" xr3:uid="{E9A2A827-A7E3-E44F-8034-982633580E8D}" name="Term Source REF [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="4"/>
+    <tableColumn id="80" xr3:uid="{ECB588C7-B9C0-8741-BE8A-1CDECCED4ED4}" name="Term Accession Number [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="3"/>
+    <tableColumn id="81" xr3:uid="{125431A9-D115-4A4B-A917-1C0A2F361D5C}" name="Parameter [Sample storage]" dataDxfId="2"/>
+    <tableColumn id="82" xr3:uid="{A56F8F05-EAAB-FD40-8F2F-AD66235065C4}" name="Term Source REF [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="1"/>
+    <tableColumn id="83" xr3:uid="{AB05BD40-EE64-3547-80D7-EDD26BB0F77A}" name="Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2183,13 +2186,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3613D5-BDC4-E141-9C9A-87C99351C8EE}">
-  <dimension ref="A1:CK73"/>
+  <dimension ref="A1:CG75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="20" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16:XFD16"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3409,27 +3412,27 @@
       <c r="L11" s="32"/>
       <c r="M11" s="32"/>
       <c r="N11" s="32" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O11" s="32"/>
       <c r="P11" s="32"/>
       <c r="Q11" s="32" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R11" s="32"/>
       <c r="S11" s="32"/>
       <c r="T11" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="U11" s="32"/>
       <c r="V11" s="32"/>
       <c r="W11" s="33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="X11" s="33"/>
       <c r="Y11" s="33"/>
       <c r="Z11" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AA11" s="33"/>
       <c r="AB11" s="32"/>
@@ -3439,7 +3442,7 @@
       <c r="AD11" s="32"/>
       <c r="AE11" s="32"/>
       <c r="AF11" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AG11" s="32"/>
       <c r="AH11" s="32"/>
@@ -3447,7 +3450,7 @@
       <c r="AJ11" s="32"/>
       <c r="AK11" s="32"/>
       <c r="AL11" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AM11" s="32"/>
       <c r="AN11" s="32"/>
@@ -3455,7 +3458,7 @@
       <c r="AP11" s="32"/>
       <c r="AQ11" s="32"/>
       <c r="AR11" s="32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AS11" s="32"/>
       <c r="AT11" s="32"/>
@@ -3463,7 +3466,7 @@
       <c r="AV11" s="32"/>
       <c r="AW11" s="32"/>
       <c r="AX11" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AY11" s="32"/>
       <c r="AZ11" s="32"/>
@@ -3471,7 +3474,7 @@
       <c r="BB11" s="32"/>
       <c r="BC11" s="32"/>
       <c r="BD11" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="BE11" s="32"/>
       <c r="BF11" s="32"/>
@@ -3479,27 +3482,27 @@
       <c r="BH11" s="32"/>
       <c r="BI11" s="32"/>
       <c r="BJ11" s="32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="BK11" s="32"/>
       <c r="BL11" s="32"/>
       <c r="BM11" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="BN11" s="32"/>
       <c r="BO11" s="32"/>
       <c r="BP11" s="32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="BQ11" s="32"/>
       <c r="BR11" s="32"/>
       <c r="BS11" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="BT11" s="32"/>
       <c r="BU11" s="32"/>
       <c r="BV11" s="32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="BW11" s="32"/>
       <c r="BX11" s="32"/>
@@ -3554,17 +3557,17 @@
       <c r="R12" s="36"/>
       <c r="S12" s="36"/>
       <c r="T12" s="36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="U12" s="36"/>
       <c r="V12" s="36"/>
       <c r="W12" s="36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="X12" s="37"/>
       <c r="Y12" s="37"/>
       <c r="Z12" s="37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AA12" s="37"/>
       <c r="AB12" s="38"/>
@@ -3574,7 +3577,7 @@
       <c r="AD12" s="36"/>
       <c r="AE12" s="36"/>
       <c r="AF12" s="36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AG12" s="36"/>
       <c r="AH12" s="36"/>
@@ -3582,7 +3585,7 @@
       <c r="AJ12" s="36"/>
       <c r="AK12" s="36"/>
       <c r="AL12" s="38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AM12" s="38"/>
       <c r="AN12" s="38"/>
@@ -3590,7 +3593,7 @@
       <c r="AP12" s="38"/>
       <c r="AQ12" s="38"/>
       <c r="AR12" s="38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AS12" s="38"/>
       <c r="AT12" s="38"/>
@@ -3598,7 +3601,7 @@
       <c r="AV12" s="38"/>
       <c r="AW12" s="38"/>
       <c r="AX12" s="38" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AY12" s="38"/>
       <c r="AZ12" s="38"/>
@@ -3606,7 +3609,7 @@
       <c r="BB12" s="38"/>
       <c r="BC12" s="38"/>
       <c r="BD12" s="36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BE12" s="36"/>
       <c r="BF12" s="36"/>
@@ -3614,42 +3617,42 @@
       <c r="BH12" s="36"/>
       <c r="BI12" s="36"/>
       <c r="BJ12" s="36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="BK12" s="36"/>
       <c r="BL12" s="36"/>
       <c r="BM12" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="BN12" s="36"/>
       <c r="BO12" s="36"/>
       <c r="BP12" s="36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="BQ12" s="36"/>
       <c r="BR12" s="36"/>
       <c r="BS12" s="36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="BT12" s="36"/>
       <c r="BU12" s="36"/>
       <c r="BV12" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="BW12" s="36"/>
       <c r="BX12" s="36"/>
       <c r="BY12" s="36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="BZ12" s="36"/>
       <c r="CA12" s="36"/>
       <c r="CB12" s="36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="CC12" s="36"/>
       <c r="CD12" s="36"/>
       <c r="CE12" s="36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="CF12" s="37"/>
       <c r="CG12" s="37"/>
@@ -3684,7 +3687,7 @@
       <c r="U13" s="40"/>
       <c r="V13" s="40"/>
       <c r="W13" s="42" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="X13" s="41"/>
       <c r="Y13" s="41"/>
@@ -3873,7 +3876,7 @@
         <v>165</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C15" s="44"/>
       <c r="D15" s="44"/>
@@ -4573,66 +4576,66 @@
         <v>173</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
       <c r="K22" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
       <c r="N22" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
       <c r="Q22" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R22" s="15"/>
       <c r="S22" s="15"/>
       <c r="T22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="U22" s="15"/>
       <c r="V22" s="15"/>
       <c r="W22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="X22" s="10"/>
       <c r="Y22" s="10"/>
       <c r="Z22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AA22" s="15"/>
       <c r="AB22" s="15"/>
       <c r="AC22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AD22" s="15"/>
       <c r="AE22" s="15"/>
       <c r="AF22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AG22" s="15"/>
       <c r="AH22" s="15"/>
       <c r="AI22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AJ22" s="15"/>
       <c r="AK22" s="15"/>
       <c r="AL22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AM22" s="15"/>
       <c r="AN22" s="15"/>
@@ -4640,7 +4643,7 @@
       <c r="AP22" s="15"/>
       <c r="AQ22" s="15"/>
       <c r="AR22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AS22" s="15"/>
       <c r="AT22" s="15"/>
@@ -4648,7 +4651,7 @@
       <c r="AV22" s="15"/>
       <c r="AW22" s="15"/>
       <c r="AX22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AY22" s="15"/>
       <c r="AZ22" s="15"/>
@@ -4656,7 +4659,7 @@
       <c r="BB22" s="15"/>
       <c r="BC22" s="15"/>
       <c r="BD22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="BE22" s="15"/>
       <c r="BF22" s="15"/>
@@ -4664,42 +4667,42 @@
       <c r="BH22" s="15"/>
       <c r="BI22" s="15"/>
       <c r="BJ22" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BK22" s="15"/>
       <c r="BL22" s="15"/>
       <c r="BM22" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BN22" s="15"/>
       <c r="BO22" s="15"/>
       <c r="BP22" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BQ22" s="15"/>
       <c r="BR22" s="15"/>
       <c r="BS22" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BT22" s="15"/>
       <c r="BU22" s="15"/>
       <c r="BV22" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BW22" s="15"/>
       <c r="BX22" s="15"/>
       <c r="BY22" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="BZ22" s="15"/>
       <c r="CA22" s="15"/>
       <c r="CB22" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="CC22" s="15"/>
       <c r="CD22" s="15"/>
       <c r="CE22" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="CF22" s="10"/>
       <c r="CG22" s="10"/>
@@ -4709,71 +4712,71 @@
         <v>172</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C23" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>183</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>184</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
       <c r="N23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
       <c r="Q23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="R23" s="15"/>
       <c r="S23" s="15"/>
       <c r="T23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="U23" s="15"/>
       <c r="V23" s="15"/>
       <c r="W23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="X23" s="10"/>
       <c r="Y23" s="10"/>
       <c r="Z23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AA23" s="15"/>
       <c r="AB23" s="15"/>
       <c r="AC23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AD23" s="15"/>
       <c r="AE23" s="15"/>
       <c r="AF23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AG23" s="15"/>
       <c r="AH23" s="15"/>
       <c r="AI23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AJ23" s="15"/>
       <c r="AK23" s="15"/>
       <c r="AL23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AM23" s="15"/>
       <c r="AN23" s="15"/>
@@ -4781,7 +4784,7 @@
       <c r="AP23" s="15"/>
       <c r="AQ23" s="15"/>
       <c r="AR23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AS23" s="15"/>
       <c r="AT23" s="15"/>
@@ -4789,7 +4792,7 @@
       <c r="AV23" s="15"/>
       <c r="AW23" s="15"/>
       <c r="AX23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AY23" s="15"/>
       <c r="AZ23" s="15"/>
@@ -4797,7 +4800,7 @@
       <c r="BB23" s="15"/>
       <c r="BC23" s="15"/>
       <c r="BD23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BE23" s="15"/>
       <c r="BF23" s="15"/>
@@ -4805,42 +4808,42 @@
       <c r="BH23" s="15"/>
       <c r="BI23" s="15"/>
       <c r="BJ23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BK23" s="15"/>
       <c r="BL23" s="15"/>
       <c r="BM23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BN23" s="15"/>
       <c r="BO23" s="15"/>
       <c r="BP23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BQ23" s="15"/>
       <c r="BR23" s="15"/>
       <c r="BS23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BT23" s="15"/>
       <c r="BU23" s="15"/>
       <c r="BV23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BW23" s="15"/>
       <c r="BX23" s="15"/>
       <c r="BY23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BZ23" s="15"/>
       <c r="CA23" s="15"/>
       <c r="CB23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="CC23" s="15"/>
       <c r="CD23" s="15"/>
       <c r="CE23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="CF23" s="10"/>
       <c r="CG23" s="10"/>
@@ -4850,7 +4853,7 @@
         <v>172</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C24" s="15">
         <v>5</v>
@@ -4945,7 +4948,7 @@
         <v>172</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -5036,7 +5039,7 @@
         <v>172</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>174</v>
+        <v>222</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -5126,190 +5129,190 @@
       <c r="CF26" s="10"/>
       <c r="CG26" s="10"/>
     </row>
-    <row r="27" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="6"/>
-      <c r="X27" s="5"/>
-      <c r="Y27" s="5"/>
-      <c r="Z27" s="6"/>
-      <c r="AA27" s="5"/>
-      <c r="AB27" s="5"/>
-      <c r="AC27" s="6"/>
-      <c r="AD27" s="5"/>
-      <c r="AE27" s="5"/>
-      <c r="AF27" s="7"/>
-      <c r="AG27" s="5"/>
-      <c r="AH27" s="5"/>
-      <c r="AI27" s="5"/>
-      <c r="AJ27" s="5"/>
-      <c r="AK27" s="5"/>
-      <c r="AL27" s="8"/>
-      <c r="AM27" s="5"/>
-      <c r="AN27" s="5"/>
-      <c r="AO27" s="5"/>
-      <c r="AP27" s="5"/>
-      <c r="AQ27" s="5"/>
-      <c r="AR27" s="8"/>
-      <c r="AS27" s="5"/>
-      <c r="AT27" s="5"/>
-      <c r="AU27" s="5"/>
-      <c r="AV27" s="5"/>
-      <c r="AW27" s="5"/>
-      <c r="AX27" s="9"/>
-      <c r="AY27" s="5"/>
-      <c r="AZ27" s="5"/>
-      <c r="BA27" s="5"/>
-      <c r="BB27" s="5"/>
-      <c r="BC27" s="5"/>
-      <c r="BD27" s="9"/>
-      <c r="BE27" s="5"/>
-      <c r="BF27" s="5"/>
-      <c r="BG27" s="5"/>
-      <c r="BH27" s="5"/>
-      <c r="BI27" s="5"/>
-      <c r="BJ27" s="6"/>
-      <c r="BK27" s="5"/>
-      <c r="BL27" s="5"/>
-      <c r="BM27" s="6"/>
-      <c r="BN27" s="5"/>
-      <c r="BO27" s="5"/>
-      <c r="BP27" s="6"/>
-      <c r="BQ27" s="5"/>
-      <c r="BR27" s="5"/>
-      <c r="BS27" s="6"/>
-      <c r="BT27" s="5"/>
-      <c r="BU27" s="5"/>
-      <c r="BV27" s="6"/>
-      <c r="BW27" s="5"/>
-      <c r="BX27" s="5"/>
-      <c r="BY27" s="6"/>
-      <c r="BZ27" s="5"/>
-      <c r="CA27" s="5"/>
-      <c r="CB27" s="6"/>
-      <c r="CC27" s="5"/>
-      <c r="CD27" s="5"/>
-      <c r="CE27" s="6"/>
-      <c r="CF27" s="5"/>
-      <c r="CG27" s="5"/>
-    </row>
-    <row r="28" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
-      <c r="T28" s="10"/>
-      <c r="U28" s="10"/>
-      <c r="V28" s="10"/>
-      <c r="W28" s="10"/>
-      <c r="X28" s="10"/>
-      <c r="Y28" s="10"/>
-      <c r="Z28" s="10"/>
-      <c r="AA28" s="10"/>
-      <c r="AB28" s="10"/>
-      <c r="AC28" s="10"/>
-      <c r="AD28" s="10"/>
-      <c r="AE28" s="10"/>
-      <c r="AF28" s="10"/>
-      <c r="AG28" s="10"/>
-      <c r="AH28" s="10"/>
-      <c r="AI28" s="10"/>
-      <c r="AJ28" s="10"/>
-      <c r="AK28" s="10"/>
-      <c r="AL28" s="10"/>
-      <c r="AM28" s="10"/>
-      <c r="AN28" s="10"/>
-      <c r="AO28" s="10"/>
-      <c r="AP28" s="10"/>
-      <c r="AQ28" s="10"/>
-      <c r="AR28" s="10"/>
-      <c r="AS28" s="10"/>
-      <c r="AT28" s="10"/>
-      <c r="AU28" s="10"/>
-      <c r="AV28" s="10"/>
-      <c r="AW28" s="10"/>
-      <c r="AX28" s="10"/>
-      <c r="AY28" s="10"/>
-      <c r="AZ28" s="10"/>
-      <c r="BA28" s="10"/>
-      <c r="BB28" s="10"/>
-      <c r="BC28" s="10"/>
-      <c r="BD28" s="10"/>
-      <c r="BE28" s="10"/>
-      <c r="BF28" s="10"/>
-      <c r="BG28" s="10"/>
-      <c r="BH28" s="10"/>
-      <c r="BI28" s="10"/>
-      <c r="BJ28" s="10"/>
-      <c r="BK28" s="10"/>
-      <c r="BL28" s="10"/>
-      <c r="BM28" s="10"/>
-      <c r="BN28" s="10"/>
-      <c r="BO28" s="10"/>
-      <c r="BP28" s="10"/>
-      <c r="BQ28" s="10"/>
-      <c r="BR28" s="10"/>
-      <c r="BS28" s="10"/>
-      <c r="BT28" s="10"/>
-      <c r="BU28" s="10"/>
-      <c r="BV28" s="10"/>
-      <c r="BW28" s="10"/>
-      <c r="BX28" s="10"/>
-      <c r="BY28" s="10"/>
-      <c r="BZ28" s="10"/>
-      <c r="CA28" s="10"/>
-      <c r="CB28" s="10"/>
-      <c r="CC28" s="10"/>
-      <c r="CD28" s="10"/>
-      <c r="CE28" s="10"/>
-      <c r="CF28" s="10"/>
-      <c r="CG28" s="10"/>
+    <row r="27" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="15"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="15"/>
+      <c r="AA27" s="15"/>
+      <c r="AB27" s="15"/>
+      <c r="AC27" s="15"/>
+      <c r="AD27" s="15"/>
+      <c r="AE27" s="15"/>
+      <c r="AF27" s="15"/>
+      <c r="AG27" s="15"/>
+      <c r="AH27" s="15"/>
+      <c r="AI27" s="15"/>
+      <c r="AJ27" s="15"/>
+      <c r="AK27" s="15"/>
+      <c r="AL27" s="15"/>
+      <c r="AM27" s="15"/>
+      <c r="AN27" s="15"/>
+      <c r="AO27" s="15"/>
+      <c r="AP27" s="15"/>
+      <c r="AQ27" s="15"/>
+      <c r="AR27" s="15"/>
+      <c r="AS27" s="15"/>
+      <c r="AT27" s="15"/>
+      <c r="AU27" s="15"/>
+      <c r="AV27" s="15"/>
+      <c r="AW27" s="15"/>
+      <c r="AX27" s="15"/>
+      <c r="AY27" s="15"/>
+      <c r="AZ27" s="15"/>
+      <c r="BA27" s="15"/>
+      <c r="BB27" s="15"/>
+      <c r="BC27" s="15"/>
+      <c r="BD27" s="15"/>
+      <c r="BE27" s="15"/>
+      <c r="BF27" s="15"/>
+      <c r="BG27" s="15"/>
+      <c r="BH27" s="15"/>
+      <c r="BI27" s="15"/>
+      <c r="BJ27" s="15"/>
+      <c r="BK27" s="15"/>
+      <c r="BL27" s="15"/>
+      <c r="BM27" s="15"/>
+      <c r="BN27" s="15"/>
+      <c r="BO27" s="15"/>
+      <c r="BP27" s="15"/>
+      <c r="BQ27" s="15"/>
+      <c r="BR27" s="15"/>
+      <c r="BS27" s="15"/>
+      <c r="BT27" s="15"/>
+      <c r="BU27" s="15"/>
+      <c r="BV27" s="15"/>
+      <c r="BW27" s="15"/>
+      <c r="BX27" s="15"/>
+      <c r="BY27" s="15"/>
+      <c r="BZ27" s="15"/>
+      <c r="CA27" s="15"/>
+      <c r="CB27" s="15"/>
+      <c r="CC27" s="15"/>
+      <c r="CD27" s="15"/>
+      <c r="CE27" s="15"/>
+      <c r="CF27" s="10"/>
+      <c r="CG27" s="10"/>
+    </row>
+    <row r="28" spans="1:85" x14ac:dyDescent="0.2">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="6"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="7"/>
+      <c r="AG28" s="5"/>
+      <c r="AH28" s="5"/>
+      <c r="AI28" s="5"/>
+      <c r="AJ28" s="5"/>
+      <c r="AK28" s="5"/>
+      <c r="AL28" s="8"/>
+      <c r="AM28" s="5"/>
+      <c r="AN28" s="5"/>
+      <c r="AO28" s="5"/>
+      <c r="AP28" s="5"/>
+      <c r="AQ28" s="5"/>
+      <c r="AR28" s="8"/>
+      <c r="AS28" s="5"/>
+      <c r="AT28" s="5"/>
+      <c r="AU28" s="5"/>
+      <c r="AV28" s="5"/>
+      <c r="AW28" s="5"/>
+      <c r="AX28" s="9"/>
+      <c r="AY28" s="5"/>
+      <c r="AZ28" s="5"/>
+      <c r="BA28" s="5"/>
+      <c r="BB28" s="5"/>
+      <c r="BC28" s="5"/>
+      <c r="BD28" s="9"/>
+      <c r="BE28" s="5"/>
+      <c r="BF28" s="5"/>
+      <c r="BG28" s="5"/>
+      <c r="BH28" s="5"/>
+      <c r="BI28" s="5"/>
+      <c r="BJ28" s="6"/>
+      <c r="BK28" s="5"/>
+      <c r="BL28" s="5"/>
+      <c r="BM28" s="6"/>
+      <c r="BN28" s="5"/>
+      <c r="BO28" s="5"/>
+      <c r="BP28" s="6"/>
+      <c r="BQ28" s="5"/>
+      <c r="BR28" s="5"/>
+      <c r="BS28" s="6"/>
+      <c r="BT28" s="5"/>
+      <c r="BU28" s="5"/>
+      <c r="BV28" s="6"/>
+      <c r="BW28" s="5"/>
+      <c r="BX28" s="5"/>
+      <c r="BY28" s="6"/>
+      <c r="BZ28" s="5"/>
+      <c r="CA28" s="5"/>
+      <c r="CB28" s="6"/>
+      <c r="CC28" s="5"/>
+      <c r="CD28" s="5"/>
+      <c r="CE28" s="6"/>
+      <c r="CF28" s="5"/>
+      <c r="CG28" s="5"/>
     </row>
     <row r="29" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>221</v>
+        <v>173</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -5397,10 +5400,10 @@
     </row>
     <row r="30" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -5488,10 +5491,10 @@
     </row>
     <row r="31" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -5579,10 +5582,10 @@
     </row>
     <row r="32" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -5668,254 +5671,282 @@
       <c r="CF32" s="10"/>
       <c r="CG32" s="10"/>
     </row>
-    <row r="33" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="6"/>
-      <c r="U33" s="5"/>
-      <c r="V33" s="5"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="5"/>
-      <c r="Y33" s="5"/>
-      <c r="Z33" s="6"/>
-      <c r="AA33" s="5"/>
-      <c r="AB33" s="5"/>
-      <c r="AC33" s="6"/>
-      <c r="AD33" s="5"/>
-      <c r="AE33" s="5"/>
-      <c r="AF33" s="7"/>
-      <c r="AG33" s="5"/>
-      <c r="AH33" s="5"/>
-      <c r="AI33" s="5"/>
-      <c r="AJ33" s="5"/>
-      <c r="AK33" s="5"/>
-      <c r="AL33" s="8"/>
-      <c r="AM33" s="5"/>
-      <c r="AN33" s="5"/>
-      <c r="AO33" s="5"/>
-      <c r="AP33" s="5"/>
-      <c r="AQ33" s="5"/>
-      <c r="AR33" s="8"/>
-      <c r="AS33" s="5"/>
-      <c r="AT33" s="5"/>
-      <c r="AU33" s="5"/>
-      <c r="AV33" s="5"/>
-      <c r="AW33" s="5"/>
-      <c r="AX33" s="9"/>
-      <c r="AY33" s="5"/>
-      <c r="AZ33" s="5"/>
-      <c r="BA33" s="5"/>
-      <c r="BB33" s="5"/>
-      <c r="BC33" s="5"/>
-      <c r="BD33" s="9"/>
-      <c r="BE33" s="5"/>
-      <c r="BF33" s="5"/>
-      <c r="BG33" s="5"/>
-      <c r="BH33" s="5"/>
-      <c r="BI33" s="5"/>
-      <c r="BJ33" s="6"/>
-      <c r="BK33" s="5"/>
-      <c r="BL33" s="5"/>
-      <c r="BM33" s="6"/>
-      <c r="BN33" s="5"/>
-      <c r="BO33" s="5"/>
-      <c r="BP33" s="6"/>
-      <c r="BQ33" s="5"/>
-      <c r="BR33" s="5"/>
-      <c r="BS33" s="6"/>
-      <c r="BT33" s="5"/>
-      <c r="BU33" s="5"/>
-      <c r="BV33" s="6"/>
-      <c r="BW33" s="5"/>
-      <c r="BX33" s="5"/>
-      <c r="BY33" s="6"/>
-      <c r="BZ33" s="5"/>
-      <c r="CA33" s="5"/>
-      <c r="CB33" s="6"/>
-      <c r="CC33" s="5"/>
-      <c r="CD33" s="5"/>
-      <c r="CE33" s="6"/>
-      <c r="CF33" s="5"/>
-      <c r="CG33" s="5"/>
+    <row r="33" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
+      <c r="W33" s="10"/>
+      <c r="X33" s="10"/>
+      <c r="Y33" s="10"/>
+      <c r="Z33" s="10"/>
+      <c r="AA33" s="10"/>
+      <c r="AB33" s="10"/>
+      <c r="AC33" s="10"/>
+      <c r="AD33" s="10"/>
+      <c r="AE33" s="10"/>
+      <c r="AF33" s="10"/>
+      <c r="AG33" s="10"/>
+      <c r="AH33" s="10"/>
+      <c r="AI33" s="10"/>
+      <c r="AJ33" s="10"/>
+      <c r="AK33" s="10"/>
+      <c r="AL33" s="10"/>
+      <c r="AM33" s="10"/>
+      <c r="AN33" s="10"/>
+      <c r="AO33" s="10"/>
+      <c r="AP33" s="10"/>
+      <c r="AQ33" s="10"/>
+      <c r="AR33" s="10"/>
+      <c r="AS33" s="10"/>
+      <c r="AT33" s="10"/>
+      <c r="AU33" s="10"/>
+      <c r="AV33" s="10"/>
+      <c r="AW33" s="10"/>
+      <c r="AX33" s="10"/>
+      <c r="AY33" s="10"/>
+      <c r="AZ33" s="10"/>
+      <c r="BA33" s="10"/>
+      <c r="BB33" s="10"/>
+      <c r="BC33" s="10"/>
+      <c r="BD33" s="10"/>
+      <c r="BE33" s="10"/>
+      <c r="BF33" s="10"/>
+      <c r="BG33" s="10"/>
+      <c r="BH33" s="10"/>
+      <c r="BI33" s="10"/>
+      <c r="BJ33" s="10"/>
+      <c r="BK33" s="10"/>
+      <c r="BL33" s="10"/>
+      <c r="BM33" s="10"/>
+      <c r="BN33" s="10"/>
+      <c r="BO33" s="10"/>
+      <c r="BP33" s="10"/>
+      <c r="BQ33" s="10"/>
+      <c r="BR33" s="10"/>
+      <c r="BS33" s="10"/>
+      <c r="BT33" s="10"/>
+      <c r="BU33" s="10"/>
+      <c r="BV33" s="10"/>
+      <c r="BW33" s="10"/>
+      <c r="BX33" s="10"/>
+      <c r="BY33" s="10"/>
+      <c r="BZ33" s="10"/>
+      <c r="CA33" s="10"/>
+      <c r="CB33" s="10"/>
+      <c r="CC33" s="10"/>
+      <c r="CD33" s="10"/>
+      <c r="CE33" s="10"/>
+      <c r="CF33" s="10"/>
+      <c r="CG33" s="10"/>
     </row>
     <row r="34" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="29"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="30"/>
-      <c r="S34" s="30"/>
-      <c r="T34" s="30"/>
-      <c r="U34" s="30"/>
-      <c r="V34" s="30"/>
-      <c r="W34" s="30"/>
-      <c r="Z34" s="30"/>
-      <c r="AA34" s="30"/>
-      <c r="AB34" s="30"/>
-      <c r="AC34" s="30"/>
-      <c r="AD34" s="30"/>
-      <c r="AE34" s="30"/>
-      <c r="AF34" s="30"/>
-      <c r="AG34" s="30"/>
-      <c r="AH34" s="30"/>
-      <c r="AI34" s="30"/>
-      <c r="AJ34" s="30"/>
-      <c r="AK34" s="30"/>
-      <c r="AL34" s="30"/>
-      <c r="AM34" s="30"/>
-      <c r="AN34" s="30"/>
-      <c r="AO34" s="30"/>
-      <c r="AP34" s="30"/>
-      <c r="AQ34" s="30"/>
-      <c r="AR34" s="30"/>
-      <c r="AS34" s="30"/>
-      <c r="AT34" s="30"/>
-      <c r="AU34" s="30"/>
-      <c r="AV34" s="30"/>
-      <c r="AW34" s="30"/>
-      <c r="AX34" s="30"/>
-      <c r="AY34" s="30"/>
-      <c r="AZ34" s="30"/>
-      <c r="BA34" s="30"/>
-      <c r="BB34" s="30"/>
-      <c r="BC34" s="30"/>
-      <c r="BD34" s="30"/>
-      <c r="BE34" s="30"/>
-      <c r="BF34" s="30"/>
-      <c r="BG34" s="30"/>
-      <c r="BH34" s="30"/>
-      <c r="BI34" s="30"/>
-      <c r="BJ34" s="30"/>
-      <c r="BK34" s="30"/>
-      <c r="BL34" s="30"/>
-      <c r="BM34" s="30"/>
-      <c r="BN34" s="30"/>
-      <c r="BO34" s="30"/>
-      <c r="BP34" s="30"/>
-      <c r="BQ34" s="30"/>
-      <c r="BR34" s="30"/>
-      <c r="BS34" s="30"/>
-      <c r="BT34" s="30"/>
-      <c r="BU34" s="30"/>
-      <c r="BV34" s="30"/>
-      <c r="BW34" s="30"/>
-      <c r="BX34" s="30"/>
-      <c r="BY34" s="30"/>
-      <c r="BZ34" s="30"/>
-      <c r="CA34" s="30"/>
-      <c r="CB34" s="30"/>
-      <c r="CC34" s="30"/>
-      <c r="CD34" s="30"/>
-      <c r="CE34" s="30"/>
-    </row>
-    <row r="35" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="29"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="H35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="30"/>
-      <c r="O35" s="30"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="30"/>
-      <c r="S35" s="30"/>
-      <c r="T35" s="30"/>
-      <c r="U35" s="30"/>
-      <c r="V35" s="30"/>
-      <c r="W35" s="30"/>
-      <c r="Z35" s="30"/>
-      <c r="AA35" s="30"/>
-      <c r="AB35" s="30"/>
-      <c r="AC35" s="30"/>
-      <c r="AD35" s="30"/>
-      <c r="AE35" s="30"/>
-      <c r="AF35" s="30"/>
-      <c r="AG35" s="30"/>
-      <c r="AH35" s="30"/>
-      <c r="AI35" s="30"/>
-      <c r="AJ35" s="30"/>
-      <c r="AK35" s="30"/>
-      <c r="AL35" s="30"/>
-      <c r="AM35" s="30"/>
-      <c r="AN35" s="30"/>
-      <c r="AO35" s="30"/>
-      <c r="AP35" s="30"/>
-      <c r="AQ35" s="30"/>
-      <c r="AR35" s="30"/>
-      <c r="AS35" s="30"/>
-      <c r="AT35" s="30"/>
-      <c r="AU35" s="30"/>
-      <c r="AV35" s="30"/>
-      <c r="AW35" s="30"/>
-      <c r="AX35" s="30"/>
-      <c r="AY35" s="30"/>
-      <c r="AZ35" s="30"/>
-      <c r="BA35" s="30"/>
-      <c r="BB35" s="30"/>
-      <c r="BC35" s="30"/>
-      <c r="BD35" s="30"/>
-      <c r="BE35" s="30"/>
-      <c r="BF35" s="30"/>
-      <c r="BG35" s="30"/>
-      <c r="BH35" s="30"/>
-      <c r="BI35" s="30"/>
-      <c r="BJ35" s="30"/>
-      <c r="BK35" s="30"/>
-      <c r="BL35" s="30"/>
-      <c r="BM35" s="30"/>
-      <c r="BN35" s="30"/>
-      <c r="BO35" s="30"/>
-      <c r="BP35" s="30"/>
-      <c r="BQ35" s="30"/>
-      <c r="BR35" s="30"/>
-      <c r="BS35" s="30"/>
-      <c r="BT35" s="30"/>
-      <c r="BU35" s="30"/>
-      <c r="BV35" s="30"/>
-      <c r="BW35" s="30"/>
-      <c r="BX35" s="30"/>
-      <c r="BY35" s="30"/>
-      <c r="BZ35" s="30"/>
-      <c r="CA35" s="30"/>
-      <c r="CB35" s="30"/>
-      <c r="CC35" s="30"/>
-      <c r="CD35" s="30"/>
-      <c r="CE35" s="30"/>
+      <c r="A34" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+      <c r="Y34" s="10"/>
+      <c r="Z34" s="10"/>
+      <c r="AA34" s="10"/>
+      <c r="AB34" s="10"/>
+      <c r="AC34" s="10"/>
+      <c r="AD34" s="10"/>
+      <c r="AE34" s="10"/>
+      <c r="AF34" s="10"/>
+      <c r="AG34" s="10"/>
+      <c r="AH34" s="10"/>
+      <c r="AI34" s="10"/>
+      <c r="AJ34" s="10"/>
+      <c r="AK34" s="10"/>
+      <c r="AL34" s="10"/>
+      <c r="AM34" s="10"/>
+      <c r="AN34" s="10"/>
+      <c r="AO34" s="10"/>
+      <c r="AP34" s="10"/>
+      <c r="AQ34" s="10"/>
+      <c r="AR34" s="10"/>
+      <c r="AS34" s="10"/>
+      <c r="AT34" s="10"/>
+      <c r="AU34" s="10"/>
+      <c r="AV34" s="10"/>
+      <c r="AW34" s="10"/>
+      <c r="AX34" s="10"/>
+      <c r="AY34" s="10"/>
+      <c r="AZ34" s="10"/>
+      <c r="BA34" s="10"/>
+      <c r="BB34" s="10"/>
+      <c r="BC34" s="10"/>
+      <c r="BD34" s="10"/>
+      <c r="BE34" s="10"/>
+      <c r="BF34" s="10"/>
+      <c r="BG34" s="10"/>
+      <c r="BH34" s="10"/>
+      <c r="BI34" s="10"/>
+      <c r="BJ34" s="10"/>
+      <c r="BK34" s="10"/>
+      <c r="BL34" s="10"/>
+      <c r="BM34" s="10"/>
+      <c r="BN34" s="10"/>
+      <c r="BO34" s="10"/>
+      <c r="BP34" s="10"/>
+      <c r="BQ34" s="10"/>
+      <c r="BR34" s="10"/>
+      <c r="BS34" s="10"/>
+      <c r="BT34" s="10"/>
+      <c r="BU34" s="10"/>
+      <c r="BV34" s="10"/>
+      <c r="BW34" s="10"/>
+      <c r="BX34" s="10"/>
+      <c r="BY34" s="10"/>
+      <c r="BZ34" s="10"/>
+      <c r="CA34" s="10"/>
+      <c r="CB34" s="10"/>
+      <c r="CC34" s="10"/>
+      <c r="CD34" s="10"/>
+      <c r="CE34" s="10"/>
+      <c r="CF34" s="10"/>
+      <c r="CG34" s="10"/>
+    </row>
+    <row r="35" spans="1:85" x14ac:dyDescent="0.2">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="6"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="6"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="6"/>
+      <c r="AA35" s="5"/>
+      <c r="AB35" s="5"/>
+      <c r="AC35" s="6"/>
+      <c r="AD35" s="5"/>
+      <c r="AE35" s="5"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="5"/>
+      <c r="AH35" s="5"/>
+      <c r="AI35" s="5"/>
+      <c r="AJ35" s="5"/>
+      <c r="AK35" s="5"/>
+      <c r="AL35" s="8"/>
+      <c r="AM35" s="5"/>
+      <c r="AN35" s="5"/>
+      <c r="AO35" s="5"/>
+      <c r="AP35" s="5"/>
+      <c r="AQ35" s="5"/>
+      <c r="AR35" s="8"/>
+      <c r="AS35" s="5"/>
+      <c r="AT35" s="5"/>
+      <c r="AU35" s="5"/>
+      <c r="AV35" s="5"/>
+      <c r="AW35" s="5"/>
+      <c r="AX35" s="9"/>
+      <c r="AY35" s="5"/>
+      <c r="AZ35" s="5"/>
+      <c r="BA35" s="5"/>
+      <c r="BB35" s="5"/>
+      <c r="BC35" s="5"/>
+      <c r="BD35" s="9"/>
+      <c r="BE35" s="5"/>
+      <c r="BF35" s="5"/>
+      <c r="BG35" s="5"/>
+      <c r="BH35" s="5"/>
+      <c r="BI35" s="5"/>
+      <c r="BJ35" s="6"/>
+      <c r="BK35" s="5"/>
+      <c r="BL35" s="5"/>
+      <c r="BM35" s="6"/>
+      <c r="BN35" s="5"/>
+      <c r="BO35" s="5"/>
+      <c r="BP35" s="6"/>
+      <c r="BQ35" s="5"/>
+      <c r="BR35" s="5"/>
+      <c r="BS35" s="6"/>
+      <c r="BT35" s="5"/>
+      <c r="BU35" s="5"/>
+      <c r="BV35" s="6"/>
+      <c r="BW35" s="5"/>
+      <c r="BX35" s="5"/>
+      <c r="BY35" s="6"/>
+      <c r="BZ35" s="5"/>
+      <c r="CA35" s="5"/>
+      <c r="CB35" s="6"/>
+      <c r="CC35" s="5"/>
+      <c r="CD35" s="5"/>
+      <c r="CE35" s="6"/>
+      <c r="CF35" s="5"/>
+      <c r="CG35" s="5"/>
     </row>
     <row r="36" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="29"/>
       <c r="C36" s="28"/>
       <c r="D36" s="28"/>
       <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
       <c r="K36" s="30"/>
       <c r="L36" s="30"/>
       <c r="M36" s="30"/>
@@ -5993,8 +6024,6 @@
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
       <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
       <c r="K37" s="30"/>
       <c r="L37" s="30"/>
       <c r="M37" s="30"/>
@@ -6067,20 +6096,168 @@
       <c r="CD37" s="30"/>
       <c r="CE37" s="30"/>
     </row>
-    <row r="40" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M40" s="30"/>
-      <c r="BF40" s="28"/>
-    </row>
-    <row r="41" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M41" s="15"/>
-    </row>
-    <row r="44" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="28"/>
-      <c r="C44" s="25"/>
-    </row>
-    <row r="45" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="28"/>
-      <c r="C45" s="25"/>
+    <row r="38" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="29"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="H38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
+      <c r="M38" s="30"/>
+      <c r="N38" s="30"/>
+      <c r="O38" s="30"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="30"/>
+      <c r="S38" s="30"/>
+      <c r="T38" s="30"/>
+      <c r="U38" s="30"/>
+      <c r="V38" s="30"/>
+      <c r="W38" s="30"/>
+      <c r="Z38" s="30"/>
+      <c r="AA38" s="30"/>
+      <c r="AB38" s="30"/>
+      <c r="AC38" s="30"/>
+      <c r="AD38" s="30"/>
+      <c r="AE38" s="30"/>
+      <c r="AF38" s="30"/>
+      <c r="AG38" s="30"/>
+      <c r="AH38" s="30"/>
+      <c r="AI38" s="30"/>
+      <c r="AJ38" s="30"/>
+      <c r="AK38" s="30"/>
+      <c r="AL38" s="30"/>
+      <c r="AM38" s="30"/>
+      <c r="AN38" s="30"/>
+      <c r="AO38" s="30"/>
+      <c r="AP38" s="30"/>
+      <c r="AQ38" s="30"/>
+      <c r="AR38" s="30"/>
+      <c r="AS38" s="30"/>
+      <c r="AT38" s="30"/>
+      <c r="AU38" s="30"/>
+      <c r="AV38" s="30"/>
+      <c r="AW38" s="30"/>
+      <c r="AX38" s="30"/>
+      <c r="AY38" s="30"/>
+      <c r="AZ38" s="30"/>
+      <c r="BA38" s="30"/>
+      <c r="BB38" s="30"/>
+      <c r="BC38" s="30"/>
+      <c r="BD38" s="30"/>
+      <c r="BE38" s="30"/>
+      <c r="BF38" s="30"/>
+      <c r="BG38" s="30"/>
+      <c r="BH38" s="30"/>
+      <c r="BI38" s="30"/>
+      <c r="BJ38" s="30"/>
+      <c r="BK38" s="30"/>
+      <c r="BL38" s="30"/>
+      <c r="BM38" s="30"/>
+      <c r="BN38" s="30"/>
+      <c r="BO38" s="30"/>
+      <c r="BP38" s="30"/>
+      <c r="BQ38" s="30"/>
+      <c r="BR38" s="30"/>
+      <c r="BS38" s="30"/>
+      <c r="BT38" s="30"/>
+      <c r="BU38" s="30"/>
+      <c r="BV38" s="30"/>
+      <c r="BW38" s="30"/>
+      <c r="BX38" s="30"/>
+      <c r="BY38" s="30"/>
+      <c r="BZ38" s="30"/>
+      <c r="CA38" s="30"/>
+      <c r="CB38" s="30"/>
+      <c r="CC38" s="30"/>
+      <c r="CD38" s="30"/>
+      <c r="CE38" s="30"/>
+    </row>
+    <row r="39" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="29"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="30"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="30"/>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="30"/>
+      <c r="S39" s="30"/>
+      <c r="T39" s="30"/>
+      <c r="U39" s="30"/>
+      <c r="V39" s="30"/>
+      <c r="W39" s="30"/>
+      <c r="Z39" s="30"/>
+      <c r="AA39" s="30"/>
+      <c r="AB39" s="30"/>
+      <c r="AC39" s="30"/>
+      <c r="AD39" s="30"/>
+      <c r="AE39" s="30"/>
+      <c r="AF39" s="30"/>
+      <c r="AG39" s="30"/>
+      <c r="AH39" s="30"/>
+      <c r="AI39" s="30"/>
+      <c r="AJ39" s="30"/>
+      <c r="AK39" s="30"/>
+      <c r="AL39" s="30"/>
+      <c r="AM39" s="30"/>
+      <c r="AN39" s="30"/>
+      <c r="AO39" s="30"/>
+      <c r="AP39" s="30"/>
+      <c r="AQ39" s="30"/>
+      <c r="AR39" s="30"/>
+      <c r="AS39" s="30"/>
+      <c r="AT39" s="30"/>
+      <c r="AU39" s="30"/>
+      <c r="AV39" s="30"/>
+      <c r="AW39" s="30"/>
+      <c r="AX39" s="30"/>
+      <c r="AY39" s="30"/>
+      <c r="AZ39" s="30"/>
+      <c r="BA39" s="30"/>
+      <c r="BB39" s="30"/>
+      <c r="BC39" s="30"/>
+      <c r="BD39" s="30"/>
+      <c r="BE39" s="30"/>
+      <c r="BF39" s="30"/>
+      <c r="BG39" s="30"/>
+      <c r="BH39" s="30"/>
+      <c r="BI39" s="30"/>
+      <c r="BJ39" s="30"/>
+      <c r="BK39" s="30"/>
+      <c r="BL39" s="30"/>
+      <c r="BM39" s="30"/>
+      <c r="BN39" s="30"/>
+      <c r="BO39" s="30"/>
+      <c r="BP39" s="30"/>
+      <c r="BQ39" s="30"/>
+      <c r="BR39" s="30"/>
+      <c r="BS39" s="30"/>
+      <c r="BT39" s="30"/>
+      <c r="BU39" s="30"/>
+      <c r="BV39" s="30"/>
+      <c r="BW39" s="30"/>
+      <c r="BX39" s="30"/>
+      <c r="BY39" s="30"/>
+      <c r="BZ39" s="30"/>
+      <c r="CA39" s="30"/>
+      <c r="CB39" s="30"/>
+      <c r="CC39" s="30"/>
+      <c r="CD39" s="30"/>
+      <c r="CE39" s="30"/>
+    </row>
+    <row r="42" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M42" s="30"/>
+      <c r="BF42" s="28"/>
+    </row>
+    <row r="43" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M43" s="15"/>
     </row>
     <row r="46" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="28"/>
@@ -6088,11 +6265,11 @@
     </row>
     <row r="47" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="28"/>
-      <c r="C47" s="26"/>
+      <c r="C47" s="25"/>
     </row>
     <row r="48" spans="1:85" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="28"/>
-      <c r="C48" s="26"/>
+      <c r="C48" s="25"/>
     </row>
     <row r="49" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="28"/>
@@ -6104,7 +6281,7 @@
     </row>
     <row r="51" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="28"/>
-      <c r="C51" s="27"/>
+      <c r="C51" s="26"/>
     </row>
     <row r="52" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="28"/>
@@ -6112,7 +6289,7 @@
     </row>
     <row r="53" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="28"/>
-      <c r="C53" s="26"/>
+      <c r="C53" s="27"/>
     </row>
     <row r="54" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="28"/>
@@ -6128,11 +6305,11 @@
     </row>
     <row r="57" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="28"/>
-      <c r="C57" s="27"/>
+      <c r="C57" s="26"/>
     </row>
     <row r="58" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="28"/>
-      <c r="C58" s="27"/>
+      <c r="C58" s="26"/>
     </row>
     <row r="59" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="28"/>
@@ -6178,61 +6355,69 @@
       <c r="B69" s="28"/>
       <c r="C69" s="27"/>
     </row>
-    <row r="72" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="26"/>
-      <c r="F72" s="26"/>
-      <c r="G72" s="26"/>
-      <c r="H72" s="26"/>
-      <c r="I72" s="27"/>
-      <c r="J72" s="26"/>
-      <c r="K72" s="26"/>
-      <c r="L72" s="26"/>
-      <c r="M72" s="26"/>
-      <c r="N72" s="26"/>
-      <c r="O72" s="27"/>
-      <c r="P72" s="27"/>
-      <c r="Q72" s="27"/>
-      <c r="R72" s="27"/>
-      <c r="S72" s="27"/>
-      <c r="T72" s="27"/>
-      <c r="U72" s="27"/>
-      <c r="V72" s="27"/>
-      <c r="W72" s="27"/>
-      <c r="X72" s="27"/>
-      <c r="Y72" s="27"/>
-      <c r="Z72" s="27"/>
-      <c r="AA72" s="27"/>
-    </row>
-    <row r="73" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="28"/>
-      <c r="C73" s="28"/>
-      <c r="D73" s="28"/>
-      <c r="E73" s="28"/>
-      <c r="F73" s="28"/>
-      <c r="G73" s="28"/>
-      <c r="H73" s="28"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="28"/>
-      <c r="K73" s="28"/>
-      <c r="L73" s="28"/>
-      <c r="M73" s="28"/>
-      <c r="N73" s="28"/>
-      <c r="O73" s="28"/>
-      <c r="P73" s="28"/>
-      <c r="Q73" s="28"/>
-      <c r="R73" s="28"/>
-      <c r="S73" s="28"/>
-      <c r="T73" s="28"/>
-      <c r="U73" s="28"/>
-      <c r="V73" s="28"/>
-      <c r="W73" s="28"/>
-      <c r="X73" s="28"/>
-      <c r="Y73" s="28"/>
-      <c r="Z73" s="28"/>
-      <c r="AA73" s="28"/>
+    <row r="70" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="28"/>
+      <c r="C70" s="27"/>
+    </row>
+    <row r="71" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="28"/>
+      <c r="C71" s="27"/>
+    </row>
+    <row r="74" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="25"/>
+      <c r="C74" s="25"/>
+      <c r="D74" s="25"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="26"/>
+      <c r="G74" s="26"/>
+      <c r="H74" s="26"/>
+      <c r="I74" s="27"/>
+      <c r="J74" s="26"/>
+      <c r="K74" s="26"/>
+      <c r="L74" s="26"/>
+      <c r="M74" s="26"/>
+      <c r="N74" s="26"/>
+      <c r="O74" s="27"/>
+      <c r="P74" s="27"/>
+      <c r="Q74" s="27"/>
+      <c r="R74" s="27"/>
+      <c r="S74" s="27"/>
+      <c r="T74" s="27"/>
+      <c r="U74" s="27"/>
+      <c r="V74" s="27"/>
+      <c r="W74" s="27"/>
+      <c r="X74" s="27"/>
+      <c r="Y74" s="27"/>
+      <c r="Z74" s="27"/>
+      <c r="AA74" s="27"/>
+    </row>
+    <row r="75" spans="2:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="28"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="28"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="28"/>
+      <c r="I75" s="28"/>
+      <c r="J75" s="28"/>
+      <c r="K75" s="28"/>
+      <c r="L75" s="28"/>
+      <c r="M75" s="28"/>
+      <c r="N75" s="28"/>
+      <c r="O75" s="28"/>
+      <c r="P75" s="28"/>
+      <c r="Q75" s="28"/>
+      <c r="R75" s="28"/>
+      <c r="S75" s="28"/>
+      <c r="T75" s="28"/>
+      <c r="U75" s="28"/>
+      <c r="V75" s="28"/>
+      <c r="W75" s="28"/>
+      <c r="X75" s="28"/>
+      <c r="Y75" s="28"/>
+      <c r="Z75" s="28"/>
+      <c r="AA75" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
bug fix. sample storage / sample type
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants/1SPL01_plants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/1SPL01_plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CD3173-3707-A944-8B70-DA4ABD8861D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78C6747-973C-E649-B459-929C8ABEE4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4720" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="2" r:id="rId1"/>
@@ -1659,6 +1659,94 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
@@ -1705,7 +1793,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1722,6 +1809,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1730,7 +1818,397 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00\ &quot;percent&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00\ &quot;percent&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00\ &quot;microeinstein per square meter per second&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1747,6 +2225,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1755,7 +2234,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1772,6 +2250,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1780,7 +2259,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1797,6 +2275,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1805,7 +2284,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1822,489 +2300,11 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00\ &quot;percent&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00\ &quot;percent&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;microeinstein per square meter per second&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2714,93 +2714,93 @@
     <tableColumn id="126" xr3:uid="{D48EF60D-FFC4-DA42-8A84-9D7BEC94EB5C}" name="Characteristics [Developmental Stage]" dataDxfId="89"/>
     <tableColumn id="127" xr3:uid="{B7FB233D-7D8A-A34E-91AE-3E96612329F2}" name="Term Source REF [Developmental Stage] (#h; #tNFDI4PSO:0000070)" dataDxfId="88"/>
     <tableColumn id="128" xr3:uid="{0CFCFB6B-CC3F-A24A-B1A8-77F2863EAED6}" name="Term Accession Number [Developmental Stage] (#h; #tNFDI4PSO:0000070)" dataDxfId="87"/>
-    <tableColumn id="129" xr3:uid="{A1014B91-8574-664B-A628-2DDC01083E67}" name="Characteristics [Plant disease]" dataDxfId="18"/>
-    <tableColumn id="130" xr3:uid="{CF451DD4-AB45-1144-8BBF-C2C23EAE7EBC}" name="Term Source REF [Plant disease] (#h; #tNFDI4PSO:0000071)" dataDxfId="20"/>
-    <tableColumn id="131" xr3:uid="{4A90236E-F6AF-BE44-8703-08F06FE96AF5}" name="Term Accession Number [Plant disease] (#h; #tNFDI4PSO:0000071)" dataDxfId="19"/>
-    <tableColumn id="132" xr3:uid="{1F37D0D2-6260-584B-9CC0-9A72C472F841}" name="Characteristics [Plant disease stage]" dataDxfId="15"/>
-    <tableColumn id="133" xr3:uid="{2348DA4F-92E0-8547-AA7D-FCB641272A62}" name="Term Source REF [Plant disease stage] (#h; #tNFDI4PSO:0000072)" dataDxfId="17"/>
-    <tableColumn id="134" xr3:uid="{76B2929E-FEFA-C94A-9351-B07EA87DB902}" name="Term Accession Number [Plant disease stage] (#h; #tNFDI4PSO:0000072)" dataDxfId="16"/>
-    <tableColumn id="135" xr3:uid="{BEBD2093-9306-0C42-AFAE-735502002BE7}" name="Characteristics [Phenotype]" dataDxfId="12"/>
-    <tableColumn id="136" xr3:uid="{109579A2-3212-484D-A514-9571CF9305C5}" name="Term Source REF [Phenotype] (#h; #tNFDI4PSO:0000073)" dataDxfId="14"/>
-    <tableColumn id="137" xr3:uid="{77978229-5807-DE4F-A777-C5E343D79A55}" name="Term Accession Number [Phenotype] (#h; #tNFDI4PSO:0000073)" dataDxfId="13"/>
-    <tableColumn id="138" xr3:uid="{65D76AFE-F9A3-544C-B9C1-4D6C71488C92}" name="Characteristics [whole plant size]" dataDxfId="9"/>
-    <tableColumn id="139" xr3:uid="{91B73049-DC8D-D94B-8B5F-76E283D04557}" name="Term Source REF [whole plant size] (#h; #tTO:1000012)" dataDxfId="11"/>
-    <tableColumn id="140" xr3:uid="{6FB79EF4-9E54-8D45-BB9F-CE997665B054}" name="Term Accession Number [whole plant size] (#h; #tTO:1000012)" dataDxfId="10"/>
-    <tableColumn id="26" xr3:uid="{5E219BCA-059A-CC41-93BF-8CD61AA9572D}" name="Characteristics [study type]" dataDxfId="86"/>
-    <tableColumn id="27" xr3:uid="{5FF2BBBF-350F-9842-8FDF-2F895B07EADF}" name="Term Source REF [study type] (#h; #tPECO:0007231)" dataDxfId="85"/>
-    <tableColumn id="28" xr3:uid="{E12790EC-754D-3244-8A7A-1242F7942612}" name="Term Accession Number [study type] (#h; #tPECO:0007231)" dataDxfId="84"/>
-    <tableColumn id="23" xr3:uid="{E0A293FE-1EF5-A949-9C12-ADF40314B418}" name="Characteristics [plant growth medium exposure]" dataDxfId="83"/>
-    <tableColumn id="24" xr3:uid="{0C19F4A6-F9E8-1F4F-9B61-EB31E6DF451A}" name="Term Source REF [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="82"/>
-    <tableColumn id="25" xr3:uid="{7BBED07D-F814-A245-B090-723342B3D631}" name="Term Accession Number [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="81"/>
-    <tableColumn id="29" xr3:uid="{C386EF1A-F4F8-C543-99A0-ABD311BD175F}" name="Characteristics [growth plot design]" dataDxfId="80"/>
-    <tableColumn id="30" xr3:uid="{86FAE20B-4F89-EE4F-91E6-CE3B7E712F95}" name="Term Source REF [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="79"/>
-    <tableColumn id="31" xr3:uid="{C0949892-595C-9742-BCD1-75134FAC012F}" name="Term Accession Number [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="78"/>
-    <tableColumn id="32" xr3:uid="{B90A4652-69D5-2E4F-8A64-A3A5A5CB24DB}" name="Characteristics [Growth day length]" dataDxfId="77"/>
-    <tableColumn id="33" xr3:uid="{4E2448E1-3D08-504C-8FE3-D71B801F4DC9}" name="Term Source REF [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="76"/>
-    <tableColumn id="34" xr3:uid="{D47410BE-0000-B648-8CE5-966EE8968909}" name="Term Accession Number [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="75"/>
-    <tableColumn id="35" xr3:uid="{27034924-8879-044A-819B-7DC832A9D603}" name="Characteristics [light intensity exposure]" dataDxfId="74"/>
-    <tableColumn id="36" xr3:uid="{FD04748E-7F58-4A46-A167-E5EB1375A50B}" name="Term Source REF [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="73"/>
-    <tableColumn id="37" xr3:uid="{D76E6422-DF20-B94A-B5A6-4FD7F7923EBF}" name="Term Accession Number [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{8E446DD1-817A-E84A-9536-47B88B72BFD8}" name="Unit [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{BCB29467-6D87-F141-98A0-60243765731F}" name="Term Source REF [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="70"/>
-    <tableColumn id="8" xr3:uid="{D2565EAD-7C86-C343-800D-E37FD463093B}" name="Term Accession Number [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="69"/>
-    <tableColumn id="38" xr3:uid="{21746D48-E9A2-5B42-BC00-F5AFD4793AA7}" name="Characteristics [Humidity Day]" dataDxfId="68"/>
-    <tableColumn id="39" xr3:uid="{8B1D9CC4-6026-674C-9852-06A06365907B}" name="Term Source REF [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="67"/>
-    <tableColumn id="40" xr3:uid="{8CCA0026-8267-884E-8F9A-369ACCB825EA}" name="Term Accession Number [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="66"/>
-    <tableColumn id="9" xr3:uid="{9508FD23-5388-F64E-8286-05B533856CA2}" name="Unit [percent] (#h; #tUO:0000187; #u)" dataDxfId="65"/>
-    <tableColumn id="10" xr3:uid="{F796BC22-CBE1-6D41-824E-F655C3F9D5B6}" name="Term Source REF [percent] (#h; #tUO:0000187; #u)" dataDxfId="64"/>
-    <tableColumn id="11" xr3:uid="{32AC3DD8-82CD-4349-BFD5-0805A34144D8}" name="Term Accession Number [percent] (#h; #tUO:0000187; #u)" dataDxfId="63"/>
-    <tableColumn id="41" xr3:uid="{F4E42B79-6B62-E34C-95BE-8906E80BFBC8}" name="Characteristics [Humidity Night]" dataDxfId="62"/>
-    <tableColumn id="42" xr3:uid="{FE26FC08-E3D1-7547-8E20-1363EF47EE86}" name="Term Source REF [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="61"/>
-    <tableColumn id="43" xr3:uid="{C6D20AF0-60A8-874E-9614-2A2F483EB262}" name="Term Accession Number [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{2866C2CF-81B3-694E-B2D9-F69059F54AA2}" name="Unit [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="59"/>
-    <tableColumn id="13" xr3:uid="{A885FE47-7729-3B45-B73D-03FF1F114CD5}" name="Term Source REF [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="58"/>
-    <tableColumn id="65" xr3:uid="{A3AEBB25-5500-F249-866E-C98439259F17}" name="Term Accession Number [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="57"/>
-    <tableColumn id="44" xr3:uid="{F0571376-132B-F940-9609-6B59D9845B1B}" name="Characteristics [Temperature Day]" dataDxfId="56"/>
-    <tableColumn id="45" xr3:uid="{23233498-CFC4-9F46-94D5-39E7A6B5AFB5}" name="Term Source REF [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="55"/>
-    <tableColumn id="46" xr3:uid="{346D483D-D0DE-5140-A015-4AD0367BAD4D}" name="Term Accession Number [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="54"/>
-    <tableColumn id="66" xr3:uid="{57808D06-1B53-8D41-BEB4-1644A20F7763}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="53"/>
-    <tableColumn id="67" xr3:uid="{A7356A0D-0EFD-3D44-9B2F-4566273E79E8}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="52"/>
-    <tableColumn id="68" xr3:uid="{AD21FFE5-445B-CB42-B199-FDD8BAD5635D}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="51"/>
-    <tableColumn id="47" xr3:uid="{2AB78931-B301-314A-9311-2CC2C21128D4}" name="Characteristics [Temperature Night]" dataDxfId="50"/>
-    <tableColumn id="48" xr3:uid="{3A76D4EC-C74F-0A4B-B340-8EF3D8B86ECB}" name="Term Source REF [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="49"/>
-    <tableColumn id="49" xr3:uid="{87034985-F2AC-A145-AA6A-9EDB63F919F9}" name="Term Accession Number [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="48"/>
-    <tableColumn id="69" xr3:uid="{6D54D968-A087-944D-BF64-3AC3D5B08F80}" name="Unit [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="47"/>
-    <tableColumn id="70" xr3:uid="{AE04B49D-BF47-F34B-B52A-752ECD10B8C7}" name="Term Source REF [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="46"/>
-    <tableColumn id="71" xr3:uid="{2A40040A-D450-EF49-AB82-0CEEB3D8A599}" name="Term Accession Number [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="45"/>
-    <tableColumn id="50" xr3:uid="{FC29A38A-1769-7349-A9E5-A5184C62F33A}" name="Characteristics [watering exposure]" dataDxfId="44"/>
-    <tableColumn id="51" xr3:uid="{808AA82E-ECE0-AD47-92D3-27D7C93007B7}" name="Term Source REF [watering exposure] (#h; #tPECO:0007383)" dataDxfId="43"/>
-    <tableColumn id="52" xr3:uid="{7C45B5F9-759B-E646-A40E-CB5363DF17A8}" name="Term Accession Number [watering exposure] (#h; #tPECO:0007383)" dataDxfId="42"/>
-    <tableColumn id="53" xr3:uid="{70DF5752-BECA-5342-9001-FA7F5271BC54}" name="Characteristics [plant nutrient exposure]" dataDxfId="41"/>
-    <tableColumn id="54" xr3:uid="{FD6AD7C0-D253-D04C-8B67-6124B6C5D685}" name="Term Source REF [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="40"/>
-    <tableColumn id="55" xr3:uid="{95BC5752-0FFE-8C4E-BFE3-4FED8B72A648}" name="Term Accession Number [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="39"/>
-    <tableColumn id="56" xr3:uid="{25540F7D-0E49-F74B-8EF6-6E2314EBD1B1}" name="Characteristics [abiotic plant exposure]" dataDxfId="38"/>
-    <tableColumn id="57" xr3:uid="{19EC9032-1152-F940-ADB1-397E054EED4E}" name="Term Source REF [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="37"/>
-    <tableColumn id="58" xr3:uid="{40EA0154-215C-C44C-A5D6-852F5DA9A25C}" name="Term Accession Number [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="36"/>
-    <tableColumn id="59" xr3:uid="{C208C009-B835-0041-9A5C-978B7EABB59C}" name="Characteristics [biotic plant exposure]" dataDxfId="35"/>
-    <tableColumn id="60" xr3:uid="{2836636A-01C7-9C4E-9B41-EE6FEE3D7B80}" name="Term Source REF [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="34"/>
-    <tableColumn id="61" xr3:uid="{E4A74FCF-2E01-354A-99CE-0602774F8706}" name="Term Accession Number [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="33"/>
-    <tableColumn id="141" xr3:uid="{76BC0B00-263D-ED4F-A9A2-143148146694}" name="Characteristics [Geogaphic Area]" dataDxfId="6"/>
-    <tableColumn id="142" xr3:uid="{752BC19A-0C01-7F45-9374-DD0350C7B0D8}" name="Term Source REF [Geogaphic Area] (#h; #tNFDI4PSO:0000074)" dataDxfId="8"/>
-    <tableColumn id="143" xr3:uid="{5E52848A-36B7-4E4F-B77F-EFA6EC9BD00B}" name="Term Accession Number [Geogaphic Area] (#h; #tNFDI4PSO:0000074)" dataDxfId="7"/>
-    <tableColumn id="144" xr3:uid="{AD03CA40-5B78-8B41-9E4D-03DCE23E11E1}" name="Characteristics [Sample Collection Date]" dataDxfId="5"/>
-    <tableColumn id="145" xr3:uid="{6AC68041-2E25-9444-831A-05A07C9D4229}" name="Term Source REF [Sample Collection Date] (#h; #tNFDI4PSO:0000075)" dataDxfId="4"/>
-    <tableColumn id="146" xr3:uid="{7C695C41-0D47-6842-83E2-1435AFB1EF52}" name="Term Accession Number [Sample Collection Date] (#h; #tNFDI4PSO:0000075)" dataDxfId="3"/>
-    <tableColumn id="147" xr3:uid="{1F9082F2-7F61-614D-B072-F3DE7238714F}" name="Characteristics [Sample Collected By]" dataDxfId="2"/>
-    <tableColumn id="148" xr3:uid="{5F6F8541-8734-6242-A386-C4FCE4A4D156}" name="Term Source REF [Sample Collected By] (#h; #tNFDI4PSO:0000076)" dataDxfId="1"/>
-    <tableColumn id="149" xr3:uid="{36185F91-0DB8-EE4B-96A2-DF807E8CD12E}" name="Term Accession Number [Sample Collected By] (#h; #tNFDI4PSO:0000076)" dataDxfId="0"/>
-    <tableColumn id="62" xr3:uid="{12C4BED6-C71D-CC43-B976-AECFD0AF0BCF}" name="Characteristics [Time point]" dataDxfId="32"/>
-    <tableColumn id="63" xr3:uid="{D78E63DF-76E2-AE4F-A9AA-86CB096E0FD1}" name="Term Source REF [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="31"/>
-    <tableColumn id="64" xr3:uid="{4E3E838B-D518-9B41-95E4-AE65DE3C4242}" name="Term Accession Number [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="30"/>
-    <tableColumn id="75" xr3:uid="{7FBEC602-6866-EE4C-901B-A620EADE0B55}" name="Parameter [Sample Collection Method]" dataDxfId="29"/>
-    <tableColumn id="76" xr3:uid="{082E37E1-9067-2344-AFED-4C0AB2E6608F}" name="Term Source REF [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="28"/>
-    <tableColumn id="77" xr3:uid="{23CA10DE-9FDA-A94D-84CF-7C5F7143EE90}" name="Term Accession Number [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="27"/>
-    <tableColumn id="78" xr3:uid="{DD36BBD7-7DDE-4B4B-B0E7-E088C0737C72}" name="Parameter [Metabolism quenching method]" dataDxfId="26"/>
-    <tableColumn id="79" xr3:uid="{E9A2A827-A7E3-E44F-8034-982633580E8D}" name="Term Source REF [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="25"/>
-    <tableColumn id="80" xr3:uid="{ECB588C7-B9C0-8741-BE8A-1CDECCED4ED4}" name="Term Accession Number [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="24"/>
-    <tableColumn id="81" xr3:uid="{125431A9-D115-4A4B-A917-1C0A2F361D5C}" name="Parameter [Sample storage]" dataDxfId="23"/>
-    <tableColumn id="82" xr3:uid="{A56F8F05-EAAB-FD40-8F2F-AD66235065C4}" name="Term Source REF [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="22"/>
-    <tableColumn id="83" xr3:uid="{AB05BD40-EE64-3547-80D7-EDD26BB0F77A}" name="Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="21"/>
+    <tableColumn id="129" xr3:uid="{A1014B91-8574-664B-A628-2DDC01083E67}" name="Characteristics [Plant disease]" dataDxfId="86"/>
+    <tableColumn id="130" xr3:uid="{CF451DD4-AB45-1144-8BBF-C2C23EAE7EBC}" name="Term Source REF [Plant disease] (#h; #tNFDI4PSO:0000071)" dataDxfId="85"/>
+    <tableColumn id="131" xr3:uid="{4A90236E-F6AF-BE44-8703-08F06FE96AF5}" name="Term Accession Number [Plant disease] (#h; #tNFDI4PSO:0000071)" dataDxfId="84"/>
+    <tableColumn id="132" xr3:uid="{1F37D0D2-6260-584B-9CC0-9A72C472F841}" name="Characteristics [Plant disease stage]" dataDxfId="83"/>
+    <tableColumn id="133" xr3:uid="{2348DA4F-92E0-8547-AA7D-FCB641272A62}" name="Term Source REF [Plant disease stage] (#h; #tNFDI4PSO:0000072)" dataDxfId="82"/>
+    <tableColumn id="134" xr3:uid="{76B2929E-FEFA-C94A-9351-B07EA87DB902}" name="Term Accession Number [Plant disease stage] (#h; #tNFDI4PSO:0000072)" dataDxfId="81"/>
+    <tableColumn id="135" xr3:uid="{BEBD2093-9306-0C42-AFAE-735502002BE7}" name="Characteristics [Phenotype]" dataDxfId="80"/>
+    <tableColumn id="136" xr3:uid="{109579A2-3212-484D-A514-9571CF9305C5}" name="Term Source REF [Phenotype] (#h; #tNFDI4PSO:0000073)" dataDxfId="79"/>
+    <tableColumn id="137" xr3:uid="{77978229-5807-DE4F-A777-C5E343D79A55}" name="Term Accession Number [Phenotype] (#h; #tNFDI4PSO:0000073)" dataDxfId="78"/>
+    <tableColumn id="138" xr3:uid="{65D76AFE-F9A3-544C-B9C1-4D6C71488C92}" name="Characteristics [whole plant size]" dataDxfId="77"/>
+    <tableColumn id="139" xr3:uid="{91B73049-DC8D-D94B-8B5F-76E283D04557}" name="Term Source REF [whole plant size] (#h; #tTO:1000012)" dataDxfId="76"/>
+    <tableColumn id="140" xr3:uid="{6FB79EF4-9E54-8D45-BB9F-CE997665B054}" name="Term Accession Number [whole plant size] (#h; #tTO:1000012)" dataDxfId="75"/>
+    <tableColumn id="26" xr3:uid="{5E219BCA-059A-CC41-93BF-8CD61AA9572D}" name="Characteristics [study type]" dataDxfId="74"/>
+    <tableColumn id="27" xr3:uid="{5FF2BBBF-350F-9842-8FDF-2F895B07EADF}" name="Term Source REF [study type] (#h; #tPECO:0007231)" dataDxfId="73"/>
+    <tableColumn id="28" xr3:uid="{E12790EC-754D-3244-8A7A-1242F7942612}" name="Term Accession Number [study type] (#h; #tPECO:0007231)" dataDxfId="72"/>
+    <tableColumn id="23" xr3:uid="{E0A293FE-1EF5-A949-9C12-ADF40314B418}" name="Characteristics [plant growth medium exposure]" dataDxfId="71"/>
+    <tableColumn id="24" xr3:uid="{0C19F4A6-F9E8-1F4F-9B61-EB31E6DF451A}" name="Term Source REF [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="70"/>
+    <tableColumn id="25" xr3:uid="{7BBED07D-F814-A245-B090-723342B3D631}" name="Term Accession Number [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="69"/>
+    <tableColumn id="29" xr3:uid="{C386EF1A-F4F8-C543-99A0-ABD311BD175F}" name="Characteristics [growth plot design]" dataDxfId="68"/>
+    <tableColumn id="30" xr3:uid="{86FAE20B-4F89-EE4F-91E6-CE3B7E712F95}" name="Term Source REF [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="67"/>
+    <tableColumn id="31" xr3:uid="{C0949892-595C-9742-BCD1-75134FAC012F}" name="Term Accession Number [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="66"/>
+    <tableColumn id="32" xr3:uid="{B90A4652-69D5-2E4F-8A64-A3A5A5CB24DB}" name="Characteristics [Growth day length]" dataDxfId="65"/>
+    <tableColumn id="33" xr3:uid="{4E2448E1-3D08-504C-8FE3-D71B801F4DC9}" name="Term Source REF [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="64"/>
+    <tableColumn id="34" xr3:uid="{D47410BE-0000-B648-8CE5-966EE8968909}" name="Term Accession Number [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="63"/>
+    <tableColumn id="35" xr3:uid="{27034924-8879-044A-819B-7DC832A9D603}" name="Characteristics [light intensity exposure]" dataDxfId="62"/>
+    <tableColumn id="36" xr3:uid="{FD04748E-7F58-4A46-A167-E5EB1375A50B}" name="Term Source REF [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="61"/>
+    <tableColumn id="37" xr3:uid="{D76E6422-DF20-B94A-B5A6-4FD7F7923EBF}" name="Term Accession Number [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{8E446DD1-817A-E84A-9536-47B88B72BFD8}" name="Unit [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{BCB29467-6D87-F141-98A0-60243765731F}" name="Term Source REF [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{D2565EAD-7C86-C343-800D-E37FD463093B}" name="Term Accession Number [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="57"/>
+    <tableColumn id="38" xr3:uid="{21746D48-E9A2-5B42-BC00-F5AFD4793AA7}" name="Characteristics [Humidity Day]" dataDxfId="56"/>
+    <tableColumn id="39" xr3:uid="{8B1D9CC4-6026-674C-9852-06A06365907B}" name="Term Source REF [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="55"/>
+    <tableColumn id="40" xr3:uid="{8CCA0026-8267-884E-8F9A-369ACCB825EA}" name="Term Accession Number [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{9508FD23-5388-F64E-8286-05B533856CA2}" name="Unit [percent] (#h; #tUO:0000187; #u)" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{F796BC22-CBE1-6D41-824E-F655C3F9D5B6}" name="Term Source REF [percent] (#h; #tUO:0000187; #u)" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{32AC3DD8-82CD-4349-BFD5-0805A34144D8}" name="Term Accession Number [percent] (#h; #tUO:0000187; #u)" dataDxfId="51"/>
+    <tableColumn id="41" xr3:uid="{F4E42B79-6B62-E34C-95BE-8906E80BFBC8}" name="Characteristics [Humidity Night]" dataDxfId="50"/>
+    <tableColumn id="42" xr3:uid="{FE26FC08-E3D1-7547-8E20-1363EF47EE86}" name="Term Source REF [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="49"/>
+    <tableColumn id="43" xr3:uid="{C6D20AF0-60A8-874E-9614-2A2F483EB262}" name="Term Accession Number [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="48"/>
+    <tableColumn id="12" xr3:uid="{2866C2CF-81B3-694E-B2D9-F69059F54AA2}" name="Unit [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="47"/>
+    <tableColumn id="13" xr3:uid="{A885FE47-7729-3B45-B73D-03FF1F114CD5}" name="Term Source REF [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="46"/>
+    <tableColumn id="65" xr3:uid="{A3AEBB25-5500-F249-866E-C98439259F17}" name="Term Accession Number [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="45"/>
+    <tableColumn id="44" xr3:uid="{F0571376-132B-F940-9609-6B59D9845B1B}" name="Characteristics [Temperature Day]" dataDxfId="44"/>
+    <tableColumn id="45" xr3:uid="{23233498-CFC4-9F46-94D5-39E7A6B5AFB5}" name="Term Source REF [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="43"/>
+    <tableColumn id="46" xr3:uid="{346D483D-D0DE-5140-A015-4AD0367BAD4D}" name="Term Accession Number [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="42"/>
+    <tableColumn id="66" xr3:uid="{57808D06-1B53-8D41-BEB4-1644A20F7763}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="41"/>
+    <tableColumn id="67" xr3:uid="{A7356A0D-0EFD-3D44-9B2F-4566273E79E8}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="40"/>
+    <tableColumn id="68" xr3:uid="{AD21FFE5-445B-CB42-B199-FDD8BAD5635D}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="39"/>
+    <tableColumn id="47" xr3:uid="{2AB78931-B301-314A-9311-2CC2C21128D4}" name="Characteristics [Temperature Night]" dataDxfId="38"/>
+    <tableColumn id="48" xr3:uid="{3A76D4EC-C74F-0A4B-B340-8EF3D8B86ECB}" name="Term Source REF [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="37"/>
+    <tableColumn id="49" xr3:uid="{87034985-F2AC-A145-AA6A-9EDB63F919F9}" name="Term Accession Number [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="36"/>
+    <tableColumn id="69" xr3:uid="{6D54D968-A087-944D-BF64-3AC3D5B08F80}" name="Unit [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="35"/>
+    <tableColumn id="70" xr3:uid="{AE04B49D-BF47-F34B-B52A-752ECD10B8C7}" name="Term Source REF [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="34"/>
+    <tableColumn id="71" xr3:uid="{2A40040A-D450-EF49-AB82-0CEEB3D8A599}" name="Term Accession Number [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="33"/>
+    <tableColumn id="50" xr3:uid="{FC29A38A-1769-7349-A9E5-A5184C62F33A}" name="Characteristics [watering exposure]" dataDxfId="32"/>
+    <tableColumn id="51" xr3:uid="{808AA82E-ECE0-AD47-92D3-27D7C93007B7}" name="Term Source REF [watering exposure] (#h; #tPECO:0007383)" dataDxfId="31"/>
+    <tableColumn id="52" xr3:uid="{7C45B5F9-759B-E646-A40E-CB5363DF17A8}" name="Term Accession Number [watering exposure] (#h; #tPECO:0007383)" dataDxfId="30"/>
+    <tableColumn id="53" xr3:uid="{70DF5752-BECA-5342-9001-FA7F5271BC54}" name="Characteristics [plant nutrient exposure]" dataDxfId="29"/>
+    <tableColumn id="54" xr3:uid="{FD6AD7C0-D253-D04C-8B67-6124B6C5D685}" name="Term Source REF [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="28"/>
+    <tableColumn id="55" xr3:uid="{95BC5752-0FFE-8C4E-BFE3-4FED8B72A648}" name="Term Accession Number [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="27"/>
+    <tableColumn id="56" xr3:uid="{25540F7D-0E49-F74B-8EF6-6E2314EBD1B1}" name="Characteristics [abiotic plant exposure]" dataDxfId="26"/>
+    <tableColumn id="57" xr3:uid="{19EC9032-1152-F940-ADB1-397E054EED4E}" name="Term Source REF [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="25"/>
+    <tableColumn id="58" xr3:uid="{40EA0154-215C-C44C-A5D6-852F5DA9A25C}" name="Term Accession Number [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="24"/>
+    <tableColumn id="59" xr3:uid="{C208C009-B835-0041-9A5C-978B7EABB59C}" name="Characteristics [biotic plant exposure]" dataDxfId="23"/>
+    <tableColumn id="60" xr3:uid="{2836636A-01C7-9C4E-9B41-EE6FEE3D7B80}" name="Term Source REF [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="22"/>
+    <tableColumn id="61" xr3:uid="{E4A74FCF-2E01-354A-99CE-0602774F8706}" name="Term Accession Number [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="21"/>
+    <tableColumn id="141" xr3:uid="{76BC0B00-263D-ED4F-A9A2-143148146694}" name="Characteristics [Geogaphic Area]" dataDxfId="20"/>
+    <tableColumn id="142" xr3:uid="{752BC19A-0C01-7F45-9374-DD0350C7B0D8}" name="Term Source REF [Geogaphic Area] (#h; #tNFDI4PSO:0000074)" dataDxfId="19"/>
+    <tableColumn id="143" xr3:uid="{5E52848A-36B7-4E4F-B77F-EFA6EC9BD00B}" name="Term Accession Number [Geogaphic Area] (#h; #tNFDI4PSO:0000074)" dataDxfId="18"/>
+    <tableColumn id="144" xr3:uid="{AD03CA40-5B78-8B41-9E4D-03DCE23E11E1}" name="Characteristics [Sample Collection Date]" dataDxfId="17"/>
+    <tableColumn id="145" xr3:uid="{6AC68041-2E25-9444-831A-05A07C9D4229}" name="Term Source REF [Sample Collection Date] (#h; #tNFDI4PSO:0000075)" dataDxfId="16"/>
+    <tableColumn id="146" xr3:uid="{7C695C41-0D47-6842-83E2-1435AFB1EF52}" name="Term Accession Number [Sample Collection Date] (#h; #tNFDI4PSO:0000075)" dataDxfId="15"/>
+    <tableColumn id="147" xr3:uid="{1F9082F2-7F61-614D-B072-F3DE7238714F}" name="Characteristics [Sample Collected By]" dataDxfId="14"/>
+    <tableColumn id="148" xr3:uid="{5F6F8541-8734-6242-A386-C4FCE4A4D156}" name="Term Source REF [Sample Collected By] (#h; #tNFDI4PSO:0000076)" dataDxfId="13"/>
+    <tableColumn id="149" xr3:uid="{36185F91-0DB8-EE4B-96A2-DF807E8CD12E}" name="Term Accession Number [Sample Collected By] (#h; #tNFDI4PSO:0000076)" dataDxfId="12"/>
+    <tableColumn id="62" xr3:uid="{12C4BED6-C71D-CC43-B976-AECFD0AF0BCF}" name="Characteristics [Time point]" dataDxfId="11"/>
+    <tableColumn id="63" xr3:uid="{D78E63DF-76E2-AE4F-A9AA-86CB096E0FD1}" name="Term Source REF [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="10"/>
+    <tableColumn id="64" xr3:uid="{4E3E838B-D518-9B41-95E4-AE65DE3C4242}" name="Term Accession Number [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="9"/>
+    <tableColumn id="75" xr3:uid="{7FBEC602-6866-EE4C-901B-A620EADE0B55}" name="Parameter [Sample Collection Method]" dataDxfId="8"/>
+    <tableColumn id="76" xr3:uid="{082E37E1-9067-2344-AFED-4C0AB2E6608F}" name="Term Source REF [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="7"/>
+    <tableColumn id="77" xr3:uid="{23CA10DE-9FDA-A94D-84CF-7C5F7143EE90}" name="Term Accession Number [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="6"/>
+    <tableColumn id="78" xr3:uid="{DD36BBD7-7DDE-4B4B-B0E7-E088C0737C72}" name="Parameter [Metabolism quenching method]" dataDxfId="5"/>
+    <tableColumn id="79" xr3:uid="{E9A2A827-A7E3-E44F-8034-982633580E8D}" name="Term Source REF [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="4"/>
+    <tableColumn id="80" xr3:uid="{ECB588C7-B9C0-8741-BE8A-1CDECCED4ED4}" name="Term Accession Number [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="3"/>
+    <tableColumn id="81" xr3:uid="{125431A9-D115-4A4B-A917-1C0A2F361D5C}" name="Parameter [Sample storage]" dataDxfId="2"/>
+    <tableColumn id="82" xr3:uid="{A56F8F05-EAAB-FD40-8F2F-AD66235065C4}" name="Term Source REF [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="1"/>
+    <tableColumn id="83" xr3:uid="{AB05BD40-EE64-3547-80D7-EDD26BB0F77A}" name="Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3125,10 +3125,10 @@
   <dimension ref="A1:EI47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="21" topLeftCell="AL22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="21" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="AE23" sqref="AE23"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.5" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3137,131 +3137,131 @@
     <col min="3" max="3" width="29.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="59.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="53.5" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="59.6640625" style="4" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="33.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="59" style="4" customWidth="1"/>
-    <col min="10" max="10" width="65.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="59" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="65.33203125" style="4" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="67.6640625" style="62" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="51.1640625" style="62" customWidth="1"/>
-    <col min="13" max="13" width="57.33203125" style="62" customWidth="1"/>
+    <col min="12" max="12" width="51.1640625" style="62" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="57.33203125" style="62" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="38" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="48.5" style="4" customWidth="1"/>
-    <col min="16" max="16" width="54.6640625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="48.5" style="4" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="54.6640625" style="4" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="35.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="49.33203125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="55.6640625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="49.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="55.6640625" style="4" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="35.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="49.5" style="4" customWidth="1"/>
-    <col min="22" max="22" width="55.83203125" style="4" customWidth="1"/>
+    <col min="21" max="21" width="49.5" style="4" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="55.83203125" style="4" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="35.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="51.1640625" style="4" customWidth="1"/>
-    <col min="25" max="25" width="57.33203125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="51.1640625" style="4" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="57.33203125" style="4" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="64.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="46.1640625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="52.33203125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="46.1640625" style="4" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="52.33203125" style="4" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="47.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="55.1640625" style="4" customWidth="1"/>
-    <col min="31" max="31" width="61.33203125" style="4" customWidth="1"/>
+    <col min="30" max="30" width="55.1640625" style="4" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="61.33203125" style="4" hidden="1" customWidth="1"/>
     <col min="32" max="32" width="38" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="49.5" style="4" customWidth="1"/>
-    <col min="34" max="34" width="55.83203125" style="4" customWidth="1"/>
+    <col min="33" max="33" width="49.5" style="4" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="55.83203125" style="4" hidden="1" customWidth="1"/>
     <col min="35" max="35" width="49" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="50.33203125" style="4" customWidth="1"/>
-    <col min="37" max="37" width="56.5" style="4" customWidth="1"/>
+    <col min="36" max="36" width="50.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="56.5" style="4" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="37.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="46" style="4" customWidth="1"/>
-    <col min="40" max="40" width="52.1640625" style="4" customWidth="1"/>
+    <col min="39" max="39" width="46" style="4" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="52.1640625" style="4" hidden="1" customWidth="1"/>
     <col min="41" max="41" width="38" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="61.33203125" style="4" customWidth="1"/>
-    <col min="43" max="43" width="67.5" style="4" customWidth="1"/>
+    <col min="42" max="42" width="61.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="67.5" style="4" hidden="1" customWidth="1"/>
     <col min="44" max="44" width="39.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="54" style="4" customWidth="1"/>
-    <col min="46" max="46" width="60.33203125" style="4" customWidth="1"/>
+    <col min="45" max="45" width="54" style="4" hidden="1" customWidth="1"/>
+    <col min="46" max="46" width="60.33203125" style="4" hidden="1" customWidth="1"/>
     <col min="47" max="47" width="35.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="59.1640625" style="4" customWidth="1"/>
-    <col min="49" max="49" width="65.5" style="4" customWidth="1"/>
+    <col min="48" max="48" width="59.1640625" style="4" hidden="1" customWidth="1"/>
+    <col min="49" max="49" width="65.5" style="4" hidden="1" customWidth="1"/>
     <col min="50" max="50" width="38.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="51.83203125" style="4" customWidth="1"/>
-    <col min="52" max="52" width="58" style="4" customWidth="1"/>
+    <col min="51" max="51" width="51.83203125" style="4" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="58" style="4" hidden="1" customWidth="1"/>
     <col min="53" max="53" width="31.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="50.33203125" style="4" customWidth="1"/>
-    <col min="55" max="55" width="56.5" style="4" customWidth="1"/>
+    <col min="54" max="54" width="50.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="56.5" style="4" hidden="1" customWidth="1"/>
     <col min="56" max="56" width="39.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="47.5" style="4" customWidth="1"/>
-    <col min="58" max="58" width="53.6640625" style="4" customWidth="1"/>
+    <col min="57" max="57" width="47.5" style="4" hidden="1" customWidth="1"/>
+    <col min="58" max="58" width="53.6640625" style="4" hidden="1" customWidth="1"/>
     <col min="59" max="59" width="44.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="65.33203125" style="4" customWidth="1"/>
-    <col min="61" max="61" width="71.5" style="4" customWidth="1"/>
+    <col min="60" max="60" width="65.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="71.5" style="4" hidden="1" customWidth="1"/>
     <col min="62" max="62" width="43" style="4" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="58.6640625" style="4" customWidth="1"/>
-    <col min="64" max="64" width="64.83203125" style="4" customWidth="1"/>
+    <col min="63" max="63" width="58.6640625" style="4" hidden="1" customWidth="1"/>
+    <col min="64" max="64" width="64.83203125" style="4" hidden="1" customWidth="1"/>
     <col min="65" max="65" width="39.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="58.6640625" style="4" customWidth="1"/>
-    <col min="67" max="67" width="64.83203125" style="4" customWidth="1"/>
+    <col min="66" max="66" width="58.6640625" style="4" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="64.83203125" style="4" hidden="1" customWidth="1"/>
     <col min="68" max="68" width="39.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="58.5" style="4" customWidth="1"/>
-    <col min="70" max="70" width="64.6640625" style="4" customWidth="1"/>
-    <col min="71" max="71" width="65.5" style="4" customWidth="1"/>
-    <col min="72" max="72" width="76.33203125" style="4" customWidth="1"/>
-    <col min="73" max="73" width="82.5" style="4" customWidth="1"/>
+    <col min="69" max="69" width="58.5" style="4" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="64.6640625" style="4" hidden="1" customWidth="1"/>
+    <col min="71" max="71" width="65.5" style="4" hidden="1" customWidth="1"/>
+    <col min="72" max="72" width="76.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="73" max="73" width="82.5" style="4" hidden="1" customWidth="1"/>
     <col min="74" max="74" width="77.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="54.6640625" style="4" customWidth="1"/>
-    <col min="76" max="76" width="61" style="4" customWidth="1"/>
-    <col min="77" max="77" width="35.5" style="4" customWidth="1"/>
-    <col min="78" max="78" width="46.33203125" style="4" customWidth="1"/>
-    <col min="79" max="79" width="52.5" style="4" customWidth="1"/>
+    <col min="75" max="75" width="54.6640625" style="4" hidden="1" customWidth="1"/>
+    <col min="76" max="76" width="61" style="4" hidden="1" customWidth="1"/>
+    <col min="77" max="77" width="35.5" style="4" hidden="1" customWidth="1"/>
+    <col min="78" max="78" width="46.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="79" max="79" width="52.5" style="4" hidden="1" customWidth="1"/>
     <col min="80" max="80" width="30.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="56" style="4" customWidth="1"/>
-    <col min="82" max="82" width="62.1640625" style="4" customWidth="1"/>
-    <col min="83" max="83" width="38.5" style="4" customWidth="1"/>
-    <col min="84" max="84" width="49.33203125" style="4" customWidth="1"/>
-    <col min="85" max="85" width="55.6640625" style="4" customWidth="1"/>
+    <col min="81" max="81" width="56" style="4" hidden="1" customWidth="1"/>
+    <col min="82" max="82" width="62.1640625" style="4" hidden="1" customWidth="1"/>
+    <col min="83" max="83" width="38.5" style="4" hidden="1" customWidth="1"/>
+    <col min="84" max="84" width="49.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="85" max="85" width="55.6640625" style="4" hidden="1" customWidth="1"/>
     <col min="86" max="86" width="79.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="57.83203125" style="4" customWidth="1"/>
-    <col min="88" max="88" width="64" style="4" customWidth="1"/>
-    <col min="89" max="89" width="41.33203125" style="4" customWidth="1"/>
-    <col min="90" max="90" width="52.1640625" style="4" customWidth="1"/>
-    <col min="91" max="91" width="58.33203125" style="4" customWidth="1"/>
+    <col min="87" max="87" width="57.83203125" style="4" hidden="1" customWidth="1"/>
+    <col min="88" max="88" width="64" style="4" hidden="1" customWidth="1"/>
+    <col min="89" max="89" width="41.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="90" max="90" width="52.1640625" style="4" hidden="1" customWidth="1"/>
+    <col min="91" max="91" width="58.33203125" style="4" hidden="1" customWidth="1"/>
     <col min="92" max="92" width="40.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="59" style="4" customWidth="1"/>
-    <col min="94" max="94" width="65.33203125" style="4" customWidth="1"/>
-    <col min="95" max="95" width="44.33203125" style="4" customWidth="1"/>
-    <col min="96" max="96" width="55.33203125" style="4" customWidth="1"/>
-    <col min="97" max="97" width="61.5" style="4" customWidth="1"/>
+    <col min="93" max="93" width="59" style="4" hidden="1" customWidth="1"/>
+    <col min="94" max="94" width="65.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="95" max="95" width="44.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="96" max="96" width="55.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="97" max="97" width="61.5" style="4" hidden="1" customWidth="1"/>
     <col min="98" max="98" width="39.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="54.33203125" style="4" customWidth="1"/>
-    <col min="100" max="100" width="60.6640625" style="4" customWidth="1"/>
+    <col min="99" max="99" width="54.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="100" max="100" width="60.6640625" style="4" hidden="1" customWidth="1"/>
     <col min="101" max="101" width="39.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="58.33203125" style="4" customWidth="1"/>
-    <col min="103" max="103" width="64.5" style="4" customWidth="1"/>
+    <col min="102" max="102" width="58.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="103" max="103" width="64.5" style="4" hidden="1" customWidth="1"/>
     <col min="104" max="104" width="39.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="57.33203125" style="4" customWidth="1"/>
-    <col min="106" max="106" width="63.5" style="4" customWidth="1"/>
+    <col min="105" max="105" width="57.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="106" max="106" width="63.5" style="4" hidden="1" customWidth="1"/>
     <col min="107" max="107" width="85.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="56.33203125" style="4" customWidth="1"/>
-    <col min="109" max="109" width="62.5" style="4" customWidth="1"/>
-    <col min="110" max="110" width="35.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="56.33203125" style="4" customWidth="1"/>
-    <col min="112" max="112" width="62.5" style="4" customWidth="1"/>
-    <col min="113" max="113" width="37.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="62.6640625" style="4" customWidth="1"/>
-    <col min="115" max="115" width="68.83203125" style="4" customWidth="1"/>
-    <col min="116" max="116" width="35" style="4" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="60.33203125" style="4" customWidth="1"/>
-    <col min="118" max="118" width="66.5" style="4" customWidth="1"/>
-    <col min="119" max="119" width="60.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="52" style="4" customWidth="1"/>
-    <col min="121" max="121" width="58.1640625" style="4" customWidth="1"/>
+    <col min="108" max="108" width="56.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="109" max="109" width="62.5" style="4" hidden="1" customWidth="1"/>
+    <col min="110" max="110" width="38" style="4" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="56.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="112" max="112" width="62.5" style="4" hidden="1" customWidth="1"/>
+    <col min="113" max="113" width="38" style="4" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="62.6640625" style="4" hidden="1" customWidth="1"/>
+    <col min="115" max="115" width="68.83203125" style="4" hidden="1" customWidth="1"/>
+    <col min="116" max="116" width="38" style="4" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="60.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="118" max="118" width="66.5" style="4" hidden="1" customWidth="1"/>
+    <col min="119" max="119" width="35.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="52" style="4" hidden="1" customWidth="1"/>
+    <col min="121" max="121" width="58.1640625" style="4" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="36.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="65" style="4" customWidth="1"/>
-    <col min="124" max="124" width="71.33203125" style="4" customWidth="1"/>
+    <col min="123" max="123" width="65" style="4" hidden="1" customWidth="1"/>
+    <col min="124" max="124" width="71.33203125" style="4" hidden="1" customWidth="1"/>
     <col min="125" max="125" width="40.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="69.1640625" style="4" customWidth="1"/>
-    <col min="127" max="127" width="75.33203125" style="4" customWidth="1"/>
-    <col min="128" max="128" width="27.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="56.1640625" style="4" customWidth="1"/>
-    <col min="130" max="130" width="62.33203125" style="4" customWidth="1"/>
+    <col min="126" max="126" width="69.1640625" style="4" hidden="1" customWidth="1"/>
+    <col min="127" max="127" width="75.33203125" style="4" hidden="1" customWidth="1"/>
+    <col min="128" max="128" width="60.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="56.1640625" style="4" hidden="1" customWidth="1"/>
+    <col min="130" max="130" width="62.33203125" style="4" hidden="1" customWidth="1"/>
     <col min="131" max="16384" width="30.5" style="4"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Update Plant template to fix Swobup error and checklist
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants/1SPL01_plants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\SWATE_templates\templates\1SPL01_plants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2703D69F-EB79-419A-9C26-9A656470654E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EE26C3-1025-4123-95AA-C61FE06DDC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
@@ -1559,7 +1559,7 @@
     <numFmt numFmtId="165" formatCode="0.00\ &quot;percent&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1643,12 +1643,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1992,22 +1986,6 @@
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -3075,6 +3053,22 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3125,137 +3119,137 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7A0FDF1-D7A7-5444-9FF6-B24A8DE79F17}" name="annotationTable" displayName="annotationTable" ref="D2:EA3" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A7A0FDF1-D7A7-5444-9FF6-B24A8DE79F17}" name="annotationTable" displayName="annotationTable" ref="D2:EA3" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128">
   <autoFilter ref="D2:EA3" xr:uid="{8A7F28C9-E08B-8A4D-99FD-3313667921ED}"/>
   <tableColumns count="128">
-    <tableColumn id="1" xr3:uid="{9B8F9057-2F20-7A45-8C27-9A36422B26D5}" name="Source Name" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{CC93B5FA-49F4-9B4C-B1F6-452471229F30}" name="Sample Name" dataDxfId="128"/>
-    <tableColumn id="101" xr3:uid="{AA189B85-0B08-424F-93B5-6C2D3D660371}" name="Characteristics [Sample type]" dataDxfId="127"/>
-    <tableColumn id="102" xr3:uid="{B5019B54-7F43-2042-A406-B19B1779B047}" name="Term Source REF [Sample type] (#h; #tNFDI4PSO:0000064)" dataDxfId="126"/>
-    <tableColumn id="103" xr3:uid="{10BC9619-E39D-4A45-853C-57DD06C07840}" name="Term Accession Number [Sample type] (#h; #tNFDI4PSO:0000064)" dataDxfId="125"/>
-    <tableColumn id="72" xr3:uid="{A33FCD3B-AD29-A742-9D63-6ECAFBEE068E}" name="Characteristics [Biological replicate]" dataDxfId="124"/>
-    <tableColumn id="73" xr3:uid="{4059FECC-FE9D-5947-9219-570196389DAE}" name="Term Source REF [Biological replicate] (#h; #tNFDI4PSO:0000042)" dataDxfId="123"/>
-    <tableColumn id="74" xr3:uid="{E04811ED-EF58-AD4F-84F5-156D9251E904}" name="Term Accession Number [Biological replicate] (#h; #tNFDI4PSO:0000042)" dataDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{6A7FF2B3-5F1E-8245-AC4F-6198097A8123}" name="Characteristics [Organism]" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{CC831F2C-80A0-C84F-829F-23F6C78F2EEB}" name="Term Source REF [Organism] (#h; #tNFDI4PSO:0000030)" dataDxfId="120"/>
-    <tableColumn id="5" xr3:uid="{D6E59B6D-D53F-A840-A182-24AE5A460E1D}" name="Term Accession Number [Organism] (#h; #tNFDI4PSO:0000030)" dataDxfId="119"/>
-    <tableColumn id="114" xr3:uid="{DD7E5619-DB6E-F44E-B75B-1CA6BECA8011}" name="Characteristics [Isolate]" dataDxfId="118"/>
-    <tableColumn id="115" xr3:uid="{08C77E06-D2B6-CA44-AEE6-39AB1D06F432}" name="Term Source REF [Isolate] (#h; #tNFDI4PSO:0000065)" dataDxfId="117"/>
-    <tableColumn id="116" xr3:uid="{0E95421D-DECB-4248-99A3-002C66A0AEBF}" name="Term Accession Number [Isolate] (#h; #tNFDI4PSO:0000065)" dataDxfId="116"/>
-    <tableColumn id="107" xr3:uid="{CAC9E02B-4310-AC47-9C0B-C1B0925DA497}" name="Characteristics [Cultivar]" dataDxfId="115"/>
-    <tableColumn id="108" xr3:uid="{88369A2F-DDBC-7D42-9993-9C41B71C3C2F}" name="Term Source REF [Cultivar] (#h; #tNFDI4PSO:0000066)" dataDxfId="114"/>
-    <tableColumn id="109" xr3:uid="{C5014D52-D324-3246-B46B-898151F9B990}" name="Term Accession Number [Cultivar] (#h; #tNFDI4PSO:0000066)" dataDxfId="113"/>
-    <tableColumn id="110" xr3:uid="{700C615F-5CF8-8F43-8A5A-ABCBAE4EAD2E}" name="Characteristics [Ecotype]" dataDxfId="112"/>
-    <tableColumn id="111" xr3:uid="{BBBA29E7-DCD6-D342-B661-681AD683DD93}" name="Term Source REF [Ecotype] (#h; #tNFDI4PSO:0000067)" dataDxfId="111"/>
-    <tableColumn id="112" xr3:uid="{8EB5249F-48BB-634B-A2B1-ABD06733E545}" name="Term Accession Number [Ecotype] (#h; #tNFDI4PSO:0000067)" dataDxfId="110"/>
-    <tableColumn id="14" xr3:uid="{000DCCE3-5EF7-4F4E-A82A-AD088FF36730}" name="Characteristics [Genotype]" dataDxfId="109"/>
-    <tableColumn id="15" xr3:uid="{E2A1AEEB-EF2B-F448-824C-2953C18CC24A}" name="Term Source REF [Genotype] (#h; #tNFDI4PSO:0000031)" dataDxfId="108"/>
-    <tableColumn id="16" xr3:uid="{A998FE5F-8994-6E40-94FA-F0EF6DC905E4}" name="Term Accession Number [Genotype] (#h; #tNFDI4PSO:0000031)" dataDxfId="107"/>
-    <tableColumn id="117" xr3:uid="{FBA29C11-8E4B-6142-8B9C-9221A56EEA2B}" name="Characteristics [population]" dataDxfId="106"/>
-    <tableColumn id="118" xr3:uid="{B481BDF5-2297-0548-9D1D-97160F39EC7F}" name="Term Source REF [population] (#h; #tOBI:0000181)" dataDxfId="105"/>
-    <tableColumn id="119" xr3:uid="{F95C8EA9-3541-BC43-BA8C-78ED526D9471}" name="Term Accession Number [population] (#h; #tOBI:0000181)" dataDxfId="104"/>
-    <tableColumn id="17" xr3:uid="{0EB867DC-9BB4-6243-BEE9-01764D9FEB35}" name="Characteristics [Organism part]" dataDxfId="103"/>
-    <tableColumn id="18" xr3:uid="{B0CCF08F-B694-6C4F-94E6-E17AFD4C0A63}" name="Term Source REF [Organism part] (#h; #tNFDI4PSO:0000032)" dataDxfId="102"/>
-    <tableColumn id="19" xr3:uid="{6A02A31E-2B72-BE41-BF86-71E587B29D13}" name="Term Accession Number [Organism part] (#h; #tNFDI4PSO:0000032)" dataDxfId="101"/>
-    <tableColumn id="120" xr3:uid="{AD004493-349E-2948-B660-FFC9B04A3756}" name="Characteristics [Cell line]" dataDxfId="100"/>
-    <tableColumn id="121" xr3:uid="{2A484165-7392-6F45-8DA4-DB1A88B93DEC}" name="Term Source REF [Cell line] (#h; #tNFDI4PSO:0000068)" dataDxfId="99"/>
-    <tableColumn id="122" xr3:uid="{9AE3D69F-0281-4045-BFE6-C023EC048A62}" name="Term Accession Number [Cell line] (#h; #tNFDI4PSO:0000068)" dataDxfId="98"/>
-    <tableColumn id="123" xr3:uid="{B1A6199C-7EDD-564A-8155-ECC5A48569C0}" name="Characteristics [Cell type]" dataDxfId="97"/>
-    <tableColumn id="124" xr3:uid="{49433E8D-29BA-2E4F-9009-1F477D0C0EE1}" name="Term Source REF [Cell type] (#h; #tNFDI4PSO:0000069)" dataDxfId="96"/>
-    <tableColumn id="125" xr3:uid="{FC41F627-5506-0346-B969-E2BFB7E8F3BE}" name="Term Accession Number [Cell type] (#h; #tNFDI4PSO:0000069)" dataDxfId="95"/>
-    <tableColumn id="20" xr3:uid="{96C34AC4-65C0-774B-A5A0-1BC98C955028}" name="Characteristics [age]" dataDxfId="94"/>
-    <tableColumn id="21" xr3:uid="{325D3F43-A306-2F47-AD9C-92F61C0649E5}" name="Term Source REF [age] (#h; #tNFDI4PSO:0000033)" dataDxfId="93"/>
-    <tableColumn id="22" xr3:uid="{334AF647-E268-2E41-950D-8973A43E29C8}" name="Term Accession Number [age] (#h; #tNFDI4PSO:0000033)" dataDxfId="92"/>
-    <tableColumn id="126" xr3:uid="{D48EF60D-FFC4-DA42-8A84-9D7BEC94EB5C}" name="Characteristics [Developmental Stage]" dataDxfId="91"/>
-    <tableColumn id="127" xr3:uid="{B7FB233D-7D8A-A34E-91AE-3E96612329F2}" name="Term Source REF [Developmental Stage] (#h; #tNFDI4PSO:0000070)" dataDxfId="90"/>
-    <tableColumn id="128" xr3:uid="{0CFCFB6B-CC3F-A24A-B1A8-77F2863EAED6}" name="Term Accession Number [Developmental Stage] (#h; #tNFDI4PSO:0000070)" dataDxfId="89"/>
-    <tableColumn id="129" xr3:uid="{A1014B91-8574-664B-A628-2DDC01083E67}" name="Characteristics [Plant disease]" dataDxfId="88"/>
-    <tableColumn id="130" xr3:uid="{CF451DD4-AB45-1144-8BBF-C2C23EAE7EBC}" name="Term Source REF [Plant disease] (#h; #tNFDI4PSO:0000071)" dataDxfId="87"/>
-    <tableColumn id="131" xr3:uid="{4A90236E-F6AF-BE44-8703-08F06FE96AF5}" name="Term Accession Number [Plant disease] (#h; #tNFDI4PSO:0000071)" dataDxfId="86"/>
-    <tableColumn id="132" xr3:uid="{1F37D0D2-6260-584B-9CC0-9A72C472F841}" name="Characteristics [Plant disease stage]" dataDxfId="85"/>
-    <tableColumn id="133" xr3:uid="{2348DA4F-92E0-8547-AA7D-FCB641272A62}" name="Term Source REF [Plant disease stage] (#h; #tNFDI4PSO:0000072)" dataDxfId="84"/>
-    <tableColumn id="134" xr3:uid="{76B2929E-FEFA-C94A-9351-B07EA87DB902}" name="Term Accession Number [Plant disease stage] (#h; #tNFDI4PSO:0000072)" dataDxfId="83"/>
-    <tableColumn id="135" xr3:uid="{BEBD2093-9306-0C42-AFAE-735502002BE7}" name="Characteristics [Phenotype]" dataDxfId="82"/>
-    <tableColumn id="136" xr3:uid="{109579A2-3212-484D-A514-9571CF9305C5}" name="Term Source REF [Phenotype] (#h; #tNFDI4PSO:0000073)" dataDxfId="81"/>
-    <tableColumn id="137" xr3:uid="{77978229-5807-DE4F-A777-C5E343D79A55}" name="Term Accession Number [Phenotype] (#h; #tNFDI4PSO:0000073)" dataDxfId="80"/>
-    <tableColumn id="138" xr3:uid="{65D76AFE-F9A3-544C-B9C1-4D6C71488C92}" name="Characteristics [whole plant size]" dataDxfId="79"/>
-    <tableColumn id="139" xr3:uid="{91B73049-DC8D-D94B-8B5F-76E283D04557}" name="Term Source REF [whole plant size] (#h; #tTO:1000012)" dataDxfId="78"/>
-    <tableColumn id="140" xr3:uid="{6FB79EF4-9E54-8D45-BB9F-CE997665B054}" name="Term Accession Number [whole plant size] (#h; #tTO:1000012)" dataDxfId="77"/>
-    <tableColumn id="26" xr3:uid="{5E219BCA-059A-CC41-93BF-8CD61AA9572D}" name="Characteristics [study type]" dataDxfId="76"/>
-    <tableColumn id="27" xr3:uid="{5FF2BBBF-350F-9842-8FDF-2F895B07EADF}" name="Term Source REF [study type] (#h; #tPECO:0007231)" dataDxfId="75"/>
-    <tableColumn id="28" xr3:uid="{E12790EC-754D-3244-8A7A-1242F7942612}" name="Term Accession Number [study type] (#h; #tPECO:0007231)" dataDxfId="74"/>
-    <tableColumn id="23" xr3:uid="{E0A293FE-1EF5-A949-9C12-ADF40314B418}" name="Characteristics [plant growth medium exposure]" dataDxfId="73"/>
-    <tableColumn id="24" xr3:uid="{0C19F4A6-F9E8-1F4F-9B61-EB31E6DF451A}" name="Term Source REF [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="72"/>
-    <tableColumn id="25" xr3:uid="{7BBED07D-F814-A245-B090-723342B3D631}" name="Term Accession Number [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="71"/>
-    <tableColumn id="29" xr3:uid="{C386EF1A-F4F8-C543-99A0-ABD311BD175F}" name="Characteristics [growth plot design]" dataDxfId="70"/>
-    <tableColumn id="30" xr3:uid="{86FAE20B-4F89-EE4F-91E6-CE3B7E712F95}" name="Term Source REF [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="69"/>
-    <tableColumn id="31" xr3:uid="{C0949892-595C-9742-BCD1-75134FAC012F}" name="Term Accession Number [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="68"/>
-    <tableColumn id="32" xr3:uid="{B90A4652-69D5-2E4F-8A64-A3A5A5CB24DB}" name="Characteristics [Growth day length]" dataDxfId="67"/>
-    <tableColumn id="33" xr3:uid="{4E2448E1-3D08-504C-8FE3-D71B801F4DC9}" name="Term Source REF [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="66"/>
-    <tableColumn id="34" xr3:uid="{D47410BE-0000-B648-8CE5-966EE8968909}" name="Term Accession Number [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="65"/>
-    <tableColumn id="35" xr3:uid="{27034924-8879-044A-819B-7DC832A9D603}" name="Characteristics [light intensity exposure]" dataDxfId="64"/>
-    <tableColumn id="36" xr3:uid="{FD04748E-7F58-4A46-A167-E5EB1375A50B}" name="Term Source REF [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="63"/>
-    <tableColumn id="37" xr3:uid="{D76E6422-DF20-B94A-B5A6-4FD7F7923EBF}" name="Term Accession Number [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{8E446DD1-817A-E84A-9536-47B88B72BFD8}" name="Unit [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{BCB29467-6D87-F141-98A0-60243765731F}" name="Term Source REF [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{D2565EAD-7C86-C343-800D-E37FD463093B}" name="Term Accession Number [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="59"/>
-    <tableColumn id="38" xr3:uid="{21746D48-E9A2-5B42-BC00-F5AFD4793AA7}" name="Characteristics [Humidity Day]" dataDxfId="58"/>
-    <tableColumn id="39" xr3:uid="{8B1D9CC4-6026-674C-9852-06A06365907B}" name="Term Source REF [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="57"/>
-    <tableColumn id="40" xr3:uid="{8CCA0026-8267-884E-8F9A-369ACCB825EA}" name="Term Accession Number [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="56"/>
-    <tableColumn id="9" xr3:uid="{9508FD23-5388-F64E-8286-05B533856CA2}" name="Unit [percent] (#h; #tUO:0000187; #u)" dataDxfId="55"/>
-    <tableColumn id="10" xr3:uid="{F796BC22-CBE1-6D41-824E-F655C3F9D5B6}" name="Term Source REF [percent] (#h; #tUO:0000187; #u)" dataDxfId="54"/>
-    <tableColumn id="11" xr3:uid="{32AC3DD8-82CD-4349-BFD5-0805A34144D8}" name="Term Accession Number [percent] (#h; #tUO:0000187; #u)" dataDxfId="53"/>
-    <tableColumn id="41" xr3:uid="{F4E42B79-6B62-E34C-95BE-8906E80BFBC8}" name="Characteristics [Humidity Night]" dataDxfId="52"/>
-    <tableColumn id="42" xr3:uid="{FE26FC08-E3D1-7547-8E20-1363EF47EE86}" name="Term Source REF [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="51"/>
-    <tableColumn id="43" xr3:uid="{C6D20AF0-60A8-874E-9614-2A2F483EB262}" name="Term Accession Number [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="50"/>
-    <tableColumn id="12" xr3:uid="{2866C2CF-81B3-694E-B2D9-F69059F54AA2}" name="Unit [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="49"/>
-    <tableColumn id="13" xr3:uid="{A885FE47-7729-3B45-B73D-03FF1F114CD5}" name="Term Source REF [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="48"/>
-    <tableColumn id="65" xr3:uid="{A3AEBB25-5500-F249-866E-C98439259F17}" name="Term Accession Number [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="47"/>
-    <tableColumn id="44" xr3:uid="{F0571376-132B-F940-9609-6B59D9845B1B}" name="Characteristics [Temperature Day]" dataDxfId="46"/>
-    <tableColumn id="45" xr3:uid="{23233498-CFC4-9F46-94D5-39E7A6B5AFB5}" name="Term Source REF [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="45"/>
-    <tableColumn id="46" xr3:uid="{346D483D-D0DE-5140-A015-4AD0367BAD4D}" name="Term Accession Number [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="44"/>
-    <tableColumn id="66" xr3:uid="{57808D06-1B53-8D41-BEB4-1644A20F7763}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="43"/>
-    <tableColumn id="67" xr3:uid="{A7356A0D-0EFD-3D44-9B2F-4566273E79E8}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="42"/>
-    <tableColumn id="68" xr3:uid="{AD21FFE5-445B-CB42-B199-FDD8BAD5635D}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="41"/>
-    <tableColumn id="47" xr3:uid="{2AB78931-B301-314A-9311-2CC2C21128D4}" name="Characteristics [Temperature Night]" dataDxfId="40"/>
-    <tableColumn id="48" xr3:uid="{3A76D4EC-C74F-0A4B-B340-8EF3D8B86ECB}" name="Term Source REF [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="39"/>
-    <tableColumn id="49" xr3:uid="{87034985-F2AC-A145-AA6A-9EDB63F919F9}" name="Term Accession Number [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="38"/>
-    <tableColumn id="69" xr3:uid="{6D54D968-A087-944D-BF64-3AC3D5B08F80}" name="Unit [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="37"/>
-    <tableColumn id="70" xr3:uid="{AE04B49D-BF47-F34B-B52A-752ECD10B8C7}" name="Term Source REF [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="36"/>
-    <tableColumn id="71" xr3:uid="{2A40040A-D450-EF49-AB82-0CEEB3D8A599}" name="Term Accession Number [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="35"/>
-    <tableColumn id="50" xr3:uid="{FC29A38A-1769-7349-A9E5-A5184C62F33A}" name="Characteristics [watering exposure]" dataDxfId="34"/>
-    <tableColumn id="51" xr3:uid="{808AA82E-ECE0-AD47-92D3-27D7C93007B7}" name="Term Source REF [watering exposure] (#h; #tPECO:0007383)" dataDxfId="33"/>
-    <tableColumn id="52" xr3:uid="{7C45B5F9-759B-E646-A40E-CB5363DF17A8}" name="Term Accession Number [watering exposure] (#h; #tPECO:0007383)" dataDxfId="32"/>
-    <tableColumn id="53" xr3:uid="{70DF5752-BECA-5342-9001-FA7F5271BC54}" name="Characteristics [plant nutrient exposure]" dataDxfId="31"/>
-    <tableColumn id="54" xr3:uid="{FD6AD7C0-D253-D04C-8B67-6124B6C5D685}" name="Term Source REF [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="30"/>
-    <tableColumn id="55" xr3:uid="{95BC5752-0FFE-8C4E-BFE3-4FED8B72A648}" name="Term Accession Number [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="29"/>
-    <tableColumn id="56" xr3:uid="{25540F7D-0E49-F74B-8EF6-6E2314EBD1B1}" name="Characteristics [abiotic plant exposure]" dataDxfId="28"/>
-    <tableColumn id="57" xr3:uid="{19EC9032-1152-F940-ADB1-397E054EED4E}" name="Term Source REF [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="27"/>
-    <tableColumn id="58" xr3:uid="{40EA0154-215C-C44C-A5D6-852F5DA9A25C}" name="Term Accession Number [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="26"/>
-    <tableColumn id="59" xr3:uid="{C208C009-B835-0041-9A5C-978B7EABB59C}" name="Characteristics [biotic plant exposure]" dataDxfId="25"/>
-    <tableColumn id="60" xr3:uid="{2836636A-01C7-9C4E-9B41-EE6FEE3D7B80}" name="Term Source REF [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="24"/>
-    <tableColumn id="61" xr3:uid="{E4A74FCF-2E01-354A-99CE-0602774F8706}" name="Term Accession Number [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="23"/>
-    <tableColumn id="141" xr3:uid="{76BC0B00-263D-ED4F-A9A2-143148146694}" name="Characteristics [Geographic Area]" dataDxfId="22"/>
-    <tableColumn id="142" xr3:uid="{752BC19A-0C01-7F45-9374-DD0350C7B0D8}" name="Term Source REF [Geogaphic Area] (#h; #tNFDI4PSO:0000074)" dataDxfId="21"/>
-    <tableColumn id="143" xr3:uid="{5E52848A-36B7-4E4F-B77F-EFA6EC9BD00B}" name="Term Accession Number [Geogaphic Area] (#h; #tNFDI4PSO:0000074)" dataDxfId="20"/>
-    <tableColumn id="144" xr3:uid="{AD03CA40-5B78-8B41-9E4D-03DCE23E11E1}" name="Characteristics [Sample Collection Date]" dataDxfId="19"/>
-    <tableColumn id="145" xr3:uid="{6AC68041-2E25-9444-831A-05A07C9D4229}" name="Term Source REF [Sample Collection Date] (#h; #tNFDI4PSO:0000075)" dataDxfId="18"/>
-    <tableColumn id="146" xr3:uid="{7C695C41-0D47-6842-83E2-1435AFB1EF52}" name="Term Accession Number [Sample Collection Date] (#h; #tNFDI4PSO:0000075)" dataDxfId="17"/>
-    <tableColumn id="147" xr3:uid="{1F9082F2-7F61-614D-B072-F3DE7238714F}" name="Characteristics [Sample Collected By]" dataDxfId="16"/>
-    <tableColumn id="148" xr3:uid="{5F6F8541-8734-6242-A386-C4FCE4A4D156}" name="Term Source REF [Sample Collected By] (#h; #tNFDI4PSO:0000076)" dataDxfId="15"/>
-    <tableColumn id="149" xr3:uid="{36185F91-0DB8-EE4B-96A2-DF807E8CD12E}" name="Term Accession Number [Sample Collected By] (#h; #tNFDI4PSO:0000076)" dataDxfId="14"/>
-    <tableColumn id="62" xr3:uid="{12C4BED6-C71D-CC43-B976-AECFD0AF0BCF}" name="Characteristics [Time point]" dataDxfId="13"/>
-    <tableColumn id="63" xr3:uid="{D78E63DF-76E2-AE4F-A9AA-86CB096E0FD1}" name="Term Source REF [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="12"/>
-    <tableColumn id="64" xr3:uid="{4E3E838B-D518-9B41-95E4-AE65DE3C4242}" name="Term Accession Number [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="11"/>
-    <tableColumn id="75" xr3:uid="{7FBEC602-6866-EE4C-901B-A620EADE0B55}" name="Parameter [Sample Collection Method]" dataDxfId="10"/>
-    <tableColumn id="76" xr3:uid="{082E37E1-9067-2344-AFED-4C0AB2E6608F}" name="Term Source REF [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="9"/>
-    <tableColumn id="77" xr3:uid="{23CA10DE-9FDA-A94D-84CF-7C5F7143EE90}" name="Term Accession Number [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="8"/>
-    <tableColumn id="78" xr3:uid="{DD36BBD7-7DDE-4B4B-B0E7-E088C0737C72}" name="Parameter [Metabolism quenching method]" dataDxfId="7"/>
-    <tableColumn id="79" xr3:uid="{E9A2A827-A7E3-E44F-8034-982633580E8D}" name="Term Source REF [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="6"/>
-    <tableColumn id="80" xr3:uid="{ECB588C7-B9C0-8741-BE8A-1CDECCED4ED4}" name="Term Accession Number [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="5"/>
-    <tableColumn id="81" xr3:uid="{125431A9-D115-4A4B-A917-1C0A2F361D5C}" name="Parameter [Sample storage]" dataDxfId="4"/>
-    <tableColumn id="82" xr3:uid="{A56F8F05-EAAB-FD40-8F2F-AD66235065C4}" name="Term Source REF [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="3"/>
-    <tableColumn id="83" xr3:uid="{AB05BD40-EE64-3547-80D7-EDD26BB0F77A}" name="Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9B8F9057-2F20-7A45-8C27-9A36422B26D5}" name="Source Name" dataDxfId="127"/>
+    <tableColumn id="2" xr3:uid="{CC93B5FA-49F4-9B4C-B1F6-452471229F30}" name="Sample Name" dataDxfId="126"/>
+    <tableColumn id="101" xr3:uid="{AA189B85-0B08-424F-93B5-6C2D3D660371}" name="Characteristics [Sample type]" dataDxfId="125"/>
+    <tableColumn id="102" xr3:uid="{B5019B54-7F43-2042-A406-B19B1779B047}" name="Term Source REF [Sample type] (#h; #tNFDI4PSO:0000064)" dataDxfId="124"/>
+    <tableColumn id="103" xr3:uid="{10BC9619-E39D-4A45-853C-57DD06C07840}" name="Term Accession Number [Sample type] (#h; #tNFDI4PSO:0000064)" dataDxfId="123"/>
+    <tableColumn id="72" xr3:uid="{A33FCD3B-AD29-A742-9D63-6ECAFBEE068E}" name="Characteristics [Biological replicate]" dataDxfId="122"/>
+    <tableColumn id="73" xr3:uid="{4059FECC-FE9D-5947-9219-570196389DAE}" name="Term Source REF [Biological replicate] (#h; #tNFDI4PSO:0000042)" dataDxfId="121"/>
+    <tableColumn id="74" xr3:uid="{E04811ED-EF58-AD4F-84F5-156D9251E904}" name="Term Accession Number [Biological replicate] (#h; #tNFDI4PSO:0000042)" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{6A7FF2B3-5F1E-8245-AC4F-6198097A8123}" name="Characteristics [Organism]" dataDxfId="119"/>
+    <tableColumn id="4" xr3:uid="{CC831F2C-80A0-C84F-829F-23F6C78F2EEB}" name="Term Source REF [Organism] (#h; #tNFDI4PSO:0000030)" dataDxfId="118"/>
+    <tableColumn id="5" xr3:uid="{D6E59B6D-D53F-A840-A182-24AE5A460E1D}" name="Term Accession Number [Organism] (#h; #tNFDI4PSO:0000030)" dataDxfId="117"/>
+    <tableColumn id="114" xr3:uid="{DD7E5619-DB6E-F44E-B75B-1CA6BECA8011}" name="Characteristics [Isolate]" dataDxfId="116"/>
+    <tableColumn id="115" xr3:uid="{08C77E06-D2B6-CA44-AEE6-39AB1D06F432}" name="Term Source REF [Isolate] (#h; #tNFDI4PSO:0000065)" dataDxfId="115"/>
+    <tableColumn id="116" xr3:uid="{0E95421D-DECB-4248-99A3-002C66A0AEBF}" name="Term Accession Number [Isolate] (#h; #tNFDI4PSO:0000065)" dataDxfId="114"/>
+    <tableColumn id="107" xr3:uid="{CAC9E02B-4310-AC47-9C0B-C1B0925DA497}" name="Characteristics [Cultivar]" dataDxfId="113"/>
+    <tableColumn id="108" xr3:uid="{88369A2F-DDBC-7D42-9993-9C41B71C3C2F}" name="Term Source REF [Cultivar] (#h; #tNFDI4PSO:0000066)" dataDxfId="112"/>
+    <tableColumn id="109" xr3:uid="{C5014D52-D324-3246-B46B-898151F9B990}" name="Term Accession Number [Cultivar] (#h; #tNFDI4PSO:0000066)" dataDxfId="111"/>
+    <tableColumn id="110" xr3:uid="{700C615F-5CF8-8F43-8A5A-ABCBAE4EAD2E}" name="Characteristics [Ecotype]" dataDxfId="110"/>
+    <tableColumn id="111" xr3:uid="{BBBA29E7-DCD6-D342-B661-681AD683DD93}" name="Term Source REF [Ecotype] (#h; #tNFDI4PSO:0000067)" dataDxfId="109"/>
+    <tableColumn id="112" xr3:uid="{8EB5249F-48BB-634B-A2B1-ABD06733E545}" name="Term Accession Number [Ecotype] (#h; #tNFDI4PSO:0000067)" dataDxfId="108"/>
+    <tableColumn id="14" xr3:uid="{000DCCE3-5EF7-4F4E-A82A-AD088FF36730}" name="Characteristics [Genotype]" dataDxfId="107"/>
+    <tableColumn id="15" xr3:uid="{E2A1AEEB-EF2B-F448-824C-2953C18CC24A}" name="Term Source REF [Genotype] (#h; #tNFDI4PSO:0000031)" dataDxfId="106"/>
+    <tableColumn id="16" xr3:uid="{A998FE5F-8994-6E40-94FA-F0EF6DC905E4}" name="Term Accession Number [Genotype] (#h; #tNFDI4PSO:0000031)" dataDxfId="105"/>
+    <tableColumn id="117" xr3:uid="{FBA29C11-8E4B-6142-8B9C-9221A56EEA2B}" name="Characteristics [population]" dataDxfId="104"/>
+    <tableColumn id="118" xr3:uid="{B481BDF5-2297-0548-9D1D-97160F39EC7F}" name="Term Source REF [population] (#h; #tOBI:0000181)" dataDxfId="103"/>
+    <tableColumn id="119" xr3:uid="{F95C8EA9-3541-BC43-BA8C-78ED526D9471}" name="Term Accession Number [population] (#h; #tOBI:0000181)" dataDxfId="102"/>
+    <tableColumn id="17" xr3:uid="{0EB867DC-9BB4-6243-BEE9-01764D9FEB35}" name="Characteristics [Organism part]" dataDxfId="101"/>
+    <tableColumn id="18" xr3:uid="{B0CCF08F-B694-6C4F-94E6-E17AFD4C0A63}" name="Term Source REF [Organism part] (#h; #tNFDI4PSO:0000032)" dataDxfId="100"/>
+    <tableColumn id="19" xr3:uid="{6A02A31E-2B72-BE41-BF86-71E587B29D13}" name="Term Accession Number [Organism part] (#h; #tNFDI4PSO:0000032)" dataDxfId="99"/>
+    <tableColumn id="120" xr3:uid="{AD004493-349E-2948-B660-FFC9B04A3756}" name="Characteristics [Cell line]" dataDxfId="98"/>
+    <tableColumn id="121" xr3:uid="{2A484165-7392-6F45-8DA4-DB1A88B93DEC}" name="Term Source REF [Cell line] (#h; #tNFDI4PSO:0000068)" dataDxfId="97"/>
+    <tableColumn id="122" xr3:uid="{9AE3D69F-0281-4045-BFE6-C023EC048A62}" name="Term Accession Number [Cell line] (#h; #tNFDI4PSO:0000068)" dataDxfId="96"/>
+    <tableColumn id="123" xr3:uid="{B1A6199C-7EDD-564A-8155-ECC5A48569C0}" name="Characteristics [Cell type]" dataDxfId="95"/>
+    <tableColumn id="124" xr3:uid="{49433E8D-29BA-2E4F-9009-1F477D0C0EE1}" name="Term Source REF [Cell type] (#h; #tNFDI4PSO:0000069)" dataDxfId="94"/>
+    <tableColumn id="125" xr3:uid="{FC41F627-5506-0346-B969-E2BFB7E8F3BE}" name="Term Accession Number [Cell type] (#h; #tNFDI4PSO:0000069)" dataDxfId="93"/>
+    <tableColumn id="20" xr3:uid="{96C34AC4-65C0-774B-A5A0-1BC98C955028}" name="Characteristics [age]" dataDxfId="92"/>
+    <tableColumn id="21" xr3:uid="{325D3F43-A306-2F47-AD9C-92F61C0649E5}" name="Term Source REF [age] (#h; #tNFDI4PSO:0000033)" dataDxfId="91"/>
+    <tableColumn id="22" xr3:uid="{334AF647-E268-2E41-950D-8973A43E29C8}" name="Term Accession Number [age] (#h; #tNFDI4PSO:0000033)" dataDxfId="90"/>
+    <tableColumn id="126" xr3:uid="{D48EF60D-FFC4-DA42-8A84-9D7BEC94EB5C}" name="Characteristics [Developmental Stage]" dataDxfId="89"/>
+    <tableColumn id="127" xr3:uid="{B7FB233D-7D8A-A34E-91AE-3E96612329F2}" name="Term Source REF [Developmental Stage] (#h; #tNFDI4PSO:0000070)" dataDxfId="88"/>
+    <tableColumn id="128" xr3:uid="{0CFCFB6B-CC3F-A24A-B1A8-77F2863EAED6}" name="Term Accession Number [Developmental Stage] (#h; #tNFDI4PSO:0000070)" dataDxfId="87"/>
+    <tableColumn id="129" xr3:uid="{A1014B91-8574-664B-A628-2DDC01083E67}" name="Characteristics [Plant disease]" dataDxfId="86"/>
+    <tableColumn id="130" xr3:uid="{CF451DD4-AB45-1144-8BBF-C2C23EAE7EBC}" name="Term Source REF [Plant disease] (#h; #tNFDI4PSO:0000071)" dataDxfId="85"/>
+    <tableColumn id="131" xr3:uid="{4A90236E-F6AF-BE44-8703-08F06FE96AF5}" name="Term Accession Number [Plant disease] (#h; #tNFDI4PSO:0000071)" dataDxfId="84"/>
+    <tableColumn id="132" xr3:uid="{1F37D0D2-6260-584B-9CC0-9A72C472F841}" name="Characteristics [Plant disease stage]" dataDxfId="83"/>
+    <tableColumn id="133" xr3:uid="{2348DA4F-92E0-8547-AA7D-FCB641272A62}" name="Term Source REF [Plant disease stage] (#h; #tNFDI4PSO:0000072)" dataDxfId="82"/>
+    <tableColumn id="134" xr3:uid="{76B2929E-FEFA-C94A-9351-B07EA87DB902}" name="Term Accession Number [Plant disease stage] (#h; #tNFDI4PSO:0000072)" dataDxfId="81"/>
+    <tableColumn id="135" xr3:uid="{BEBD2093-9306-0C42-AFAE-735502002BE7}" name="Characteristics [Phenotype]" dataDxfId="80"/>
+    <tableColumn id="136" xr3:uid="{109579A2-3212-484D-A514-9571CF9305C5}" name="Term Source REF [Phenotype] (#h; #tNFDI4PSO:0000073)" dataDxfId="79"/>
+    <tableColumn id="137" xr3:uid="{77978229-5807-DE4F-A777-C5E343D79A55}" name="Term Accession Number [Phenotype] (#h; #tNFDI4PSO:0000073)" dataDxfId="78"/>
+    <tableColumn id="138" xr3:uid="{65D76AFE-F9A3-544C-B9C1-4D6C71488C92}" name="Characteristics [whole plant size]" dataDxfId="77"/>
+    <tableColumn id="139" xr3:uid="{91B73049-DC8D-D94B-8B5F-76E283D04557}" name="Term Source REF [whole plant size] (#h; #tTO:1000012)" dataDxfId="76"/>
+    <tableColumn id="140" xr3:uid="{6FB79EF4-9E54-8D45-BB9F-CE997665B054}" name="Term Accession Number [whole plant size] (#h; #tTO:1000012)" dataDxfId="75"/>
+    <tableColumn id="26" xr3:uid="{5E219BCA-059A-CC41-93BF-8CD61AA9572D}" name="Characteristics [study type]" dataDxfId="74"/>
+    <tableColumn id="27" xr3:uid="{5FF2BBBF-350F-9842-8FDF-2F895B07EADF}" name="Term Source REF [study type] (#h; #tPECO:0007231)" dataDxfId="73"/>
+    <tableColumn id="28" xr3:uid="{E12790EC-754D-3244-8A7A-1242F7942612}" name="Term Accession Number [study type] (#h; #tPECO:0007231)" dataDxfId="72"/>
+    <tableColumn id="23" xr3:uid="{E0A293FE-1EF5-A949-9C12-ADF40314B418}" name="Characteristics [plant growth medium exposure]" dataDxfId="71"/>
+    <tableColumn id="24" xr3:uid="{0C19F4A6-F9E8-1F4F-9B61-EB31E6DF451A}" name="Term Source REF [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="70"/>
+    <tableColumn id="25" xr3:uid="{7BBED07D-F814-A245-B090-723342B3D631}" name="Term Accession Number [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="69"/>
+    <tableColumn id="29" xr3:uid="{C386EF1A-F4F8-C543-99A0-ABD311BD175F}" name="Characteristics [growth plot design]" dataDxfId="68"/>
+    <tableColumn id="30" xr3:uid="{86FAE20B-4F89-EE4F-91E6-CE3B7E712F95}" name="Term Source REF [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="67"/>
+    <tableColumn id="31" xr3:uid="{C0949892-595C-9742-BCD1-75134FAC012F}" name="Term Accession Number [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="66"/>
+    <tableColumn id="32" xr3:uid="{B90A4652-69D5-2E4F-8A64-A3A5A5CB24DB}" name="Characteristics [Growth day length]" dataDxfId="65"/>
+    <tableColumn id="33" xr3:uid="{4E2448E1-3D08-504C-8FE3-D71B801F4DC9}" name="Term Source REF [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="64"/>
+    <tableColumn id="34" xr3:uid="{D47410BE-0000-B648-8CE5-966EE8968909}" name="Term Accession Number [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="63"/>
+    <tableColumn id="35" xr3:uid="{27034924-8879-044A-819B-7DC832A9D603}" name="Characteristics [light intensity exposure]" dataDxfId="62"/>
+    <tableColumn id="36" xr3:uid="{FD04748E-7F58-4A46-A167-E5EB1375A50B}" name="Term Source REF [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="61"/>
+    <tableColumn id="37" xr3:uid="{D76E6422-DF20-B94A-B5A6-4FD7F7923EBF}" name="Term Accession Number [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{8E446DD1-817A-E84A-9536-47B88B72BFD8}" name="Unit [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{BCB29467-6D87-F141-98A0-60243765731F}" name="Term Source REF [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{D2565EAD-7C86-C343-800D-E37FD463093B}" name="Term Accession Number [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="57"/>
+    <tableColumn id="38" xr3:uid="{21746D48-E9A2-5B42-BC00-F5AFD4793AA7}" name="Characteristics [Humidity Day]" dataDxfId="56"/>
+    <tableColumn id="39" xr3:uid="{8B1D9CC4-6026-674C-9852-06A06365907B}" name="Term Source REF [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="55"/>
+    <tableColumn id="40" xr3:uid="{8CCA0026-8267-884E-8F9A-369ACCB825EA}" name="Term Accession Number [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{9508FD23-5388-F64E-8286-05B533856CA2}" name="Unit [percent] (#h; #tUO:0000187; #u)" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{F796BC22-CBE1-6D41-824E-F655C3F9D5B6}" name="Term Source REF [percent] (#h; #tUO:0000187; #u)" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{32AC3DD8-82CD-4349-BFD5-0805A34144D8}" name="Term Accession Number [percent] (#h; #tUO:0000187; #u)" dataDxfId="51"/>
+    <tableColumn id="41" xr3:uid="{F4E42B79-6B62-E34C-95BE-8906E80BFBC8}" name="Characteristics [Humidity Night]" dataDxfId="50"/>
+    <tableColumn id="42" xr3:uid="{FE26FC08-E3D1-7547-8E20-1363EF47EE86}" name="Term Source REF [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="49"/>
+    <tableColumn id="43" xr3:uid="{C6D20AF0-60A8-874E-9614-2A2F483EB262}" name="Term Accession Number [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="48"/>
+    <tableColumn id="12" xr3:uid="{2866C2CF-81B3-694E-B2D9-F69059F54AA2}" name="Unit [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="47"/>
+    <tableColumn id="13" xr3:uid="{A885FE47-7729-3B45-B73D-03FF1F114CD5}" name="Term Source REF [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="46"/>
+    <tableColumn id="65" xr3:uid="{A3AEBB25-5500-F249-866E-C98439259F17}" name="Term Accession Number [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="45"/>
+    <tableColumn id="44" xr3:uid="{F0571376-132B-F940-9609-6B59D9845B1B}" name="Characteristics [Temperature Day]" dataDxfId="44"/>
+    <tableColumn id="45" xr3:uid="{23233498-CFC4-9F46-94D5-39E7A6B5AFB5}" name="Term Source REF [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="43"/>
+    <tableColumn id="46" xr3:uid="{346D483D-D0DE-5140-A015-4AD0367BAD4D}" name="Term Accession Number [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="42"/>
+    <tableColumn id="66" xr3:uid="{57808D06-1B53-8D41-BEB4-1644A20F7763}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="41"/>
+    <tableColumn id="67" xr3:uid="{A7356A0D-0EFD-3D44-9B2F-4566273E79E8}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="40"/>
+    <tableColumn id="68" xr3:uid="{AD21FFE5-445B-CB42-B199-FDD8BAD5635D}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="39"/>
+    <tableColumn id="47" xr3:uid="{2AB78931-B301-314A-9311-2CC2C21128D4}" name="Characteristics [Temperature Night]" dataDxfId="38"/>
+    <tableColumn id="48" xr3:uid="{3A76D4EC-C74F-0A4B-B340-8EF3D8B86ECB}" name="Term Source REF [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="37"/>
+    <tableColumn id="49" xr3:uid="{87034985-F2AC-A145-AA6A-9EDB63F919F9}" name="Term Accession Number [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="36"/>
+    <tableColumn id="69" xr3:uid="{6D54D968-A087-944D-BF64-3AC3D5B08F80}" name="Unit [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="35"/>
+    <tableColumn id="70" xr3:uid="{AE04B49D-BF47-F34B-B52A-752ECD10B8C7}" name="Term Source REF [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="34"/>
+    <tableColumn id="71" xr3:uid="{2A40040A-D450-EF49-AB82-0CEEB3D8A599}" name="Term Accession Number [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="33"/>
+    <tableColumn id="50" xr3:uid="{FC29A38A-1769-7349-A9E5-A5184C62F33A}" name="Characteristics [watering exposure]" dataDxfId="32"/>
+    <tableColumn id="51" xr3:uid="{808AA82E-ECE0-AD47-92D3-27D7C93007B7}" name="Term Source REF [watering exposure] (#h; #tPECO:0007383)" dataDxfId="31"/>
+    <tableColumn id="52" xr3:uid="{7C45B5F9-759B-E646-A40E-CB5363DF17A8}" name="Term Accession Number [watering exposure] (#h; #tPECO:0007383)" dataDxfId="30"/>
+    <tableColumn id="53" xr3:uid="{70DF5752-BECA-5342-9001-FA7F5271BC54}" name="Characteristics [plant nutrient exposure]" dataDxfId="29"/>
+    <tableColumn id="54" xr3:uid="{FD6AD7C0-D253-D04C-8B67-6124B6C5D685}" name="Term Source REF [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="28"/>
+    <tableColumn id="55" xr3:uid="{95BC5752-0FFE-8C4E-BFE3-4FED8B72A648}" name="Term Accession Number [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="27"/>
+    <tableColumn id="56" xr3:uid="{25540F7D-0E49-F74B-8EF6-6E2314EBD1B1}" name="Characteristics [abiotic plant exposure]" dataDxfId="26"/>
+    <tableColumn id="57" xr3:uid="{19EC9032-1152-F940-ADB1-397E054EED4E}" name="Term Source REF [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="25"/>
+    <tableColumn id="58" xr3:uid="{40EA0154-215C-C44C-A5D6-852F5DA9A25C}" name="Term Accession Number [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="24"/>
+    <tableColumn id="59" xr3:uid="{C208C009-B835-0041-9A5C-978B7EABB59C}" name="Characteristics [biotic plant exposure]" dataDxfId="23"/>
+    <tableColumn id="60" xr3:uid="{2836636A-01C7-9C4E-9B41-EE6FEE3D7B80}" name="Term Source REF [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="22"/>
+    <tableColumn id="61" xr3:uid="{E4A74FCF-2E01-354A-99CE-0602774F8706}" name="Term Accession Number [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="21"/>
+    <tableColumn id="141" xr3:uid="{76BC0B00-263D-ED4F-A9A2-143148146694}" name="Characteristics [Geographic Area]" dataDxfId="20"/>
+    <tableColumn id="142" xr3:uid="{752BC19A-0C01-7F45-9374-DD0350C7B0D8}" name="Term Source REF [Geogaphic Area] (#h; #tNFDI4PSO:0000074)" dataDxfId="19"/>
+    <tableColumn id="143" xr3:uid="{5E52848A-36B7-4E4F-B77F-EFA6EC9BD00B}" name="Term Accession Number [Geogaphic Area] (#h; #tNFDI4PSO:0000074)" dataDxfId="18"/>
+    <tableColumn id="144" xr3:uid="{AD03CA40-5B78-8B41-9E4D-03DCE23E11E1}" name="Characteristics [Sample Collection Date]" dataDxfId="17"/>
+    <tableColumn id="145" xr3:uid="{6AC68041-2E25-9444-831A-05A07C9D4229}" name="Term Source REF [Sample Collection Date] (#h; #tNFDI4PSO:0000075)" dataDxfId="16"/>
+    <tableColumn id="146" xr3:uid="{7C695C41-0D47-6842-83E2-1435AFB1EF52}" name="Term Accession Number [Sample Collection Date] (#h; #tNFDI4PSO:0000075)" dataDxfId="15"/>
+    <tableColumn id="147" xr3:uid="{1F9082F2-7F61-614D-B072-F3DE7238714F}" name="Characteristics [Sample Collected By]" dataDxfId="14"/>
+    <tableColumn id="148" xr3:uid="{5F6F8541-8734-6242-A386-C4FCE4A4D156}" name="Term Source REF [Sample Collected By] (#h; #tNFDI4PSO:0000076)" dataDxfId="13"/>
+    <tableColumn id="149" xr3:uid="{36185F91-0DB8-EE4B-96A2-DF807E8CD12E}" name="Term Accession Number [Sample Collected By] (#h; #tNFDI4PSO:0000076)" dataDxfId="12"/>
+    <tableColumn id="62" xr3:uid="{12C4BED6-C71D-CC43-B976-AECFD0AF0BCF}" name="Characteristics [Time point]" dataDxfId="11"/>
+    <tableColumn id="63" xr3:uid="{D78E63DF-76E2-AE4F-A9AA-86CB096E0FD1}" name="Term Source REF [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="10"/>
+    <tableColumn id="64" xr3:uid="{4E3E838B-D518-9B41-95E4-AE65DE3C4242}" name="Term Accession Number [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="9"/>
+    <tableColumn id="75" xr3:uid="{7FBEC602-6866-EE4C-901B-A620EADE0B55}" name="Parameter [Sample Collection Method]" dataDxfId="8"/>
+    <tableColumn id="76" xr3:uid="{082E37E1-9067-2344-AFED-4C0AB2E6608F}" name="Term Source REF [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="7"/>
+    <tableColumn id="77" xr3:uid="{23CA10DE-9FDA-A94D-84CF-7C5F7143EE90}" name="Term Accession Number [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="6"/>
+    <tableColumn id="78" xr3:uid="{DD36BBD7-7DDE-4B4B-B0E7-E088C0737C72}" name="Parameter [Metabolism quenching method]" dataDxfId="5"/>
+    <tableColumn id="79" xr3:uid="{E9A2A827-A7E3-E44F-8034-982633580E8D}" name="Term Source REF [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="4"/>
+    <tableColumn id="80" xr3:uid="{ECB588C7-B9C0-8741-BE8A-1CDECCED4ED4}" name="Term Accession Number [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="3"/>
+    <tableColumn id="81" xr3:uid="{125431A9-D115-4A4B-A917-1C0A2F361D5C}" name="Parameter [Sample storage]" dataDxfId="2"/>
+    <tableColumn id="82" xr3:uid="{A56F8F05-EAAB-FD40-8F2F-AD66235065C4}" name="Term Source REF [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="1"/>
+    <tableColumn id="83" xr3:uid="{AB05BD40-EE64-3547-80D7-EDD26BB0F77A}" name="Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3569,7 +3563,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="729" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -3594,7 +3588,7 @@
       <pane xSplit="3" ySplit="22" topLeftCell="D41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="D48" sqref="D48"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.5" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12326,11 +12320,11 @@
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <customXml>
   <SwateTable Table="annotationTable" Worksheet="1SPL01_plants">
-    <TableValidation DateTime="2021-04-29 14:10" SwateVersion="0.4.0" TableName="annotationTable" Userlist="" WorksheetName="1SPL01_plants">
-      <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="None" Unit="None" ValidationFormat="None"/>
-      <ColumnValidation ColumnAdress="1" ColumnHeader="Sample Name" Importance="None" Unit="None" ValidationFormat="None"/>
-      <ColumnValidation ColumnAdress="2" ColumnHeader="Characteristics [Sample type]" Importance="None" Unit="None" ValidationFormat="None"/>
-      <ColumnValidation ColumnAdress="5" ColumnHeader="Characteristics [Biological replicate]" Importance="3" Unit="None" ValidationFormat="None"/>
+    <TableValidation DateTime="2021-08-06 11:46" SwateVersion="0.4.7" TableName="annotationTable" Userlist="" WorksheetName="1SPL01_plants">
+      <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="None" Unit="None" ValidationFormat="Text"/>
+      <ColumnValidation ColumnAdress="1" ColumnHeader="Sample Name" Importance="None" Unit="None" ValidationFormat="Text"/>
+      <ColumnValidation ColumnAdress="2" ColumnHeader="Characteristics [Sample type]" Importance="None" Unit="None" ValidationFormat="OntologyTerm Sample type"/>
+      <ColumnValidation ColumnAdress="5" ColumnHeader="Characteristics [Biological replicate]" Importance="3" Unit="None" ValidationFormat="Int"/>
       <ColumnValidation ColumnAdress="8" ColumnHeader="Characteristics [Organism]" Importance="4" Unit="None" ValidationFormat="OntologyTerm Organism"/>
       <ColumnValidation ColumnAdress="11" ColumnHeader="Characteristics [Isolate]" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="14" ColumnHeader="Characteristics [Cultivar]" Importance="None" Unit="None" ValidationFormat="None"/>
@@ -12359,7 +12353,7 @@
       <ColumnValidation ColumnAdress="98" ColumnHeader="Characteristics [plant nutrient exposure]" Importance="4" Unit="None" ValidationFormat="OntologyTerm plant nutrient exposure"/>
       <ColumnValidation ColumnAdress="101" ColumnHeader="Characteristics [abiotic plant exposure]" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="104" ColumnHeader="Characteristics [biotic plant exposure]" Importance="None" Unit="None" ValidationFormat="None"/>
-      <ColumnValidation ColumnAdress="107" ColumnHeader="Characteristics [Geogaphic Area]" Importance="5" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="107" ColumnHeader="Characteristics [Geographic Area]" Importance="5" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="110" ColumnHeader="Characteristics [Sample Collection Date]" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="113" ColumnHeader="Characteristics [Sample Collected By]" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="116" ColumnHeader="Characteristics [Time point]" Importance="None" Unit="None" ValidationFormat="None"/>
@@ -12372,7 +12366,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32232BCB-4AA3-0D49-B180-4BB43230D66C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DD0D14F-19F8-4F51-9987-EE16A8E11E60}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
checked semantics and minor edits
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants/1SPL01_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/MetadataTemplates/SWATE_templates/templates/1SPL01_plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E5B9E0-B47D-C840-93E1-9209F1B25173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D515BF9-2A7C-4C40-8787-852C75A05F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="399">
   <si>
     <t>Source Name</t>
   </si>
@@ -1343,6 +1343,9 @@
   </si>
   <si>
     <t>Use to specify subclasses of existing terms</t>
+  </si>
+  <si>
+    <t>ER Additional information</t>
   </si>
 </sst>
 </file>
@@ -3386,7 +3389,7 @@
       <pane xSplit="3" ySplit="24" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.5" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9400,7 +9403,7 @@
         <v>175</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>173</v>
+        <v>398</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>332</v>

</xml_diff>

<commit_message>
Add MetadataSheet to all Templates
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants/1SPL01_plants.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\1SPL01_plants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA3E311-818C-48D9-9366-B7DD679EFE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB4B273-BEEE-47AD-B027-D5FA45069516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D1671A6-E5E6-4E90-817E-C23847CD9BD1}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="1" r:id="rId1"/>
+    <sheet name="SwateTemplateMetadata" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,8 +34,28 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={A6730C41-F5DE-4F01-A3FC-095AF4373E4D}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A6730C41-F5DE-4F01-A3FC-095AF4373E4D}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    The unique identifier of this template. It will be auto generated.
+Antwort:
+    id=f12e98ee-a4e7-4ada-ba56-1e13cce1a44b</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="164">
   <si>
     <t>Source Name</t>
   </si>
@@ -389,6 +409,144 @@
   </si>
   <si>
     <t>Characteristics [Time point]</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Docslink</t>
+  </si>
+  <si>
+    <t>Organisation</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>#ER list</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>ER Term Accession Number</t>
+  </si>
+  <si>
+    <t>ER Term Source REF</t>
+  </si>
+  <si>
+    <t>#TAGS list</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Tags Term Accession Number</t>
+  </si>
+  <si>
+    <t>Tags Term Source REF</t>
+  </si>
+  <si>
+    <t>#AUTHORS list</t>
+  </si>
+  <si>
+    <t>Authors Last Name</t>
+  </si>
+  <si>
+    <t>Authors First Name</t>
+  </si>
+  <si>
+    <t>Authors Mid Initials</t>
+  </si>
+  <si>
+    <t>Authors Email</t>
+  </si>
+  <si>
+    <t>Authors Phone</t>
+  </si>
+  <si>
+    <t>Authors Fax</t>
+  </si>
+  <si>
+    <t>Authors Address</t>
+  </si>
+  <si>
+    <t>Authors Affiliation</t>
+  </si>
+  <si>
+    <t>#AUTHORS ROLES list</t>
+  </si>
+  <si>
+    <t>Authors Roles</t>
+  </si>
+  <si>
+    <t>Authors Roles Term Accession Number</t>
+  </si>
+  <si>
+    <t>Authors Roles Term Source REF</t>
+  </si>
+  <si>
+    <t>f12e98ee-a4e7-4ada-ba56-1e13cce1a44b</t>
+  </si>
+  <si>
+    <t>Plant growth</t>
+  </si>
+  <si>
+    <t>Template to describe a plant growth study as well as sample collection and handling.</t>
+  </si>
+  <si>
+    <t>GEO</t>
+  </si>
+  <si>
+    <t>METABOLIGHTS</t>
+  </si>
+  <si>
+    <t>PRIDE</t>
+  </si>
+  <si>
+    <t>BIOSAMPLE</t>
+  </si>
+  <si>
+    <t>Plants</t>
+  </si>
+  <si>
+    <t>Sampling</t>
+  </si>
+  <si>
+    <t>Plant study</t>
+  </si>
+  <si>
+    <t>Jabeen</t>
+  </si>
+  <si>
+    <t>Brilhaus</t>
+  </si>
+  <si>
+    <t>Maus</t>
+  </si>
+  <si>
+    <t>Hajira</t>
+  </si>
+  <si>
+    <t>Dominik</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>annotationTableUnluckyVampirebat89</t>
+  </si>
+  <si>
+    <t>1.1.6</t>
   </si>
 </sst>
 </file>
@@ -400,7 +558,7 @@
     <numFmt numFmtId="165" formatCode="0.00\ &quot;percent&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,19 +566,121 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFF5F5F5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF217346"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0E5C2F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC21F3A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FCDB3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFEFEFE"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFEFEFE"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFEFEFE"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFEFEFE"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFEFEFE"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFEFEFE"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFEFEFE"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFEFEFE"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFEFEFE"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFEFEFE"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFEFEFE"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFEFEFE"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFEFEFE"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFEFEFE"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -429,11 +689,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -491,6 +781,78 @@
       <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="0.00\ &quot;percent&quot;"/>
     </dxf>
     <dxf>
@@ -525,78 +887,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00\ &quot;microeinstein per square meter per second&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree Celsius&quot;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -609,6 +899,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Oliver Maus" id="{BFA4ADC4-8771-41AF-BD0E-9E56E7CC4977}" userId="Oliver Maus" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -679,59 +975,59 @@
     <tableColumn id="51" xr3:uid="{2D525B40-3237-4017-98F0-27AD5E830BF7}" name="Characteristics [Growth day length]"/>
     <tableColumn id="52" xr3:uid="{A55C0CA4-8AE0-49C3-A41C-3AE50E40758A}" name="Term Source REF (NFDI4PSO:0000041)"/>
     <tableColumn id="53" xr3:uid="{1477EDD7-1DCB-4770-BA05-F1CC0EFA9AD5}" name="Term Accession Number (NFDI4PSO:0000041)"/>
-    <tableColumn id="135" xr3:uid="{85247456-E764-4D3E-BF93-12E412A41198}" name="Characteristics [light intensity exposure]" dataDxfId="28"/>
-    <tableColumn id="136" xr3:uid="{93A50CDC-1E60-4366-AB54-D4E7EE771BBF}" name="Unit" dataDxfId="27"/>
-    <tableColumn id="137" xr3:uid="{23F71F80-EA30-4D98-9A5D-F47C1E28CA7D}" name="Term Source REF (PECO:0007224)" dataDxfId="26"/>
-    <tableColumn id="138" xr3:uid="{C7FAED94-6AB6-4857-B12A-3D43248B98D9}" name="Term Accession Number (PECO:0007224)" dataDxfId="25"/>
-    <tableColumn id="139" xr3:uid="{C3243056-CD27-4381-8490-101CEDC788A9}" name="Characteristics [Humidity Day]" dataDxfId="24"/>
-    <tableColumn id="140" xr3:uid="{1859E1B1-1EAC-418E-BACC-2BB44F677FFE}" name="Unit (#2)" dataDxfId="23"/>
-    <tableColumn id="141" xr3:uid="{798016FD-2838-4531-9398-3279D6A08C58}" name="Term Source REF (NFDI4PSO:0000005)" dataDxfId="22"/>
-    <tableColumn id="142" xr3:uid="{DA5B416D-F4A5-4D4E-8C25-A2ED3C4C82D4}" name="Term Accession Number (NFDI4PSO:0000005)" dataDxfId="21"/>
-    <tableColumn id="143" xr3:uid="{CFD14F66-5E52-44A1-8428-78197BFDC3B7}" name="Characteristics [Humidity Night]" dataDxfId="20"/>
-    <tableColumn id="144" xr3:uid="{CAB23864-751E-4921-B093-E7F5F36CAB4A}" name="Unit (#3)" dataDxfId="19"/>
-    <tableColumn id="145" xr3:uid="{C79AD268-C4B2-49CA-AC34-43CF8297D031}" name="Term Source REF (NFDI4PSO:0000006)" dataDxfId="18"/>
-    <tableColumn id="146" xr3:uid="{62B5FED7-2365-42A3-9552-8A0FA76E9908}" name="Term Accession Number (NFDI4PSO:0000006)" dataDxfId="17"/>
-    <tableColumn id="147" xr3:uid="{97BBD5E2-CDBA-451A-B789-7CF61859FFCB}" name="Characteristics [Temperature Day]" dataDxfId="16"/>
-    <tableColumn id="148" xr3:uid="{1C080C4C-851A-4E7C-896C-124F4716BA8C}" name="Unit (#4)" dataDxfId="15"/>
-    <tableColumn id="149" xr3:uid="{11E152AF-B6D8-46FF-B4D5-EC76EE12832C}" name="Term Source REF (NFDI4PSO:0000007)" dataDxfId="14"/>
-    <tableColumn id="150" xr3:uid="{FA942BE5-5F5A-4091-B5F2-EA84CB5A7C27}" name="Term Accession Number (NFDI4PSO:0000007)" dataDxfId="13"/>
-    <tableColumn id="151" xr3:uid="{6408990A-DF70-48CB-B8A8-528E0DD3D4F7}" name="Characteristics [Temperature Night]" dataDxfId="12"/>
-    <tableColumn id="152" xr3:uid="{7F17C2AE-76E7-4343-9112-49EADE039C2E}" name="Unit (#5)" dataDxfId="11"/>
-    <tableColumn id="153" xr3:uid="{A0CCAF50-1E7F-4ECE-B83C-CF1AFBBF54E2}" name="Term Source REF (NFDI4PSO:0000008)" dataDxfId="10"/>
-    <tableColumn id="154" xr3:uid="{9E0149D4-5109-4383-99E6-4D9EE5914487}" name="Term Accession Number (NFDI4PSO:0000008)" dataDxfId="9"/>
-    <tableColumn id="155" xr3:uid="{0D428223-9C3F-4A3F-ABC9-B6497EC9F4C7}" name="Characteristics [watering exposure]" dataDxfId="8"/>
-    <tableColumn id="156" xr3:uid="{0A90F49E-9F46-4E82-B592-5446DD648569}" name="Term Source REF (PECO:0007383)" dataDxfId="7"/>
-    <tableColumn id="157" xr3:uid="{6216E053-90BE-49F8-9C0C-7A6470F6D3DE}" name="Term Accession Number (PECO:0007383)" dataDxfId="6"/>
-    <tableColumn id="158" xr3:uid="{1ACB13C6-536F-41C7-91F2-B62AEB2DA8A4}" name="Characteristics [plant nutrient exposure]" dataDxfId="5"/>
-    <tableColumn id="159" xr3:uid="{97FEA8C0-4955-47E8-8E42-EFE66F8E2530}" name="Term Source REF (PECO:0007241)" dataDxfId="4"/>
-    <tableColumn id="160" xr3:uid="{159271F8-4343-4546-81D3-E7AE0438BF91}" name="Term Accession Number (PECO:0007241)" dataDxfId="3"/>
-    <tableColumn id="161" xr3:uid="{AC98601D-DB44-45A0-9639-848DD3D97821}" name="Characteristics [abiotic plant exposure]" dataDxfId="2"/>
-    <tableColumn id="162" xr3:uid="{1EF71984-AE79-45A3-B85C-3D63B9A45000}" name="Term Source REF (PECO:0007191)" dataDxfId="1"/>
-    <tableColumn id="163" xr3:uid="{58575740-B787-4889-B047-BE8097574A83}" name="Term Accession Number (PECO:0007191)" dataDxfId="0"/>
-    <tableColumn id="99" xr3:uid="{0AD23E00-4026-4DE6-9B26-1D80067F6D23}" name="Characteristics [biotic plant exposure]" dataDxfId="52"/>
-    <tableColumn id="100" xr3:uid="{A73EA20C-30F6-4F5A-BE9C-1F95EDAD2075}" name="Term Source REF (PECO:0007357)" dataDxfId="51"/>
-    <tableColumn id="101" xr3:uid="{7BC176DE-D288-440D-AE07-B17C6C087D41}" name="Term Accession Number (PECO:0007357)" dataDxfId="50"/>
-    <tableColumn id="102" xr3:uid="{E4B7F22F-69B7-45D9-A3CD-B8F269AFECB1}" name="Characteristics [Geogaphic Area]" dataDxfId="49"/>
-    <tableColumn id="103" xr3:uid="{571169D2-47B6-40AA-8E2B-8629455DE18E}" name="Term Source REF (NFDI4PSO:0000074)" dataDxfId="48"/>
-    <tableColumn id="104" xr3:uid="{B601805D-FC55-4818-BE56-E15EAC614D1A}" name="Term Accession Number (NFDI4PSO:0000074)" dataDxfId="47"/>
-    <tableColumn id="105" xr3:uid="{820EF1CB-22B2-4D90-A62E-60758945BF10}" name="Characteristics [Sample Collection Date]" dataDxfId="46"/>
-    <tableColumn id="106" xr3:uid="{20297405-2B24-48CF-B8F1-5C8FD0C57F7C}" name="Term Source REF (NFDI4PSO:0000075)" dataDxfId="45"/>
-    <tableColumn id="107" xr3:uid="{3D2321BF-EE54-4E22-8362-620DB8FCDC80}" name="Term Accession Number (NFDI4PSO:0000075)" dataDxfId="44"/>
-    <tableColumn id="108" xr3:uid="{7C136999-9BAF-43E5-855D-D97F492175D8}" name="Characteristics [Sample Collected By]" dataDxfId="43"/>
-    <tableColumn id="109" xr3:uid="{CDD0FBA0-5918-486C-BB4F-FBA37D34F559}" name="Term Source REF (NFDI4PSO:0000076)" dataDxfId="42"/>
-    <tableColumn id="110" xr3:uid="{9EEEA931-289F-4558-A4CD-BAA5A89EDBCB}" name="Term Accession Number (NFDI4PSO:0000076)" dataDxfId="41"/>
-    <tableColumn id="111" xr3:uid="{D539A2BF-683E-4EB0-A3FA-26F36AB2D491}" name="Characteristics [Time point]" dataDxfId="40"/>
-    <tableColumn id="112" xr3:uid="{67D48280-3922-4AE2-A629-EAEB3D5641B8}" name="Term Source REF (NFDI4PSO:0000034)" dataDxfId="39"/>
-    <tableColumn id="113" xr3:uid="{615E7959-5992-4D06-8A7B-DD39B89C4EEC}" name="Term Accession Number (NFDI4PSO:0000034)" dataDxfId="38"/>
-    <tableColumn id="114" xr3:uid="{4D9D42EB-53DB-46E9-AC66-722486F5B239}" name="Parameter [Sample Collection Method]" dataDxfId="37"/>
-    <tableColumn id="115" xr3:uid="{13DC542E-9758-4841-8D94-D7C3116C0568}" name="Term Source REF (NFDI4PSO:0000009)" dataDxfId="36"/>
-    <tableColumn id="116" xr3:uid="{36345937-CA63-443C-9D9D-BD0EAAAF7812}" name="Term Accession Number (NFDI4PSO:0000009)" dataDxfId="35"/>
-    <tableColumn id="117" xr3:uid="{05864A64-95DE-44E0-8966-107156CE7021}" name="Parameter [Metabolism quenching method]" dataDxfId="34"/>
-    <tableColumn id="118" xr3:uid="{3D7DB003-4188-49D2-94CA-D993FAD9E4F0}" name="Term Source REF (NFDI4PSO:0000010)" dataDxfId="33"/>
-    <tableColumn id="119" xr3:uid="{786911B1-BB7C-4948-A507-1360E791FD32}" name="Term Accession Number (NFDI4PSO:0000010)" dataDxfId="32"/>
-    <tableColumn id="120" xr3:uid="{9ACB2720-1CAC-4E92-BC80-C750A5BB4732}" name="Parameter [Sample storage]" dataDxfId="31"/>
-    <tableColumn id="121" xr3:uid="{F17CF920-3ACC-4E28-BDDF-4EAB2A03C00F}" name="Term Source REF (NFDI4PSO:0000011)" dataDxfId="30"/>
-    <tableColumn id="122" xr3:uid="{89F0B1DF-DB89-45C5-91DE-1DD5DA8F371D}" name="Term Accession Number (NFDI4PSO:0000011)" dataDxfId="29"/>
+    <tableColumn id="135" xr3:uid="{85247456-E764-4D3E-BF93-12E412A41198}" name="Characteristics [light intensity exposure]" dataDxfId="52"/>
+    <tableColumn id="136" xr3:uid="{93A50CDC-1E60-4366-AB54-D4E7EE771BBF}" name="Unit" dataDxfId="51"/>
+    <tableColumn id="137" xr3:uid="{23F71F80-EA30-4D98-9A5D-F47C1E28CA7D}" name="Term Source REF (PECO:0007224)" dataDxfId="50"/>
+    <tableColumn id="138" xr3:uid="{C7FAED94-6AB6-4857-B12A-3D43248B98D9}" name="Term Accession Number (PECO:0007224)" dataDxfId="49"/>
+    <tableColumn id="139" xr3:uid="{C3243056-CD27-4381-8490-101CEDC788A9}" name="Characteristics [Humidity Day]" dataDxfId="48"/>
+    <tableColumn id="140" xr3:uid="{1859E1B1-1EAC-418E-BACC-2BB44F677FFE}" name="Unit (#2)" dataDxfId="47"/>
+    <tableColumn id="141" xr3:uid="{798016FD-2838-4531-9398-3279D6A08C58}" name="Term Source REF (NFDI4PSO:0000005)" dataDxfId="46"/>
+    <tableColumn id="142" xr3:uid="{DA5B416D-F4A5-4D4E-8C25-A2ED3C4C82D4}" name="Term Accession Number (NFDI4PSO:0000005)" dataDxfId="45"/>
+    <tableColumn id="143" xr3:uid="{CFD14F66-5E52-44A1-8428-78197BFDC3B7}" name="Characteristics [Humidity Night]" dataDxfId="44"/>
+    <tableColumn id="144" xr3:uid="{CAB23864-751E-4921-B093-E7F5F36CAB4A}" name="Unit (#3)" dataDxfId="43"/>
+    <tableColumn id="145" xr3:uid="{C79AD268-C4B2-49CA-AC34-43CF8297D031}" name="Term Source REF (NFDI4PSO:0000006)" dataDxfId="42"/>
+    <tableColumn id="146" xr3:uid="{62B5FED7-2365-42A3-9552-8A0FA76E9908}" name="Term Accession Number (NFDI4PSO:0000006)" dataDxfId="41"/>
+    <tableColumn id="147" xr3:uid="{97BBD5E2-CDBA-451A-B789-7CF61859FFCB}" name="Characteristics [Temperature Day]" dataDxfId="40"/>
+    <tableColumn id="148" xr3:uid="{1C080C4C-851A-4E7C-896C-124F4716BA8C}" name="Unit (#4)" dataDxfId="39"/>
+    <tableColumn id="149" xr3:uid="{11E152AF-B6D8-46FF-B4D5-EC76EE12832C}" name="Term Source REF (NFDI4PSO:0000007)" dataDxfId="38"/>
+    <tableColumn id="150" xr3:uid="{FA942BE5-5F5A-4091-B5F2-EA84CB5A7C27}" name="Term Accession Number (NFDI4PSO:0000007)" dataDxfId="37"/>
+    <tableColumn id="151" xr3:uid="{6408990A-DF70-48CB-B8A8-528E0DD3D4F7}" name="Characteristics [Temperature Night]" dataDxfId="36"/>
+    <tableColumn id="152" xr3:uid="{7F17C2AE-76E7-4343-9112-49EADE039C2E}" name="Unit (#5)" dataDxfId="35"/>
+    <tableColumn id="153" xr3:uid="{A0CCAF50-1E7F-4ECE-B83C-CF1AFBBF54E2}" name="Term Source REF (NFDI4PSO:0000008)" dataDxfId="34"/>
+    <tableColumn id="154" xr3:uid="{9E0149D4-5109-4383-99E6-4D9EE5914487}" name="Term Accession Number (NFDI4PSO:0000008)" dataDxfId="33"/>
+    <tableColumn id="155" xr3:uid="{0D428223-9C3F-4A3F-ABC9-B6497EC9F4C7}" name="Characteristics [watering exposure]" dataDxfId="32"/>
+    <tableColumn id="156" xr3:uid="{0A90F49E-9F46-4E82-B592-5446DD648569}" name="Term Source REF (PECO:0007383)" dataDxfId="31"/>
+    <tableColumn id="157" xr3:uid="{6216E053-90BE-49F8-9C0C-7A6470F6D3DE}" name="Term Accession Number (PECO:0007383)" dataDxfId="30"/>
+    <tableColumn id="158" xr3:uid="{1ACB13C6-536F-41C7-91F2-B62AEB2DA8A4}" name="Characteristics [plant nutrient exposure]" dataDxfId="29"/>
+    <tableColumn id="159" xr3:uid="{97FEA8C0-4955-47E8-8E42-EFE66F8E2530}" name="Term Source REF (PECO:0007241)" dataDxfId="28"/>
+    <tableColumn id="160" xr3:uid="{159271F8-4343-4546-81D3-E7AE0438BF91}" name="Term Accession Number (PECO:0007241)" dataDxfId="27"/>
+    <tableColumn id="161" xr3:uid="{AC98601D-DB44-45A0-9639-848DD3D97821}" name="Characteristics [abiotic plant exposure]" dataDxfId="26"/>
+    <tableColumn id="162" xr3:uid="{1EF71984-AE79-45A3-B85C-3D63B9A45000}" name="Term Source REF (PECO:0007191)" dataDxfId="25"/>
+    <tableColumn id="163" xr3:uid="{58575740-B787-4889-B047-BE8097574A83}" name="Term Accession Number (PECO:0007191)" dataDxfId="24"/>
+    <tableColumn id="99" xr3:uid="{0AD23E00-4026-4DE6-9B26-1D80067F6D23}" name="Characteristics [biotic plant exposure]" dataDxfId="23"/>
+    <tableColumn id="100" xr3:uid="{A73EA20C-30F6-4F5A-BE9C-1F95EDAD2075}" name="Term Source REF (PECO:0007357)" dataDxfId="22"/>
+    <tableColumn id="101" xr3:uid="{7BC176DE-D288-440D-AE07-B17C6C087D41}" name="Term Accession Number (PECO:0007357)" dataDxfId="21"/>
+    <tableColumn id="102" xr3:uid="{E4B7F22F-69B7-45D9-A3CD-B8F269AFECB1}" name="Characteristics [Geogaphic Area]" dataDxfId="20"/>
+    <tableColumn id="103" xr3:uid="{571169D2-47B6-40AA-8E2B-8629455DE18E}" name="Term Source REF (NFDI4PSO:0000074)" dataDxfId="19"/>
+    <tableColumn id="104" xr3:uid="{B601805D-FC55-4818-BE56-E15EAC614D1A}" name="Term Accession Number (NFDI4PSO:0000074)" dataDxfId="18"/>
+    <tableColumn id="105" xr3:uid="{820EF1CB-22B2-4D90-A62E-60758945BF10}" name="Characteristics [Sample Collection Date]" dataDxfId="17"/>
+    <tableColumn id="106" xr3:uid="{20297405-2B24-48CF-B8F1-5C8FD0C57F7C}" name="Term Source REF (NFDI4PSO:0000075)" dataDxfId="16"/>
+    <tableColumn id="107" xr3:uid="{3D2321BF-EE54-4E22-8362-620DB8FCDC80}" name="Term Accession Number (NFDI4PSO:0000075)" dataDxfId="15"/>
+    <tableColumn id="108" xr3:uid="{7C136999-9BAF-43E5-855D-D97F492175D8}" name="Characteristics [Sample Collected By]" dataDxfId="14"/>
+    <tableColumn id="109" xr3:uid="{CDD0FBA0-5918-486C-BB4F-FBA37D34F559}" name="Term Source REF (NFDI4PSO:0000076)" dataDxfId="13"/>
+    <tableColumn id="110" xr3:uid="{9EEEA931-289F-4558-A4CD-BAA5A89EDBCB}" name="Term Accession Number (NFDI4PSO:0000076)" dataDxfId="12"/>
+    <tableColumn id="111" xr3:uid="{D539A2BF-683E-4EB0-A3FA-26F36AB2D491}" name="Characteristics [Time point]" dataDxfId="11"/>
+    <tableColumn id="112" xr3:uid="{67D48280-3922-4AE2-A629-EAEB3D5641B8}" name="Term Source REF (NFDI4PSO:0000034)" dataDxfId="10"/>
+    <tableColumn id="113" xr3:uid="{615E7959-5992-4D06-8A7B-DD39B89C4EEC}" name="Term Accession Number (NFDI4PSO:0000034)" dataDxfId="9"/>
+    <tableColumn id="114" xr3:uid="{4D9D42EB-53DB-46E9-AC66-722486F5B239}" name="Parameter [Sample Collection Method]" dataDxfId="8"/>
+    <tableColumn id="115" xr3:uid="{13DC542E-9758-4841-8D94-D7C3116C0568}" name="Term Source REF (NFDI4PSO:0000009)" dataDxfId="7"/>
+    <tableColumn id="116" xr3:uid="{36345937-CA63-443C-9D9D-BD0EAAAF7812}" name="Term Accession Number (NFDI4PSO:0000009)" dataDxfId="6"/>
+    <tableColumn id="117" xr3:uid="{05864A64-95DE-44E0-8966-107156CE7021}" name="Parameter [Metabolism quenching method]" dataDxfId="5"/>
+    <tableColumn id="118" xr3:uid="{3D7DB003-4188-49D2-94CA-D993FAD9E4F0}" name="Term Source REF (NFDI4PSO:0000010)" dataDxfId="4"/>
+    <tableColumn id="119" xr3:uid="{786911B1-BB7C-4948-A507-1360E791FD32}" name="Term Accession Number (NFDI4PSO:0000010)" dataDxfId="3"/>
+    <tableColumn id="120" xr3:uid="{9ACB2720-1CAC-4E92-BC80-C750A5BB4732}" name="Parameter [Sample storage]" dataDxfId="2"/>
+    <tableColumn id="121" xr3:uid="{F17CF920-3ACC-4E28-BDDF-4EAB2A03C00F}" name="Term Source REF (NFDI4PSO:0000011)" dataDxfId="1"/>
+    <tableColumn id="122" xr3:uid="{89F0B1DF-DB89-45C5-91DE-1DD5DA8F371D}" name="Term Accession Number (NFDI4PSO:0000011)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{8929A4D6-2D94-4C25-8C8A-5E4C6021B93A}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1033,9 +1329,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2021-11-03T15:43:02.72" personId="{BFA4ADC4-8771-41AF-BD0E-9E56E7CC4977}" id="{A6730C41-F5DE-4F01-A3FC-095AF4373E4D}">
+    <text>The unique identifier of this template. It will be auto generated.</text>
+  </threadedComment>
+  <threadedComment ref="A1" dT="2021-11-03T15:43:02.72" personId="{BFA4ADC4-8771-41AF-BD0E-9E56E7CC4977}" id="{870147F0-D856-45E5-BAAA-42E6AA783338}" parentId="{A6730C41-F5DE-4F01-A3FC-095AF4373E4D}">
+    <text>id=f12e98ee-a4e7-4ada-ba56-1e13cce1a44b</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="610" row="1">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1595,4 +1902,326 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C806736B-09AD-44FE-B8F6-60FEE51F74DE}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<customXml>
+  <SwateTable Table="annotationTableUnluckyVampirebat89">
+    <TableValidation DateTime="2021-11-03 16:47" SwateVersion="0.5.1" TableName="annotationTableUnluckyVampirebat89" Userlist="">
+      <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="1" ColumnHeader="Characteristics [Sample type]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="4" ColumnHeader="Characteristics [Biological replicate]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="7" ColumnHeader="Characteristics [Organism]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="10" ColumnHeader="Characteristics [Isolate]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="13" ColumnHeader="Characteristics [Cultivar]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="16" ColumnHeader="Characteristics [Ecotype]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="19" ColumnHeader="Characteristics [Genotype]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="22" ColumnHeader="Characteristics [population]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="25" ColumnHeader="Characteristics [Organism part]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="28" ColumnHeader="Characteristics [Cell line]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="31" ColumnHeader="Characteristics [Cell type]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="34" ColumnHeader="Characteristics [Plant age]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="37" ColumnHeader="Characteristics [Developmental Stage]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="40" ColumnHeader="Characteristics [Plant disease]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="43" ColumnHeader="Characteristics [Plant disease stage]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="46" ColumnHeader="Characteristics [Phenotype]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="49" ColumnHeader="Characteristics [whole plant size]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="52" ColumnHeader="Characteristics [study type]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="55" ColumnHeader="Characteristics [plant growth medium exposure]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="58" ColumnHeader="Characteristics [growth plot design]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="61" ColumnHeader="Characteristics [Growth day length]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="64" ColumnHeader="Characteristics [light intensity exposure]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="68" ColumnHeader="Characteristics [Humidity Day]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="72" ColumnHeader="Characteristics [Humidity Night]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="76" ColumnHeader="Characteristics [Temperature Day]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="80" ColumnHeader="Characteristics [Temperature Night]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="84" ColumnHeader="Characteristics [watering exposure]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="87" ColumnHeader="Characteristics [plant nutrient exposure]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="90" ColumnHeader="Characteristics [abiotic plant exposure]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="93" ColumnHeader="Characteristics [biotic plant exposure]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="96" ColumnHeader="Characteristics [Geogaphic Area]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="99" ColumnHeader="Characteristics [Sample Collection Date]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="102" ColumnHeader="Characteristics [Sample Collected By]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="105" ColumnHeader="Characteristics [Time point]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="108" ColumnHeader="Parameter [Sample Collection Method]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="111" ColumnHeader="Parameter [Metabolism quenching method]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="114" ColumnHeader="Parameter [Sample storage]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="117" ColumnHeader="Sample Name" Importance="None" Unit="None" ValidationFormat="None"/>
+    </TableValidation>
+  </SwateTable>
+</customXml>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6958E146-EC71-4441-974C-EF34F37AE1B4}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update templates's ontology terms
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants/1SPL01_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\1SPL01_plants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F86A42-0FB6-4318-8EB1-2691FBA95640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DAC0D6-0303-46B7-B9E1-BAD4CB496697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D1671A6-E5E6-4E90-817E-C23847CD9BD1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2D1671A6-E5E6-4E90-817E-C23847CD9BD1}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="390">
   <si>
     <t>Source Name</t>
   </si>
@@ -1120,36 +1120,18 @@
     <t>Mutant</t>
   </si>
   <si>
-    <t>Leaf</t>
-  </si>
-  <si>
-    <t>Root</t>
-  </si>
-  <si>
-    <t>Flower</t>
-  </si>
-  <si>
     <t xml:space="preserve">Days after germination / sowing </t>
   </si>
   <si>
-    <t>Field</t>
-  </si>
-  <si>
     <t>Climate chamber</t>
   </si>
   <si>
     <t>Green house</t>
   </si>
   <si>
-    <t>Soil</t>
-  </si>
-  <si>
     <t>Hydroponic</t>
   </si>
   <si>
-    <t>Agar</t>
-  </si>
-  <si>
     <t>Completely Randomized Design</t>
   </si>
   <si>
@@ -1159,12 +1141,6 @@
     <t>Split Plot Design</t>
   </si>
   <si>
-    <t>12/12</t>
-  </si>
-  <si>
-    <t>10/14</t>
-  </si>
-  <si>
     <t xml:space="preserve">Short day </t>
   </si>
   <si>
@@ -1183,7 +1159,85 @@
     <t>-80 °C</t>
   </si>
   <si>
-    <t>1.1.8</t>
+    <t>ENVO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ENVO_02000008</t>
+  </si>
+  <si>
+    <t>NCBITaxon</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCBITaxon_1306155</t>
+  </si>
+  <si>
+    <t>user-specific</t>
+  </si>
+  <si>
+    <t>leaf</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PO_0025034</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCBITaxon_1</t>
+  </si>
+  <si>
+    <t>flower</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PO_0009046</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ENVO_01000352</t>
+  </si>
+  <si>
+    <t>soil</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ENVO_00001998</t>
+  </si>
+  <si>
+    <t>agar</t>
+  </si>
+  <si>
+    <t>CHEBI</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_2509</t>
+  </si>
+  <si>
+    <t>microeinstein per square meter per second</t>
+  </si>
+  <si>
+    <t>UO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000160</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000187</t>
+  </si>
+  <si>
+    <t>degree Celsius</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000027</t>
+  </si>
+  <si>
+    <t>1.1.9</t>
   </si>
 </sst>
 </file>
@@ -1349,7 +1403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1390,6 +1444,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal 3" xfId="1" xr:uid="{D09CA6D9-E6C7-4433-8F48-8CA6F5BF0770}"/>
@@ -2014,7 +2069,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="629" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="662" row="2">
@@ -2047,7 +2102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8916BF-D1BA-4E62-B448-EB2F6971FAFB}">
   <dimension ref="A1:DN7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2071,11 +2126,11 @@
     <col min="18" max="18" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.85546875" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="28" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="37.85546875" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="43.7109375" hidden="1" customWidth="1"/>
@@ -2085,7 +2140,7 @@
     <col min="32" max="32" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="34" max="34" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="30" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="37.5703125" bestFit="1" customWidth="1"/>
@@ -2098,11 +2153,11 @@
     <col min="45" max="45" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="46" max="46" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="47" max="47" width="28" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="30.140625" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="37.140625" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="49" max="49" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="50" max="50" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="51" max="51" width="30.140625" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="37.140625" hidden="1" customWidth="1"/>
     <col min="53" max="53" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="32.42578125" hidden="1" customWidth="1"/>
     <col min="55" max="55" width="39.5703125" hidden="1" customWidth="1"/>
@@ -2113,7 +2168,8 @@
     <col min="60" max="60" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="61" max="61" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="62" max="62" width="35" bestFit="1" customWidth="1"/>
-    <col min="63" max="64" width="0" hidden="1" customWidth="1"/>
+    <col min="63" max="63" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="64" max="64" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="65" max="65" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="7.140625" hidden="1" customWidth="1"/>
     <col min="67" max="67" width="32.42578125" hidden="1" customWidth="1"/>
@@ -2144,26 +2200,26 @@
     <col min="92" max="92" width="32.42578125" hidden="1" customWidth="1"/>
     <col min="93" max="93" width="39.5703125" hidden="1" customWidth="1"/>
     <col min="94" max="94" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="43" hidden="1" customWidth="1"/>
-    <col min="96" max="96" width="38.5703125" hidden="1" customWidth="1"/>
+    <col min="95" max="95" width="32.42578125" hidden="1" customWidth="1"/>
+    <col min="96" max="96" width="39.5703125" hidden="1" customWidth="1"/>
     <col min="97" max="97" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="28.28515625" hidden="1" customWidth="1"/>
-    <col min="99" max="99" width="43" hidden="1" customWidth="1"/>
+    <col min="98" max="98" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="99" max="99" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="100" max="100" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="15.5703125" hidden="1" customWidth="1"/>
-    <col min="102" max="102" width="28.28515625" hidden="1" customWidth="1"/>
+    <col min="101" max="101" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="102" max="102" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="103" max="103" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="43" hidden="1" customWidth="1"/>
-    <col min="105" max="105" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="104" max="104" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="105" max="105" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="106" max="106" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="28.28515625" hidden="1" customWidth="1"/>
-    <col min="108" max="108" width="43" hidden="1" customWidth="1"/>
+    <col min="107" max="107" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="108" max="108" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="109" max="109" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="15.5703125" hidden="1" customWidth="1"/>
-    <col min="111" max="111" width="28.28515625" hidden="1" customWidth="1"/>
+    <col min="110" max="110" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="111" max="111" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="112" max="112" width="43" bestFit="1" customWidth="1"/>
     <col min="113" max="113" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="114" max="114" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="114" max="114" width="43.7109375" hidden="1" customWidth="1"/>
     <col min="115" max="115" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="116" max="116" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="117" max="117" width="43.7109375" hidden="1" customWidth="1"/>
@@ -2530,50 +2586,134 @@
       <c r="B2" t="s">
         <v>340</v>
       </c>
+      <c r="C2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D2" t="s">
+        <v>364</v>
+      </c>
       <c r="H2" t="s">
         <v>346</v>
       </c>
+      <c r="I2" t="s">
+        <v>367</v>
+      </c>
+      <c r="J2" t="s">
+        <v>367</v>
+      </c>
       <c r="T2" t="s">
         <v>348</v>
       </c>
+      <c r="U2" t="s">
+        <v>367</v>
+      </c>
+      <c r="V2" t="s">
+        <v>367</v>
+      </c>
       <c r="Z2" t="s">
+        <v>368</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>369</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>370</v>
+      </c>
+      <c r="AI2" t="s">
         <v>350</v>
       </c>
-      <c r="AI2" t="s">
-        <v>353</v>
+      <c r="AJ2" t="s">
+        <v>367</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>367</v>
       </c>
       <c r="BA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>363</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>376</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>377</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>363</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>378</v>
+      </c>
+      <c r="BG2" t="s">
         <v>354</v>
       </c>
-      <c r="BD2" t="s">
-        <v>357</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>360</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>363</v>
+      <c r="BH2" t="s">
+        <v>367</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>367</v>
+      </c>
+      <c r="BJ2" s="16">
+        <v>44542</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>367</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>367</v>
       </c>
       <c r="BM2" s="1"/>
-      <c r="BN2" s="1"/>
-      <c r="BO2" s="1"/>
-      <c r="BP2" s="1"/>
+      <c r="BN2" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="BO2" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="BP2" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="BQ2" s="2"/>
-      <c r="BR2" s="2"/>
-      <c r="BS2" s="2"/>
-      <c r="BT2" s="2"/>
+      <c r="BR2" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="BS2" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="BU2" s="2"/>
-      <c r="BV2" s="2"/>
-      <c r="BW2" s="2"/>
-      <c r="BX2" s="2"/>
+      <c r="BV2" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="BW2" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BX2" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="BY2" s="3"/>
-      <c r="BZ2" s="3"/>
-      <c r="CA2" s="3"/>
-      <c r="CB2" s="3"/>
+      <c r="BZ2" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="CA2" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="CB2" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="CC2" s="3"/>
-      <c r="CD2" s="3"/>
-      <c r="CE2" s="3"/>
-      <c r="CF2" s="3"/>
+      <c r="CD2" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="CE2" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="CF2" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="CG2" s="3"/>
       <c r="CH2" s="3"/>
       <c r="CI2" s="3"/>
@@ -2599,66 +2739,156 @@
       <c r="DC2" s="3"/>
       <c r="DD2" s="3"/>
       <c r="DE2" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="DF2" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="DF2" s="3"/>
-      <c r="DG2" s="3"/>
+      <c r="DG2" s="3" t="s">
+        <v>367</v>
+      </c>
       <c r="DH2" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="DI2" s="3"/>
-      <c r="DJ2" s="3"/>
+        <v>361</v>
+      </c>
+      <c r="DI2" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="DJ2" s="3" t="s">
+        <v>367</v>
+      </c>
       <c r="DK2" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="DL2" s="3"/>
-      <c r="DM2" s="3"/>
+        <v>362</v>
+      </c>
+      <c r="DL2" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="DM2" s="3" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="3" spans="1:118" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>341</v>
       </c>
+      <c r="C3" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3" t="s">
+        <v>366</v>
+      </c>
       <c r="H3" t="s">
         <v>347</v>
       </c>
+      <c r="I3" t="s">
+        <v>367</v>
+      </c>
+      <c r="J3" t="s">
+        <v>367</v>
+      </c>
       <c r="T3" t="s">
         <v>349</v>
       </c>
+      <c r="U3" t="s">
+        <v>367</v>
+      </c>
+      <c r="V3" t="s">
+        <v>367</v>
+      </c>
       <c r="Z3" t="s">
+        <v>371</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>365</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>372</v>
+      </c>
+      <c r="BA3" t="s">
         <v>351</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BB3" t="s">
+        <v>367</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>367</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>367</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>367</v>
+      </c>
+      <c r="BG3" t="s">
         <v>355</v>
       </c>
-      <c r="BD3" t="s">
-        <v>358</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>361</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>364</v>
+      <c r="BH3" t="s">
+        <v>367</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>367</v>
+      </c>
+      <c r="BJ3" s="16">
+        <v>44483</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>367</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>367</v>
       </c>
       <c r="BM3" s="1"/>
-      <c r="BN3" s="1"/>
-      <c r="BO3" s="1"/>
-      <c r="BP3" s="1"/>
+      <c r="BN3" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="BO3" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="BP3" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="BQ3" s="2"/>
-      <c r="BR3" s="2"/>
-      <c r="BS3" s="2"/>
-      <c r="BT3" s="2"/>
+      <c r="BR3" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="BS3" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BT3" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="BU3" s="2"/>
-      <c r="BV3" s="2"/>
-      <c r="BW3" s="2"/>
-      <c r="BX3" s="2"/>
+      <c r="BV3" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="BW3" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BX3" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="BY3" s="3"/>
-      <c r="BZ3" s="3"/>
-      <c r="CA3" s="3"/>
-      <c r="CB3" s="3"/>
+      <c r="BZ3" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="CA3" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="CB3" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="CC3" s="3"/>
-      <c r="CD3" s="3"/>
-      <c r="CE3" s="3"/>
-      <c r="CF3" s="3"/>
+      <c r="CD3" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="CE3" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="CF3" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="CG3" s="3"/>
       <c r="CH3" s="3"/>
       <c r="CI3" s="3"/>
@@ -2684,10 +2914,14 @@
       <c r="DC3" s="3"/>
       <c r="DD3" s="3"/>
       <c r="DE3" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="DF3" s="3"/>
-      <c r="DG3" s="3"/>
+        <v>360</v>
+      </c>
+      <c r="DF3" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="DG3" s="3" t="s">
+        <v>367</v>
+      </c>
       <c r="DH3" s="3"/>
       <c r="DI3" s="3"/>
       <c r="DJ3" s="3"/>
@@ -2699,41 +2933,107 @@
       <c r="B4" t="s">
         <v>342</v>
       </c>
+      <c r="C4" t="s">
+        <v>367</v>
+      </c>
+      <c r="D4" t="s">
+        <v>367</v>
+      </c>
       <c r="Z4" t="s">
+        <v>373</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>369</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>374</v>
+      </c>
+      <c r="BA4" t="s">
         <v>352</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BB4" t="s">
+        <v>367</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>367</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>379</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>380</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>381</v>
+      </c>
+      <c r="BG4" t="s">
         <v>356</v>
       </c>
-      <c r="BD4" t="s">
-        <v>359</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>362</v>
+      <c r="BH4" t="s">
+        <v>367</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>367</v>
       </c>
       <c r="BJ4" t="s">
-        <v>365</v>
+        <v>357</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>367</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>367</v>
       </c>
       <c r="BM4" s="1"/>
-      <c r="BN4" s="1"/>
-      <c r="BO4" s="1"/>
-      <c r="BP4" s="1"/>
+      <c r="BN4" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="BO4" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="BP4" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="BQ4" s="2"/>
-      <c r="BR4" s="2"/>
-      <c r="BS4" s="2"/>
-      <c r="BT4" s="2"/>
+      <c r="BR4" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="BS4" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BT4" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="BU4" s="2"/>
-      <c r="BV4" s="2"/>
-      <c r="BW4" s="2"/>
-      <c r="BX4" s="2"/>
+      <c r="BV4" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="BW4" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BX4" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="BY4" s="3"/>
-      <c r="BZ4" s="3"/>
-      <c r="CA4" s="3"/>
-      <c r="CB4" s="3"/>
+      <c r="BZ4" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="CA4" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="CB4" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="CC4" s="3"/>
-      <c r="CD4" s="3"/>
-      <c r="CE4" s="3"/>
-      <c r="CF4" s="3"/>
+      <c r="CD4" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="CE4" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="CF4" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="CG4" s="3"/>
       <c r="CH4" s="3"/>
       <c r="CI4" s="3"/>
@@ -2772,29 +3072,71 @@
       <c r="B5" t="s">
         <v>343</v>
       </c>
+      <c r="C5" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5" t="s">
+        <v>367</v>
+      </c>
       <c r="BJ5" t="s">
-        <v>366</v>
+        <v>358</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>367</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>367</v>
       </c>
       <c r="BM5" s="1"/>
-      <c r="BN5" s="1"/>
-      <c r="BO5" s="1"/>
-      <c r="BP5" s="1"/>
+      <c r="BN5" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="BO5" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="BP5" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="BQ5" s="2"/>
-      <c r="BR5" s="2"/>
-      <c r="BS5" s="2"/>
-      <c r="BT5" s="2"/>
+      <c r="BR5" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="BS5" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BT5" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="BU5" s="2"/>
-      <c r="BV5" s="2"/>
-      <c r="BW5" s="2"/>
-      <c r="BX5" s="2"/>
+      <c r="BV5" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="BW5" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BX5" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="BY5" s="3"/>
-      <c r="BZ5" s="3"/>
-      <c r="CA5" s="3"/>
-      <c r="CB5" s="3"/>
+      <c r="BZ5" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="CA5" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="CB5" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="CC5" s="3"/>
-      <c r="CD5" s="3"/>
-      <c r="CE5" s="3"/>
-      <c r="CF5" s="3"/>
+      <c r="CD5" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="CE5" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="CF5" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="CG5" s="3"/>
       <c r="CH5" s="3"/>
       <c r="CI5" s="3"/>
@@ -2833,26 +3175,62 @@
       <c r="B6" t="s">
         <v>344</v>
       </c>
+      <c r="C6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D6" t="s">
+        <v>367</v>
+      </c>
       <c r="BM6" s="1"/>
-      <c r="BN6" s="1"/>
-      <c r="BO6" s="1"/>
-      <c r="BP6" s="1"/>
+      <c r="BN6" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="BO6" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="BP6" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="BQ6" s="2"/>
-      <c r="BR6" s="2"/>
-      <c r="BS6" s="2"/>
-      <c r="BT6" s="2"/>
+      <c r="BR6" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="BS6" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BT6" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="BU6" s="2"/>
-      <c r="BV6" s="2"/>
-      <c r="BW6" s="2"/>
-      <c r="BX6" s="2"/>
+      <c r="BV6" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="BW6" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BX6" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="BY6" s="3"/>
-      <c r="BZ6" s="3"/>
-      <c r="CA6" s="3"/>
-      <c r="CB6" s="3"/>
+      <c r="BZ6" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="CA6" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="CB6" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="CC6" s="3"/>
-      <c r="CD6" s="3"/>
-      <c r="CE6" s="3"/>
-      <c r="CF6" s="3"/>
+      <c r="CD6" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="CE6" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="CF6" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="CG6" s="3"/>
       <c r="CH6" s="3"/>
       <c r="CI6" s="3"/>
@@ -2891,26 +3269,62 @@
       <c r="B7" t="s">
         <v>345</v>
       </c>
+      <c r="C7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D7" t="s">
+        <v>367</v>
+      </c>
       <c r="BM7" s="1"/>
-      <c r="BN7" s="1"/>
-      <c r="BO7" s="1"/>
-      <c r="BP7" s="1"/>
+      <c r="BN7" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="BO7" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="BP7" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="BQ7" s="2"/>
-      <c r="BR7" s="2"/>
-      <c r="BS7" s="2"/>
-      <c r="BT7" s="2"/>
+      <c r="BR7" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="BS7" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BT7" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="BU7" s="2"/>
-      <c r="BV7" s="2"/>
-      <c r="BW7" s="2"/>
-      <c r="BX7" s="2"/>
+      <c r="BV7" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="BW7" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="BX7" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="BY7" s="3"/>
-      <c r="BZ7" s="3"/>
-      <c r="CA7" s="3"/>
-      <c r="CB7" s="3"/>
+      <c r="BZ7" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="CA7" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="CB7" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="CC7" s="3"/>
-      <c r="CD7" s="3"/>
-      <c r="CE7" s="3"/>
-      <c r="CF7" s="3"/>
+      <c r="CD7" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="CE7" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="CF7" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="CG7" s="3"/>
       <c r="CH7" s="3"/>
       <c r="CI7" s="3"/>
@@ -2957,7 +3371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C806736B-09AD-44FE-B8F6-60FEE51F74DE}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2989,7 +3403,7 @@
         <v>120</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>371</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>